<commit_message>
se actualizo el formulario y ahora tiene el campo de sanidad tambien piede el registro sanitario y enfermedades
</commit_message>
<xml_diff>
--- a/registros_vacas.xlsx
+++ b/registros_vacas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Downloads\Veterinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C052C0E6-AD51-46D8-BB10-CD564A7FE283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFBBA52-FF70-4CAF-B15C-F52FD8A58760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Fecha y Hora</t>
   </si>
@@ -56,6 +56,54 @@
   </si>
   <si>
     <t>Numero de parto</t>
+  </si>
+  <si>
+    <t>Vacunas</t>
+  </si>
+  <si>
+    <t>Enfermedades</t>
+  </si>
+  <si>
+    <t>2025-11-10 10:39:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro </t>
+  </si>
+  <si>
+    <t>A101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lola </t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAA0JCgsKCA0LCgsODg0PEyAVExISEyccHhcgLikxMC4pLSwzOko+MzZGNywtQFdBRkxOUlNSMj5aYVpQYEpRUk//2wBDAQ4ODhMREyYVFSZPNS01T09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT09PT0//wAARCAIwAaQDASIAAhEBAxEB/8QAGwAAAgMBAQEAAAAAAAAAAAAAAgMAAQQFBgf/xABDEAACAgEDAgUBBQUFBgYCAwABAgARAwQSITFBBRMiUWFxBhQygZEjQlKx0RU0cqHBM1NikuHwFiRUc4LxNUNEY6L/xAAYAQEBAQEBAAAAAAAAAAAAAAABAAIDBP/EACgRAQEAAgICAgMBAAICAwAAAAABAhEhMQMSQVETImFxBDIUoeHw8f/aAAwDAQACEQMRAD8ANMmXqxJxjoI98+5fSgBHtOg+JSuxVFdoCYTha3xgqe9TyTyS/Dr61iTLkIrKPT7DvI2Xabxr+U6GTTq1EICD7Sn0uMBaABM1PJiLjWQZvMH7YFR7CTFmRclX6fcxuowqnBBErycWxQBfuZ2xyxc7KU7jcduQkE8Tp+HeGZtZg3qwFe8vwvwgat97DbiU8n3+J6rFiTEgTGoVR2E62z4YkrzJ0udsowFDYNVU7ug0GPSJZpsnc+30mySZa0kkkkkkqXKkkkkkkkkkkkkkkkkkkkkklxWq/uub/A38o2K1f90zf+238oztXpWjN6PAf/61/lM3jhrwrN+X8xD0Gq07aPCFzISEAILAEGvaI8ey4/7KyDetsQFAPXmbxn7z/WLf0eTbpPTfZjHt0L5D++/8p5hjPZ+D4/K8LwDuV3H8+Z6f+RdYacfDP2ZvtHnOLQDGqn9qaJ9gOZu8PxeToMGPuEF/Wczx0+drNFpR+81n9a/rO2OBPNlxhI7Y852pKlypzbSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSePxkl4epzFk8u+Jm+848WLcWEynxPTqbZ7PsOZ4cfHbzp3uUbMOXJpj7ofeVnyNlO6/0nOy+MBxS4zXzMx8SzVS7QJ3x8OV50xc47OV2ybUI6Td4ZoMuqfkViB9R/pPKjX57vf/AJTZpfHfENKCMOegeoKgzvj4bHO5voeHDjwYxjxLSiMnhsX2r8RX8Xkv9Ur+U1YvtdqB/tNNib/CSJv8eTPvHr5J5rF9rsR/2ulYf4WB/nNWP7UeHsBuGZT3BS4emX0faO3JOWn2g8MYf3gj6oYf9ueGV/e1/Q/0l65fS9p9ujKmAeN+GH/+Wn6H+kNPFfD8h9Orxfm1Q9b9L2n22SQceXHlF4siuPdTcOBVJLkklSS5JJUkuSSSK1X90zf4G/lGxWq/uub/AAN/KM7V6Y/D/DdImkxMcKuzKGJYX1EzeN6DTJoWzY8So6kfhFXzOppP7ng/9tf5TJ48a8KyfJH85vHK+/bncZ69PIBTkyqi9WNCer0+g8R0+mXFi1yjaOFOMED4uef8Hxed4rgWuA24/lzPazt587LI5+LHe6834emozfaAnWNvyYQb9h7V+s9JON4EDl1Os1TdXeh/P+k7M5eW7ydPFP12kqXKnJ0SSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSfIC5b8TE/WVcES50kZtEDLEEQhOkZogIYg9pYmoyMQgYAhAzcZpgMsGAJYMYB3L3QLl3Nxmj3H3lhjF3LuaDRjzPjbdjdlPupqdjRfaPWYCFzEZ0H8XDfrOADLDQywxy7imVnT6BoPFtLrqXG+3J/A3X/rN8+aJkKkEGiOhnofCftC2IDFrSzp2fqR9feeXyeCznF3x8vxXqpIGLLjzYxkxOHRuhBhzzuqSSSSSReo/u+X/Af5RkXqf7tl/wAB/lKKg0Dh9DgYdDjH8ph+0bBfCyO7OBNPhOJsXhuFXIPp3D6Hmcv7VZaTBiB6ksf5TphN+RjK/oz/AGXxb9bkyn9xK/Mmeh12XydFmyfwoSJx/spXlajjncP0m3x7IV8NKDrlYIP+/wApryft5NM4cePa/AcXleF4yerksZ0YvBjGLBjxj9xQIycsru2umM1JElS5UCkkkkkkkkuSBlfy8Zar9h7wMWox5CFBpz+7HRI06LqjnBIJFEdvrEXezpUuVApJJJJJJJJJJJJJJJJJJJJJJKZlRSzGgJJcnQWYkarEehmfPrHvYgAB7yZuckPx+YwJbKOT0HaSVhwOuMfteTyaEk1tmSvkghQRCE3DViFKEsTcAhLlCEJqMrEIQRDE0FiXKlzUC5JUuajK5JJIhcu4Mk0Bgw1eoq5dxDreG+LZtC/7NvSfxIehnrvD/E9Pr1/Zttyd0PX/AKz54DG48rIwKsQR0IM4+TxTLn5dMfJcX0uSeT8N+0WbGQmq/ap/F+8P6z1OHKmbEuTEwZGFgiePLC49vRjlMuhxep/u2X/Af5RkXqP7vl/wH+UyaHRf3LB/7a/ynl/tPl3+JhP4EA/Xmeo0f9ywf+2v8p4bxLO+bX5smSgxc2B2rid/DN57cvLf1kev8CxDF4Tg4ouNx/MxXihGXxPQab/jLkfA/wCzNfhf/wCM01f7pf5TnaVm1P2lzu4oadNi/wDf6zE/7WtX/rI7ckkk5tpJJJJJJJJJJJAdHb8OUr+QMxapNcgXydX+JgOUEdC3ToQB/tGuuAKnMfReJhDs8QYk8ngTn6XB4g+py7tRmV/3ju5MfX+j2/j00k8vqMuqw6hVbWanaT/EZqzfdmwhhqdScwHBJa5aXtv4d0kAEk0BICGFqQR7icrBpcWHR+brXztfXc7H/KZNH4tgxap1XzDhPAJX/SGvpe329DJBxumRA6MCp6EROTW6XEQHzoLNdYNNEkDHmxZU348iMvuDYh2PeSSSQEHoZJJIGXCmZdrj84ckk5eo0GZF/YNvHseDMJyZvMCZEIK9iJ6KDkxpkFOob6x253x/Tlt4ky0qJQA6SR2TwrG7lhkZQe1XJLhn1zfMgyf7sQg+P/dCLEIVOmmtjD4/90IW/H/uhAAEsCakGxh0/wB2IW5P4BFgCGBNSDYgU/g/zl2n8H+cGpYE0Ni9P8MIKD+6ZQFfWXye8tnSxjU9v85DjA7GQCXuYd47q1AUvsZPT8w/M/iAMIDE/cqZrbPqVxJxGtgYC19Q+Ik8TUu2bLF0PeSh7ypJpkQA94QC/wAcXJJNKLjvnMonW8L8QGgyWuoR8Z/EhPX/AKzg3Jczlj7TVMuun0PF4x4fkUEarGCezGiIrxDxPSjQ5fK1OIuykKA1nmeDDES9595x/BN9un5a9Xg8eOPRLiCYzkRdoYvxx3qeczAtkLFwxJsm5muS51xwmPTnllb272l8c1mn0iYMYxEIKDNyamz7N6gtrNU2oyLvygNZNWbnlbhoGJ9IMzl4pZdGZ3cfSw6now/WWCD0M+cAZh0DSw+ZefWJx/B/XT8v8fRpJ85+85h/+x/+Yyfes3+9f/mMvwX7X5v4+jST5wdXn/32T/nMr77qR01GUf8AzMf/AB79r838fSJzvEdobGN7H1Di54f79qx01OYf/MwTrdV/6jIfq0p4L9i+Xb2mLVOupKhyy/8AG/SB4pqm0eDzcG1mbsHPM8YdbqibOdyfrJ9/1VV5zEfNR/CPyV1m8Y1OTMjvgX0nuSZtzeLYMwDNj2N3ABM82ddqT1yf/wCRINbqB0cf8omvxRTyZT5erzeP4ctIRkXHVMAvWc7JrNL5pOLeo+k4x8Q1HdkP/wABJ9/z3+5/ySnjkFy329Bh8bGHGUR2o+6xf9o6ZiTkZ2vr6Zw/v+b+HH/yy/7Ry/7vF/yzP4p9GZ2Opk1Gja9ruAT02yvvWmu/Oy3VXzOb/aL98WI/kf6yDxEjrgxH8jH0Hs6a63T4zePNmUjgEXxDxeKY8SFfOz9bHJ4M5B14Jv7vj/zlHXIRR0qfrC4bamdjrL4oFYsup1AJNmmPM1j7RbQaz5CT7r/0nnPveLvpx/zS21WnPTTkf/KVwg9q9A32ky2Suc/QoI7F9qKrzCrcfwkTy3n4D/8Aqb9ZBm018rkA+Jm+OL2v29kv2q0lepGv4knkRk0NcnN+kkPxw+9cgZDCDRCmGDFo4MYQYxAMMGIODQg8SDCBmoDtxPWMTmZwY7EeI1Ts0QhzKHMJeDMugwnEorGqQRLKzMya9WcrAPE0lbinSdMcnPLEKZGQ8GNKrnFrw/t7zPUtWKmxN6+Yxv4qjwaPWSNyAOu8de8TNS7Ys0lyXJJNBdyXKlSS7l3BkghXDRS/TpAxqXao13AG1eghaZBqyY1utze5lDUOOhibkkjxqcgPWGNUx7kTLJDUO2v7wf3gp+oglceQ+khT7TOD2Mq4dHsTqyNREHmPw5bGxqJ7EwMjsrEMoB+kvYepTWOsEmaGrKlL1mZlK9YzLYs0lyiYNyohe6VulGVAi3SboEqSHuk3QJVwRm6VugXKuBHuk3xdyrkjN8m6LkhtD3SboEqCHukgSS2iVWWFliWOs5bd/VAIQEoQhHY0sCGBBEIRlGhiHjNRcsGjNdjppUxgMSpsRgma3DAahjIe8BeYWwmZaEG5g5JVESE8TUFJMqWZU7Rwo0aoORdpsdDIIdgijLelrZMuoRWpJrbOg1LqXJDZ0qpYW4QS+kIcQtMicKvEWRcI8mWFmdtaBJGFYJWamTPqGSSVHYSSSSBTpNGN1ygJk6joYiVRviZrUOOMBvQaIhY0GVijCmiydy7v3h1kTMVaz2mLsnHw433itRp8eIgczp6PWDL6S3PzMOuN5jXMxMst8q4z4J02nx58oTkXO0vgmlGLcdx4uc3w0Bc4ZjU9Ecq+RSsLqYzyy3w3jMdcuJl8O09nYGFRK+H4b9QadMplJupflZm5GP8AylvKLWLkZtJhxH8DVHr4bhKK+089rh63HmZlDIRNqYczIAoFTOWd4dccMfW1ifwnEVtUIHyYKeGacCihJHuZ0fu+cii4FfMW2lyEf7UCXvftj1n05mTQ4RmRdlAnkXOt4X4HpdXkYnD+zU8m5z2sasBmsqCeJ6H7Pgqxa2ojkDpOXl8lny6+k9N6N/8ADHhf+4P6wv8Aw14WR/d/851wQfeS+OhlNWb3/wC3PUcP/wAN+GLqUH3e1oki5q/sLwj/ANDi/SacGTzdTkYWAoqjNFr3I/WYwytm5VqOd/YfhP8A6HF+kk6QK9iP1km937h1HxgGWDAUwrnoZGDCEAdIQM0BQwYsGEDFkcKAJdzUFNRqMepmUGOxtYhTGkGMV66xAMKzMN7PNEWIpm+IPqHSS/cTU4FoSRBhMB1ECdZXKxcLtBlgxZXJUkuRSpYFyQ14FwtMiXQoSgjN0lWByYS5SDx0meTwsYyBzCCw0fcKMlUamN1vRZEEiMYRZmpWbCjKhNBnSMVKklyQ2lQl61KkEKYZto17iJcUY8G6uBkWZlapSkqQQaIjWys/JMUZRlYNmDJtPvGDKCOCQfgzOQQOZXQzNxh23KdQRaZn/wCaGNTrU6ZG/SZcWUow2tzNQ1BZfmc7uNSSofENX+9tb6rDXxfVL1RT+olacNkzKCAb+Jtfw8sfwCYufOm747JtnHjuQH16cH/5SP4zhyAB9OR9KMLJ4coHWvzmLPpceMXuluUap6azQ+YzsHFj+Gdzw37Q+HYMIxM22u+0/wBJ5nFojmQMpqzxN+D7MarPjDq6AN0uYyuHyf31p6rH494VkHGtxA+zGo9fEtE59Orwn6OJ4LW+C6nSNTi/kCYvu2XshP5R4s7G79PpWnfE29t6ks18RqYMNl1UEnueZ8zTS60C8eLPXuoP+ksanxDTGhn1OM/42E5zw4b+KvZ9Q2r7D9JJ8yHjPio4+/6j/nknT1/i9nCEKCJYM7IQhCCJYMQIGEDAuWDEGgy7gXJcYKMGGrbTcSDCBmmW1GjkIuYMb19JpVpmx0lb0CEciW2ND0EzI80+oYwffqZxt07Y4+xTYeOkS+IjkTUH6gmwO8hphxNTyWH8ONjBLEbmx1yBEieiZbjyZY3G6o4XaBcMSoix1htwsBesJzxDbRRhI6g0ZYWwbi/Tzz0jOWLw17LXepqpaeo3E4nLJtFzXjQATnldOuE2U3ES0dkHJiXlisizBlmSdXJBLAkqFUzaZA1KhEQYbKwYyw456xUgPMKYt0A6GLqOsEUYJTgmxxDa0A89+kHtCqVHaVQvmN8xQPQDfuYuSZvJjoeH5Tky7aG6uJ0Dj1zMaHBnBw5GxZg6GiJ3Ex+KZlDKKUzzeSet2745e01RfcNW/wCLIFgnw8IrDLmUhhR55mnH4N4jlo5MxWaV+zTOP2uqf8pzmdvR1i5GjK6ZNjetVPUT0WD7pq9KFVsmPjqGIFxK/ZjAq0NRkHvOhpvC8GnQKrOa9zDLHLLmRSwnReGafG7Nkbziem5rmvPhwJp3/YrVdFWENJgu9kcqhRQEccMtasjNsVjUKigACh0ETqdDptUKz4Vb5miSdfWa0HNHgPhnfSqfrJOlJL1ifE5cES7nVkVy7gyXECuEDFXCBmgaDJcWDLuMBgMIGKBhg8TQGDGK5ETcIGQdDSftcoAnTc7V47Tl+FZEXIwc0xHE6HIvir7zy+Wbye7wZTHD/Q0pQgmmMCqxgqOYQYEHeLrvLVdw4bj2hvXbWt9Ac+kA9ZlyIVN9psI9YDChE5lIY9hOvjy04+XDc2zjrGiWMfFyuk7e23m1pa9ZZ5gr1jUFmZtakWMbbOnWRdML5Ebu4AhAzHvWvWKXGFHEanSAT7wkNdZm1uEufUYnJ0jMp5iSbnTFzyLkhGDOm3LQhzCgiXY95mtRDKhSobOgGUYXUyq5jsaRTCPSDVQuqzNagTKIhSjDa0qUekuRpJMS7sqD3IE+m4cQx4USugAnzbRZBj1uLIwtUcMR9DPcYftD4bl4Ofyz/wAYqcc5Lly3jdR1aEkTh1emzi8OfG/+FgY6U18FJJJIhJJJJJJJJJJJJJJJ8RBkuADLubArl3AuS4oRMsGBclxZMBhXAEKIEDDHSKENTEDlg8wbl3HaMU8zVh1ebF0ax7GYwYYMLJezjlZ06mPWYch9YKN7xoPO5Ok5AMZjyOn4WI+Jzvj+naea/LroS4ZWIPyJk1Z2uoBJIkx60fvryO4mbJl8zKWPeZwxsy5b8vkxuGp234WD4/mKfi5nx5Ch4jC4YTprVefa1PqjxwJnTl5oAMMq1iNYdiLkHJmGjLhEwAIUiDJz0mdhzNRXiIyCjN41jKFSS6kqb2xpJcqVDZGIPWXwBBuBWBzJJcoGW1pJF6SwOsoKYbWl1K6yxYgnqDArgN1hwGNtLYsdDwPQHX69cf7oG5j8T0mb7L6PJ+B3QzJ9jMfq1OSugVbnqZys9rtvqPH6n7KalDu02YN7djMRw+P6A+htQAPYkie9kh634q4eGT7S+MacgZ1V6/jx1/KbcH2zHTUaP88bf6GeoyafDlFZMSN9RObqPs54bnsnCUJ7qZftForB9qvC8tb3yYj/AMaf0nQweJ6HUf7HV4W+N4v9JwtR9jsRBOn1LKfZhOZqPsn4glnGceSvYw9r8jl7sEEWIGTJsIGx2v8AhF1PnTaTxjw82F1OKu6k1DxfaLxfTn1agt8ZFBlct9H/AF9DGRWF/wAxJPE4/tlrlWn0+Bz78iSG8v8A7/8Aq3Hgrl7oEsT0MjuEDFiEDJDklS4gQhAxYMPtHaFLBgAy7iDLkuATIDEGAximJBlq0geDCBigYQMiaDJcAGS5I0NL3V0iwZdyTXpjvf6TWekyaEWWM1Hmcc7y64zhBzCHEi8GTvMba0IGXB6G5RJijNwqIycwyeIDTUrNBXElS5VzWxpREGHAJlsaVJKuhKJJiBGQCoG7nmEDAjB6QlJuL3e8sGZpNoFgKi3FGoe+iGhZSGQOPoZbRHeCotrlkgkg3faHjQ0SosqLlamvF4prNFpm0+mbywxssBzEYPFNfp8/mpqMm7vbWD9YpycmMFvxRDLUx64tcvovgnia+J6IZKC5FO11HvOjPF/YdyNdqEvg47r857SWP0Kkkkk0EkkkkkIvrM+bQ6TOKzafG/1WaJIWS9lxn+zHhTsW8grfYNxJOzJD0ifCJJJJ0CwYVwBCHMkK5cG5dxArlg8RdwrihXzLuLuS4g6+JVxe7iWGiDQZdxYMK5AwNGBoi6hAyR4Mu4oGEDJGAy7i7lgyTfoydpqbF6zHpeEmjdU4Zdu+PRzcCDZ7wASeSZGa+BMkdmS+YsN8yriBlpVwCZLqaAiZUrcJN0QuAx9pC0WzRgqFpVwbkJqLK7lgxd3LuSNDSweYm7l3A7PUg8GOX1YHHtyJk3UOJpw5OQvv1maWdT6poDnGoINEmvyiim1j9ZGPIB7QtakHuWLylSOJZAI4MTkNTLfUek+w6D73qX/4AP8AOeznzjw4a/TYfvGm3qG7jvOrp/tRrcDBdViGQfSjMzKS1ivZSTg4PtTo8tBw2M/M6ePX6bKoOPMpB+Y3ySCRrksRW8EWCD9DBOQEWDOV/wCR/GvU7cJW8RG4sRVVJ5wHBu5m+fKn1P3STBk1LBuFMkPy5/a9XxcGXAUwrntc1gyAwZYMUO5LgAy7khXJcqVECuS4NyXEDJ4lAwSZLiDbhhuIi4StJHA3CBiQ0MGSNBhXFAwgeJI0GWnLgRQMZh5yCVvCjp4ukcBcRjPpjVNjiee13g+0EnmUWoQLlCO5V/MAEXBZppkwtUrcYovIG+Yg0NJui93zBLCIGXiy3Mom4JMYKK5LgyE1ICBEhMWDJcQaDLB94sGWOTAmjmMTg2OsQDzHIdr8+9QpPycv9YvKpviMcgMD8RJydeZzdZovcRN3hXheXxLOOCMQPqPv8RWg0WTXagIoIS/U3tPd6HT49LgXHjAFDtOfk8nrxO1rZ+HS4sWmTAEXaorpMup8M0eYEFADNL5ComZsx39Lnk5akcXVfZ5LJwt+k5WXwzWaZrx7uPbie0FnkLFu3q9aWPpNzOwXCV5DF4r4hpGAdmNdmE6On+037ubGQO9G51c+n0uUENjr5nMz+B6fJflkAzp7y9s+tnToYPGdJlPoygE9iZqGUZFtGBP1nktT4LqMXKciZhk1+jPpORQO3US9Mb0vbKdva7sh6g3JPJY/tDrEXaVRj70RJD8VXu8Mph3EgwweJ7GBXIDAuEDECBlgwJLijLkuLuTdxJGEyrgg3JcQK+JVygeJIgVwgeYuXdRBt1CDRV8SwZI4NCBiQYYMkZcfp/xkzMDH6c8GZt4akdPEfQI4VMuF6UQyw7mcK7Qx3vvxAL9hKuLYxioyb7wS3FCLLcVKLcTUZM3SXFbpYaIMJkIqvYwAYYa+G6fykkk4kIINGaNPo8+XlUO09SeIXKTtetrKTBFk1OqPCHI5yASj4U2OzvBsVD8mJ/HXLkmh9I+MH4ijifuDNe0rHqC5YNQvKIHUcdYa47Fe8drSl5F945OWAMBcbD908H2hrxW7p7wTfpNFk1pONaG0cmbcH2cAYHPkJHsOI77Nuv7VD+Lgg/E74THVk8zy555S6jtjJonRaXBplC41Cj6R4chjLGM3wIzag4LC5x7aZ3diKMWXappcLiQ3yYgjeLQcSSlzuvBjTmVh+HmI2DdyZZ44WMFDm3P04ESLBqON1bEXFlh3jpbGE9PJIEW2DG6ncFMh1NLRImd9ZjF1NTC3oXKfJOTw3Ss5O0fpJBbWWeKkm/xZse+L5fLBlSjPSByAwbkuQETJcq5VxS7lwbkuIXZEu4BMlxAw3MK4q4QPEkK5L4g3JcQYDxLBiwZdyRm6GDEgw1MkcGmnAfRcxgzXiNYxMZN4tStxQh4zQ9RuZg/YRivOdbP3+0EknrK3cCoDGjzKKrJEEtKuUZoLBl3BEZjTdyTUtjQkBJmjHgdzSiM02DeRxxOtixLiA4Fzln5NOuOBGm0SYgGy+ojse01nLXCgCA7X0iM+YYUu7JnDnK8u0xkhz5Sou6iWzsxsG5gbK7gsTD0rF7s8CdPTTNsbsRRgdws9wYzyU6bVqZTjda2X/WV5zoSCCCIc/DOo0tpMTNZWietRLaJOSho+4g49Wd3XjvGHU01GW8oPWFlMmPGQ5LbTwYrzWJNkEexUTZ5iPwTxEvgtiyzcz+2Lgb4TqBg1iE0qt6T7cz1h20LPXsBPEbGRvVz9J6jQasZ9KjE2wFGc/LPk4fTeCykUTUPegJFWT3itxfpfEB2oWeJykbGMlMbFgyw6Itr1MxZNbjXi7mPLrnY+kUJ1x8OVc75I6b5QTyQJnz6jFj6vOW+VnPLkwaWvUZ1nhnyxfJfhsfXlvSoJiMmpyk0eIjcmNrDUYRyI/N2Z0mGMYuVqmLv3gHGQeefrG71rjtL8xOLmgEKK/CJIzeh61JJPmxgmXUowdVGVcuCYwL3SboFyXEDuS4Fy4gVyShLkkl3KkiBXJcG5LkBgyXF7ql3cUMNDVom5YMk0AzXja0EwK3E04WsTGTeLRuhq8UtEyz6ZhpoVq5uCWJig/Eu5IwH5hCzxFIbaNElBAG6mvT4i56cCJwhmO0TsafEAAv6zlnnp0xxN0yBByOY1zf1lkbRx2gE2TPPvbtFIfWJl8RUbFYHqxBjyTumXVC+DOmHZrNuVU5N3NGj2jF+c5+divEHBqSPTdfSdrNxxt5d4ZL4B5hrj/aUTd+85ODU0BzZm8ZCw4egROdmls3YAW4HPcQcunUAG6jsYUYxXIMtqqip5mdtMLIyX1qHhykEBjxNBWwQAVJ7xObDYBSgRHsGblLUQCDNWgyDBkqvQ3b5nLXI7D1gCuwE3ad1YDnmGhXXOfIeFFRbvkyIQb+oggtsFGj9esvcSODyO3vPRjrXDhd/LOcW0WU/OCTaEBLMecjkURxFOQwNekibZc3IuoD9KEIJkPBNH5ljX7MhV+a7wc75NQv7NhUy0YuFR/tHH5SmIBpRxMZOXHxmUge80Y3xMoIYkfJkFkljQBuMTCwNv0mbNq1xghJiy6/K/BY17RTt+bhT0kCSecOZiep/WSWw8+YBjSsAiZ266BBMOA00AGSQyppkQklSXUkIQoFyXJDuUTBJg3ECuXcCS4hCZYMEygaiyYTIDAuzCEkcp4Ebjam+sUBxIDzM1uOhjaG/MyYnj905tikJsQN3Mm6SPwgmzNKYnNHaaPxFYBSAn6zbhDuQLMxlk3jDtJjprInUxjv0EzYse0AWZsxKaup5srt2k0ujXN/WDQB+Y1V4oAwciUDwQZjZjJkNGK1ALYxGZAb5lld2P6Tria5OfHvUgcEdJyMztjyEG1YTv5F5NzFqtMmYU457N7T0YZfbj5ML3HNTWOhvidPw7xNcmQIx2t7e84+XSPjeiePeWmEqQe/adMscbHHG5SvcYXujH5eQNp695zfDWZ9Njb3E2NYXk0Lnk1y9AgrNzfMDIpdSAeR3kTJZPEh5se8kWF49XBjsKIuSz0I5+ItRS88mEGIIrg9ZbFjdZUBbNdjCRzkS6o/EWuoXyxuPajMen16aXHk80FvWdoE6ePiuOc3G91yOLURbHHhW8xA/Oc3UePFn2Iu1ehM5mfUOznzMpY/Wd9uemzUBDkZksiJTUjGSBcznVsE2gfnEPk3cnrMSNbb8mvyuu0kVMgzMSZR4xbr5ikNxRxYnrBlXLkEqSSSRYfENDl0GsfT5uqngjuPeZGFT3/wBsfD/O8N+9BRvwGz8qeDPAZeBOPjz9pt2ymqSYthZjIJnWMF1JUIwTNAJ4lXLMoiIVcu4PMkQMGVcEGXFLuVcoyriyK4JMEmUOYwUYMYsWBDWVUjQOglE8wVMtveYbEr7TNSsGXic/dbTRiauO0LFKebloCzBfcyhzG6RQdXjB6XM2tOphwFgBXSdbT6dUUGZsG0de86WBQy3dTyZ5V6MYZixDqTHLjHuZA4CVQl+bwAOP85yJgQKpa79/iC4Dodp57Sw4K11P84rLkXaew/lIsufEV5P58zP35uprYqQASSPc95mytxtVanSVovNiLqHxi16GZsuKdLFm2oioC25iDxHZNMmTleOOk3tnbgPp94orx8xePw4FwD3nb+6N14qEuJMYN8ma96zcYLBiGLEqqOAIL5Q52HgynysDz094rcrAkUT7zMFETsNDn6w1fd1NH2ifNBU7q4HB95Au9Qb9V8c9Y6Gzyyiwp6SEgdfaRFCCr+piMzWSBxXSGiHLkohlPJPSZtWSdEzd98Ine3HQStVS+Hm+7ipudxizhyLqNTIyqQDwexFwCAb4qUOBO23HR+PG2Syouog2MhDcVGYsr4nBviFqArEsO8NnS7Hl0ICiopSQDGL0kBSxKEvmSXQkkoyQ2X0DW6V9Vo82I9HUryJ8s1eFsOXJicUyEgz6hj1GXI+112fn1niftdpfI8UbIANuUbrHv3nk8N1dPTnNzbzYFCLY0Y1uAZnYz2RxqSQTKiBSpVmUSYhHYAQQ1wX5MgUzTI5LqQKZeyRKZiTBuNOMStoEdxnVALMISEHsJYxt7R2NLENTKCHvLqoIW6XvFRZ4lSW1G74mjCbWIIjMJO6pXpY9taGaNM1ahDfeZ16Q0NN9JyrrHex5K5a5rx6mkJ3VQucbDqDsZz7VzI2rXgAjkXZnK4bb9nZHiHrpb+OZrxawlObueaGrqiGqxx7mMTVGx6rb+UzfGZk9H94J6nn3gHUN03A/HW5ycWpv8TX/ACj1z7unIuZ9WpW45QeG6jpUXkydxXEz+Z8iCWLE80PaWmttmk1LbXx+W6ki7E2Ix8sAk389Zh0rZRjJXIGF9CKqMbMF4WyxlQ1NkBPXkReQqRcSLr1EWesTkYsuwGvaUi2c7LtIJFVxEr+xQ9K6GZ/VVHk1wfeCcxsAj6TpIxaazguF633mrFtCdeR0My4lLJubgR6mkAQ0B+sKoY9jaQSSOsU3PH6y2ahZa4WlAdHLfiPSBKIHQcRHibAafDjPez9JoZfVxOf4iBkzEjIBsG2iKjj2MumIttNGACzNLdWHX8iOYvcR0nZyNLkmoGXIwWhCQ3A1PAEgZpPUrX1EeBE6MepvlY6zC1LEKzVSuIJb2gR7pIu5JJ9E4DCxZM4X2u0q5fCzkCEvjYG/jvPQrjDeotRHaJ1uH7zp3xkAh1I+s8WO5dvTbvh8kyCpnabNbiODUZMTdUYqZkae6OFLMkhlCaC5UuSiTwJBp8L8PfxLX49LjNbjyfYTr/aL7LZvCsK5sOXzsf7wqisxeA6oeG+ILqsiFgOwnV8W+0ufXl0xY/LxMKpuTC274M08gGYN3McAx7GavLXrQuVQ7TW2WcYmPUwxiA6xnSQMPa5bAdoHaVcPrKI4kAGCeIdGAwqaQTzKjKhKgaWxoCKxIAFkzp+H6LdlG9efaL0ultwfaeh8OwDdbde0Nlk8U8JOHAupwj0/vD/WcifQsR05xFMzKARyDPF+MafTabWEabKGRua9oZY/Jxy+GMOehM0piVz6hwBMqkWKj8bktQBLX0Auc66RsxaVMqMQBY/lLfQKRwKjfDcpTUhMq0G4o8TqZcBUm+053KytSOGdJkxKWU2T2lIcw/Hf0nWOG/pByacXL3OmHHkIrca9zNmHJp1ay+4+x6QG01iqiM2mINAcy4p5dAapDwrf5SzkCncjAgfu1OTtyYjQJ/OENTlX8QBjqDdbxqCC1gheDZixmY5D1KhruZW1bOACKqOwapE4rkx0NtSqxYmwAP5S1x48S7mtueL7RaOoXjizzISX5IvuBBH+bjYLS1Z7QdQxCgKBZ9jczkl3IqgOh6cy9xBDFr7VLS20BvQBzdQsbFLA6xKGga5MvEwyPz6a6zLTZjUIrZcotVFmcrUHTZEDo7YwT+I+sfqJ0tc2oGg26RwchN8GjU882qcORmx+Vm7uq7b/AMQ6Ga8c42xneRZlyYwK27ezJyGiGFi6o94YzkE0qqe4HQyn9fqQV7idGFY2AEXnbcIaYy0rJhYKSJI3REeZQb92OBNkTJoWrPR9jNANsahUM3fEEA7uYwdLlkj84FKkhAcSST6C72/qr8oORyLUsAg73MebJhVN+o1S41vm2qcTW/aLQ4i2PE75x2ocfrPLjjb072yduJ9rcGPH4oz4mBXIAT9Z51gSeBOx4hr31tbkVQOk54AB6T14yycuOWU3wzDGx7Q1w+5jpXPtNbZ2AY1EYFAlAGEAZBJONpJPPtIfmVUEGjJRjAB3kIF8R2i9srbUZ2gGSTiUZJIgJBPSUyUaMIsIJa4pAtmPxptPIiVIHNQi7MesQ1jVLj6DkQj4pqONh2kd5hI79ZYHxJH5NXqMpJfKxv5iuD1u5KkqSQGukbjzPjcOjFWHQjtFAQ6AHzM2balO893fezlnu7PW56LwvXjV4NmQjzF457ieXG6+OLj9PlOHOjC6B6A1c55YbjUyeqc8EgywQWAbpXM5mHXtkxuwHpXlvia2zMFUurIO9zjqx120HYQbdVAHtyZjYrkLKCee8WupGTcEFgSF9+IK3pCihUZKtj2IVZmr0+/aJbCG71YscdZBtUVu7R+XKmbUIRexQBXwI9DbAcL3t2EGri3xuvM35BubcOOZbIGVQSCfb2mthzDkypyOnzDx6yjySDNmTTLVggnuJj1GBEBLdIyyitXmjIPx8/EZiZWWj1vqJ586hkf0n0zXi1Zrk8RsUrqZM1+hWFd6hYcu0gCtvc+05R1BJ47zdoF3hsbnluCDM6O2nxB8uNhl2jLgr0shor8gzIx+949q5A57WKYfl/SPxu+lBTh8R6of9PaJy6VMijJpjZvlboj8puOdYvLZWpgQRDAqPBymlyjcB2bqPzlMgHQRQUhnn84IFQwLEEzth8vMuRR35E0sgXoOsHIrEek8x6oX06ueo4MzaZCATdVcZ6V5Y1J67pKFyMONrjmBWHx9iCJJmOJAaDgD2kinPfK+RrdmY/JuC1rwZVS662OfmbYDcksKTBIkl314lgjvBlyIgRLviCBLriCWTK4o31lWJCy8Ub94pJLgNkF9hFtmHbmOhs1mA6G4BYRJdm6SDGxPMdDY/MHQcyEsfiRVqGuMnkxRQUk88xgx12jAAIRJIltaLoVKAhkVBA5klha7wgPaDILMEKpKlUbkIkhLV8yiR2gk0OkWXJ+JI3fUrzDdwASe0sY2PIHEkfh1LK4Iah7Tp49XlfL5em1Lg5SAQ/f3nG2HtHY0J6kgzGWMrcthianLg3opBs0TUM6zNv8AWKB7AS0RMa7rs3BysMjcCXBbMDK53brmpaBvgGcfErKSbqNx6llJsbvkzNh265YkdiJe49enE5S6rJVChG+ezKATyJnS21PqlXgfinO1DPnUhoZMgHWanCrnDQ5mfaK59zCXS5lNM9CdFVlEBSD1mts6Dhw40Wz6j2vtNYtimRTRHX6xCdfVGrwOJITFm/EefeApIPMs3IoF8wRpffyxJPyZVAyKvMa2MIoN9ZbRewVKqodg9JXF8y2gkcX3j8HGBwR3uL28cCUG27hfBmKYPgsOw95pvAVrYcjDvMWMktsomxNaZtJpyAEbO187jQ/QQ1slEaZjZwgSTUdWXO4aZAD0AQSS0nlal9T8mSoJM6sLa1JXvA4kI7kyq9ohdSQSyr+JgIp9QgPp5lpbPuC+QDgkCZmzO3Tj6RfU2TcdLZ7Zl7WYJysRxxBVD7RqoNtER4gJ2knkkxiIPaM2ipAJbWlUBL5aGEUxuLH6uV4hs6LRPeaAi11mgquTau0LNraLDjwhhTE+8zcjpxWWjBLV0m/UY8Oz00GmXy194yrRFM/SWE7XD4JpYLEKevMtjSiKNQd9SZLB+sWzAdYoZc9RK3mDu4gk8RRhf3MvgngRNXDV9qkVZkjQjFbAJhY223uaviKXO6ptEAW55MCf59vYE0DIDhsDkzGuPmOTqFhTD9vpBBhBahIAFhBwAQRzMtANleItUrrH0dvAkRLv3kEC0oMPaCLAk2m6hqpHWBUqWvWWFox2MAiWUEgDbYgMtGhHj0yGiIgkdekYFkoS7EkoiTY3aELPIkuu8NnS146iWzE9ZXq27q494JbmG1oSmjG49Pl1GSsaH5NcCDj9R3Km3GhBZjzOl/bQxL5eFGUkfiPNzN2VZNJkOnGLBi/CLLMQN36xOXw7UYcO9k80HtiIcj61B8/JnfdYsngXVGOxtqDTOaA43Ht9IyRM2jzbQ3l6Bd4O3zMqEsv0vpH4dH5j3kcYx3erI/KaMmuVPT6iwHU8TA+qfLxj3i/fia0Gp9BmZ2OPIrLfBZgD+ck55Qsba7+DJDS24W4d4nJnRe9/SZCWbqxlbROunPZzan+Ff1iTmyvwDX0kr2ENEYniKJpifUYSrNCaezyY06Ug8HiHsdMoX5jseBmG4A1GPhUOEQ37mbVzLh0xwlQWI4aZuRkYjjK1KKkdR1jd9CzVyZc29RwLEtrQChXrKALGrgszMbJhqp7xRyIFIPWMOSLANDmGFszJQZCDcJ8+RhW41BKgCyYosB3khEkwCakOQRZazFLL0OItjcj8QSTEC5K3B2E8y0PvGihz2ltaIC2eZfCmH1MFluWzoN8y6vmWMfvDCEdogorcPGvMMJ7xi46I4hsiVOYSoL6xxT0jiFiQEzOypWriFsB5h+WC3SPTDxdQIMabhQEnllTNCKQZTjnkSBKId0ZQkF9o4YhkXcn4h1EkBBt5riMJx11ii9LtBiiYo0gQeJAQRz1kBFwtSyvzJ6RIbMrb+syT9NgOoybQ4Xi+YnICmQqTdTRo9I2d637a7DrN76DSYEyHUkEqKUB+SZm5SXRkrkFmqu0LFiLuu4gITW49Jsw6TTZvUc2TEvyu7+hjW02mDf8AlRvQtW5z/pNBWXYcY25dxWgFCUInHiUu2/8AZnsSK5/0jwwxDbtth3HWZ2ysWYY6C91J7yK9RjxYALybyeeBcS2TI6/jJA/iNVGeWWACjdv7SajFjxnbuYsOoBuoywaJUtYHv1symxvv9Lkc9AYYA28la/hNwmVNobaefiILBzjo5qSMLAcVX+HpJEPIjHZhDGO8ZtIlkgdSJrbOghQO0sA1YkU72pRf0jAgu2PHtDZTBhfK4CkD5PaOzbcDhPM3+9doLZQFC4xtAiG6wLUufT4W3Khcn37TPny+a9gbV9ouTrJbWqkxgQCCgK94zqeZJYRZfEE89IPTqZI3cAYJykHiATKv0kGSR8paAXEGxzcGKETcq5VyUSIhVyS1QnrLOMiSS+Klqx6S/LsfMNcW0XDZRRZ+I7YCtVAHB5jl5ECHZxVQ1UVREMLxcneBCU46QkShZHXpCAuatgbSj3Ux2CV54jvLHUcQMaEN0mpcdyRap3McDxxKquJAQIIdAd4OQynYfnJ5WV0LEbVHc8SQASvNSvNdHDpd9x7zfp8+FcPl53Rk+kUNPocmb9jqyhP7p5Ex7HRqaBNdhObBkC5O6Gc3UYs2B9uXGV+T0/WdBsX3XMMquzgdSneP/tHBlQpkQ5kPBUjkQ9rFqOV5WRaLVt9xAdf4CdwnWdPDhpQUcj/hM5gUZsxXEeRdAewlMtnR2lxu/qL47H7pNR+bDjyKRhdUYdf/ALmLIVVTs232LDkyIxIAIosPxKYrTRh0r42A8wUefe4OfK+PLuAD2OldIOmZyTjdq49JroYTYsjWXIDAcsP3hD5QgzZBbFQD1oj+UZ52DArIgyOT78AzNjXHiG8tuPsZbO7U1UL6iOjs7crix6T7E8wKIY2Sb95eQqT5igEHpTdPrIxLpvJ+DXvGCixsU9eJ2VgO3WQMTyW4/e6C4kAE3YH1EpRZrdZJ7TWmdmhuSRe3muOYA5NsSCPY3ciqLPqoTSmmL4/MDIQOtCjLpBGTRIoXINSHrmqr8pIHqbnaW+akhyXnMjoT6BwIlUXducbviHtEhoCaYEMhApFCj4lcmAXAlHIx6SRh4ECTY5PMvYZJQUkcQ1T3ghisJsnFSS2IJpbkBrrBBjFTdV9JFW6uJCRUjYlVupqVt7SSIATUjIS5vpLCkMI0jdwZInansIJ7gDiMCAHrDVB7S2dMq4yTGjERNKYhfIlhavvLa0Qqi4wixVStpuEeBAlbaMPjpCo+0nlsTwJIthDxEkQjiN8y0Gxq95I1QStS0Qd+sLtxCC0LkjcenZsJygekGozHVFT0MPTOf7Lf5f8A1iSamdoagAxgIELRYcGQs2oy7UXsOpjhqvD0J36fcOxsy2mViS3EYumyOQWIRfcma8fiHh+JPM+7mj/xRH9o6DKXK6Vjt5PJ5h7X6RhyaXRgFQMuT3PMx6jXvqcoHUk0FE1Y9X4fl2r9x5boObM0n7r4dqkZdEnmkWKH4Zn218HTnajS/d8YbMAHPIX2mZdK+b1IoAHViaAnU1WsTVJuTEga+SRdTI6GuDuo1xKZXS0PAy6ZbfIcvsAeIvI/mZTkVAhI6LGppVB9d0IKuNrKgKuv4b7w2dBGIMGZm2HuIo1jdlwkhu5HHE05kVV9TDcV69OZhyKyLxlB7VGcq8GKlsoc7q71NORTkAdgqKvA2LX+Uz4n2ikSiaPuZZytuG9eDyO3MdcrYnIcDd1717xqtkdSjHco5JHtM4TKCMg492BuoKZf2lljQPM1oD3quQnaCp9444w6WGGIk8erivz6RW9fMPDbT1A4qGvlAlioIroeh/KVgiHS51Ad8GTIKs0LH6iUu7Gx2iuOQen5iLC5MQtNyoTfp4r6VGjWZhwCXY8AOLr/AFkkC72AIsnptIjMmnfFxlDAnpG4To7LZcb4XI6g7lPwAR/rCXVCtqZGzJdFMiEFfzl7VaZwSHBxsCQePf8ASRjybJJ9veOdMT2BuxPf744/IiBjXEuU+e9p0Pl9/wA4+w0BbYX5qr8N1kjWOJDWLUqEPIBHMkPZbjyO72lHnrJGYsJyGr4m2SwLjcSC7PWahhFBajl0SCveGzplZXLDt7SmxMoJJnTXADTOL+YvU6cm6PEtrTjkG+YQ2945sLMeBwIHksOYo7GuPy/mVfsJePGAOTzDUAc94EAxlx7QxjCAk8mTdzY6QXcmCUDZMKuOIKLZjR6TIh8uMUDpXSVyTDAoyK6uTZQjMeJsrhUFkzo6HT49PhyazVrwtqinufeZt0nF2cywnIjSxfIWoDcb+ksqABNgGy4VVzUvkHiEeYIDOByYzTphyhnysQi+0Q67jQm7T4R9wYgClb1SvSGq+Hd2y/rNeHR6LPiZly5FWvxHpE+HaNNRuzZzs06nqe86GbP4RtGMuWA4AHAnK5fBZsegxt4c2PT5w5LWLHzJg8H1hyAZEUrXvG5temk8M36TEoO6hf1nJz+NeJ6lbViAPaU970rY7GHwMYkyLqcwxpd3KfF4LhpTlbK31heBa5tTo3+9s7MnUVFapvDcrELhO/3Aqpn9t6qYtadAeMOMgDoLgaPIhyN5i7UK9ajj5C/7HGKHFnrIwxsS+fIw2/wjp+U37ahkafDSmFQ4QPnNjGx/CnyYrWrlbIfvDbmNjj46xSZ8O+vVgN0x68fT3/rLOuwlmyaXTPdkW7cfJr3nP9t7jWppF07Y2cIpCtRCt2j8SnGyhiNt8VM2RmzAZMbnhabmriBmyq/l7zR4AbtNSWxXhpy6rI+U+WAEUkV3iUfbn81mDV7jqagAgEMBbWeetmGnlOpauF/EK6ia1pk1M7uuTzF3GwQ1cCJzj9uS7cnn00f0k1WU0caAhLvpzzFBXxkrQBrkGOM+VV4WdFKKqm2tbHI+L9pBmckH966oDmCr5NimjdUDCbcymqYnrY5HzNAxEzZN2yyO/a4JwnaCFoHuekOguIrke8tDbsNgj2MFSS6rkcsoFEryRCVWLUMv8PSrqTYB25PeHuCrWwgnkfSRmJXcgIVeOs1saRSeqtZHFXCO08VTda9oJK+Wp6u3J2muPapYKre6iL6bYex0uwbADE135/SWtbdvILdGvpALPkVQigHvRPqkUsFohQK+tf0ltGZHKZAeQtckGwYvNmd3DUVLd/cS6ajsJFdSOYGRtwUbntT9RXxGQbCCK9RT/wCPeST1npX5iSIchdLkYXxX1mvDgZFqhEaVjtO4/SWczo/BhtadHAiA249XzJlfHuscn4mTzyy3fMBSxU8wLcurVeq8CKfVB7NCvaZCCT8QNpBkjTkUjgRRNyubkqKTvIb7QgoqRge0kAccGWFJhBCesZjQ8+0kWqkVD23zHAKOIWwAXxDaKA7RirxCoECoRG3pzIun4Lpj5ebUv+EDaDM3iWq85xhT/ZY+gHczdqcjJ4LgxYGADfiPzOEdwPMzjN3dFQ+nmSwwsSzTUvWAU5oWL6WJ0CM1NxKL8fMA+ZicNtsidBM+k1iBM6DFm6Bh3hbpJ4Z5RyNizC944M1+F4Dm1efROPR+8Zy9Rh1Wk1GNExlmYjYR3nqcZTR4MYZazZaDlROXkuuvlqOL43rUCDRachceLg13nn0zp5qi+hnqNZ4HhfVO5zsu/wBXM548E0W9t2a1Xi1E3jljILKZqzv8HQL3cfzmEYNRkA2UFA96nSK4vKTAo9OM2CT1MsqfoStD5hMtRaDoDn0mLIEyc5ABZHT6ShkxUdzHdfNqTdfSaNPgyKpbYcioN2T/AIe0xahg2Q4sLXYs0ORM91roY1OPfvAPXla5+srV52LIPL2AGxfeJ0yqqnfjLZD3J/D+ULIwK+WtsSfxmOuV8FlDmfI+TIFKiwgBt/pKGTzM4G0Yr6ADi4efIxIViDQod6/OMwafJqMZdcmFEChWvk8fHvK3XNM54K2sFIDDe3XngSPiyrjxs/7/AEN9RGZQ2INjLkBhY+RFHKz4wHcEAUvwBGbFQEhqLBVHUmMxMcjumGihFlmFEAdai3T0owNbl5P51J6VAVWsXZbbREQZmVRkKowccUR3lqgH7y32+bi8RZ3CqSSOlQ1C/hBNg+/H6xRibCpBDA9SB0+sL9kcwDgqgHX3kOoyOuw5QAzWxPeEMwZdu1FboDzzDZ0oKt7lUkDse8LFp1yhivbsOTLAO8M4Oz4MAIxbdsfaDZrqPmN/g/1bYhjyFSHDAcKVNj/pFuo9O31MKII55/OasgTd5mk1WViwpg1hpMWnyPS4+p6g83CS9q0sABDkAYPVcmwP8pSeWM23UE4w44bki+1/HzNBXKiPiyudp/EBxz7ERJVcuIEZAa4o3yPmWqdorbnPpLjgWCOJThqDbeHNLXQn2hY0y413B1UBSu7bxz8+8W6OQMbsieUfw3R57/MgLLiKHaOK6heh56QTbNbbTxXp4/7MB/wud5dg1cdCPf6wxvyMMpy5CQByTzGCrKkGiu8+9EySiOTyOvc8yRThYBbVNXkA8nrFaelyggXNbuKuuZlM3lgHrGlNtUeJaJY3EyNz8yIWI6CKJ5jCtm5NgEQDYSLk8s+0bXEu7MUSEO3mWIwjcaAhLirrJARbMMoa4Maq0ITdZIpcZvmPpAoBHMEyc9YJAADwJdXIqs7hUUsx7CbV0SYV363IF/4AeTC2RH6BF1nh2TCb3YzYMTm0eHBjLZGGVh+6O00aPVZPvAxafTFMJHtVzFlw59PqnBxuV3cEjtOc3ss/3zbjIx4lW+4EPH4nQCvjVx8iZddifBlpVpW5A9orym8u9wBnX1lG3XOHR65Ayk4m+Jj1Hg+TG29MgyAcgxGJcmFgwyWPia8WsfM+za27sVmeZ0u27wvUNlZceox+tPwmaTr3yah/OCY1U1YnOw7sr0Dte6BAomRU9e0raq1Eg3Odk21Nm+IZU1moQq7Uor/FFBDu2GvLHauDNWT7mifshks16mI49ukUSMKb8pKg9Ce8ZeNQ6NRdObU6fHZHDAm/zhNlGIZNOr40xH0kAAFh83zMTeJNiF4UX1D8QHPt+UxZ8wy5N3lhR3F3KY21cOoviHktjx6TGC62AyNR57Tk7Wy6hlxqTkZuFH+kMPWLj8e6x8RakggbjwZuTXQvLZp8+XBib/Zj239YrFkC+ZkZVKE8gnqTKRlbGce0bybLXyRMzeYRSg9ZaWzWCbhS0O59o5NSUyhlpWArgdpnt8a+WR67rdfA+D7wfXkPpcBeASe0UZnBbIAwI3VRH+kdgwrwVXzcnQoeKicSj1EEtX+UZgXM+QjCHc8nd0helAKo9QexfNyDGTjDMaF1z1Imw5ceI7tUgz565U0APa/f6zM4fLeZgxQGiQOBKZbViZP2ZIxWEPQ1RMWDd2AOOABQM0I6tZ3MWFeotxQlHGMpAtjkPXjrGBWEA4hvFqO10fyh6nyqrDtCEWBzuJ9iOxgHEq5FGQMi0LPevoZEIVrOFMqj3JBIkR+ZQAYKVIPAHIhK6oxDlSi8XjawYp3UIoOLa1dVPX2uUFIUliKb9DHQ21feMYA2IKHFr6WI73GDUYfMICehT1bkzHSoeDQ6dLuOUrgyEZsJY8FRddfeoXhNeDOTnsn0E88XJifGHY48e87vwczO750xbdg2udw2rF769Sggmivq6Rl2tNGXKyOOAocbgGv6QAQ+0cvlfoK6f1gO6AhhkGQsAXJBFHuOYtMrIW8hwpqrHeWhszlfQqq9t9DLxh8hvHQ5NFm6fBlDYcJG1jkc8niq/rBIGQBPLAZerWbPxImKjgV5QP1xg/zkk/8AOgL5a5ylccbv86kmeU5CbVYcRhKk1UW1gWIwmwCw5mkoGuOxhAASUB0lkGukEgAJqG2MEcGCFsXGiIAMRHFyFAsYSJR5XpEBFDkSXcgq6MsDmhJIORL6LzC4VqM06bw/U6xd2NNuMfvtwJW6TEeOs2abQPkTzM7eVi689TNJXSaJtuJTqdT71wP6QnyJhXzta+/L+7jHQTFy+iZhxuT5eiw+Vj/ezN3/AKxep1Og0JYLeoz/AMTc1OZrPFNTnbbu2J2AmEtZu+TKYb7Xt9NL6/UvkORW210Am5vFtV/Z65wQxU0wM5I9Q9IJ+k16M1iy4MqsEcdxHLGKWmr4n96ws+bAHKdeJMKaXU1WBlvpzUrTaby38vGpO7lj/wB9oLZ9OmSsbtkUj8ZWq+Jm63qNSNOLR4zWRgFx3wDZY11oCTzxptVWiCO1kIdvQH/WLOXJgDZMTBSgvkctfFRWnyFdO2QsAxs8GqmPW3vpreujn1LJnIbGtOKuvV/0gpqMdPsUlN13toRBybsIxsFL9d/eq6RWLI6co7AAnevb44m5jGdiy5shX+EC+kVkL5FBfJfsIZW/xruDdKPSNxuGZVyn0AUC3aa6RGJyBtP4e6mMy5FcL+zAIFMR3MpQWYgKzt7gdIJAKkk8DjgSBrKpKjGb9Nk/MWQqKCTuv45lo/7xPTtL27kJBIN8GuIpSjgsejGUPTa2NrUSPeWTkGXcr7y3AqAxIYoyjeDwDxUkbnYu5UYwOOi8gRONwikFL73fEluEALVYocyimTJYrhBZ6cS19rYlba5x9FLAkkdJ0i+PDixvpz+JvSG4Ne5H/dzC4wnL/wCWxuFIA2sdxJ7x2PGGdTqFIXaFXe1VX+k55avNaxK07ltQjHCMnJNN0PzzGZMzY3KhWx+og3VDiukoZBizA4g2NVYABjf5iTPky5yXAVkBPFdPrLunqF4220q9QbBv9Y3HlKk1kfGT/Cav6yKRkwb1bCHTgDbRI9/ygNiBxhg7F/3lK/6zcu2dGLu1BRWGMV+8Tt3fJPvBxsiFgyg30tqIlbguEFty80KH/fMZlBxlciFCCLAZef07SRTlefUCPYCWqnaCoLA9L4hAu6WSgC+mviUG2c+naT6uJpkJf9qrBCOaCngX9Yen3HIC6kqOSAagg2vcoOfi5q0rYX34/Jdcxogg8V9IXiGdjbKNwY4iQetNyTCXEMqKfLAJHC9Jeo0pwKHe9re3WpnRK4I56rRoiYmrOGv9NGKg+Ullo16fn3lgYfxpS5BwaEQEbJSHeWZuPkzQ+PT4CRbjKnUFeDXyJW64qk2m/Toyndv2iwt0QfqIpv2efJlyYhbqSqmyOe4+YCEnM2chWF2QTLPmbUd8gcL+EEWBcdDYsGHWuhOH1LfbJXP6yR+lxaJsN6plOS+z1xJMXPV/+Gpjw5C4wT6oYAEtCBCIvmdnIGzm6hVxUvoK6ybtpsCSEgBlkiqrmAuS+oAjEUkFqkghR1Mrm6EclMaIkACk1zJM7+k895FcE0OojXpiRUzhGOUKnUmpJr0uA5mOTLxiT8R9/ia8/ipyr5e4phUUFXi5m1WZsWD7kppRy3zMDOB0mZN80ti67YD5SBAP1mHJlZ3LubJgkkqSBKXFlcAhSAeLPE1qQNg1uiVQPuas3cnvGpr6IOHRY+elATK2hGJBkyuCp7KQJr0WBdpdWpEBcC+pHaYyuMmzJbT21OrFNkxY8Snooq5RzK+bzBksgVRa+ehnJ3t5ysSWN889Y/S4t2ZWY36jQHX/AOoXEwep3cJj6CyeeZnOLIw6AKD2PX+s3uExepmUe19bmXK6lgFO/H1oiuYwhDZmLbnDE889q9o3Fhz58ZVLs/u12+sUcdCxZHwYzHq3xKhxkApYr3jf4FHT5EcJtDkmgAebj0x4seJ8OfD+2BNEDr36wU1hGR8mTEtutCuACO8vJnfJifLnF5Mg24yfbuQPaHKZS5PRqANgQVN3uF83z7yAWLG6ielR4xqceQKTvADKpX597/ONulCrXyqo7r4YGv8A7hlhiUrjLMzddy0VgHHmNiuhog9ZH3kAtfSwT3/rJIAGUk0CfYQl9IAPWrocwMe4mh+7zUMIcblsgBrki4pZUEMSQpUVtPf6SZMvnFd5FKKWzdD2hUyKucsCWJI9/r+stcTIQ1KSOfUBXv8AnM8Q9kZGTzKO11A6gyjbknEPSvJsd4aqfMK5NtK3qauJbFGRh5myha0nDH4MdpelFI+r9Hl4ip2E9TfSWX+95Sc2QCuQ230g/MW258O6hQFGh0rvDxsqYNu5gWa7ANEe0zZ8mX4Uch2gFN/1N1KBy8gUvue35wwjuQQrZMdcbR0+IONvwjaWoV7E88/XiPCXk8tMI2YyDYBs3u949A+3fkKFTXfqBBxeYcq4tPiYPv43UB+ftCGPI2oy5AjEI3W6on5mbTpM1lyiqAGIdeKBB9gYpmZHYYzYA4vkxjHawBxMTyQN3FfEBspIdzjGTc3L88X2moyT5mTz/NK2QLYV/MRwy487AoF8x/3UFD9OxgFLF79/8VdR9ZWzH5m7lUq+nM0DzgyDTh6ZcOQ8fkf5wmXPp9WHD7cijgqbsV/mInUMSz+WbxswPqHJIHtHaMZ9PkbJjUkotsCAaHTpM3euTxszCr6hCjZnyFTwhbkH4EsY2DbsxAF7SQQGUj4mfOzZshyAbeb4FC/9DCxEANeJsmTsSeFhzpcHptV089XDHkE8Dj6RaYcuVyVQvbdxz+sEeYCwdWs8N2j8j48enVMaPuPHLekEd6+kuj2vTE48ZrH5j8qBfT9YpMb7lRRbsfSiOGP6DpA8gqhzBTRPXngjtDV9Q+QOjsjICqHGoHXtctd1bVqMqnMxZVdjRJHHNfHEkSAyWpsm+akmpOGQKvt3hG14hqRKdA3TrNMhYkgn2iwxI2yHcODBNWBX5yQ1AHW4xGZeB09oqzfEYG9Nd5IQch+OJRyHmJdqbiUWuSE2T0+xmnwsBtQcjfgxLuJmAncdqgsfibFyjT6FsArzMhPmcXtHtM5Uxmz5W1GZ3ANsboSxosrOFY7Se1WY7A2PftQI7EG6Yjb+UyZGy+dlTAM1XzZ5H5iHt8Q+vy6D4cWl06uro4bpbcwNRqtKSgV8jUAT6e/9JlQYVJTKUXIBxfIHx7RXmFgQFTnpx0mZjb21bJ025PET5J8vHiVnBtqBcG/5TOM5dUR3O0Enp07RapsdlLKQeLHeMxFcTkqATt7jpNTGTpm20WXITSsBS9PTRPzDVlG9nqlAO5T0PtG5cWEqMxchfxH3MzO2NkGNCVQ+oknqfyjvaaN+ndFBALkcAHkf0ifMBvdiXd0BEXjRRidiwHTgHkiPw6LVOBkVCuMkCyR+UOIeaUWcbgymx0AFV72ITLYR3VKdTsKtZu+/tG6vHj0+YqudWyA/ucgD2vvLyOX2goVIHQDaBftLe+YtfYcmPy0x+kW4IIvn6wTkyFgS+9q4LdeO0sny2cqSEqgX6gxXpVSpLK45HPeM5BhxhQBjpmZboduZM+MrtVtpZuy9RFEHejOpp+QFNXHpkVMzpnUOdtJRPBhbTIvCynC2HGpBK7nLGzx2+IkN+0CIbrueIQwnHkLN0Boc2P1g7fMJONO9AdTKaVMdl3FUVieyk2AZFUoDuVQyuCLHSLdVCqGZrv1ADoI3yw2FsyM+z/iFkyTVqm0pwDJplNHJzuPN+0yDL5h9ZJrmvaXjPnqmNVxIVFNkI/zMsDNplUMm0sCyP046WIT6NNz6Ssq1R8zHvQCzYHvfSZk2FcigqSBuXi7PsIzGuXUOUQ7mx4y1k9AIGmOFVdsqvuYUrA0JcyDcqhj9Kb39DA3RuoA3spKMQFHIJq6r+sYzL5gKbn3AFqWqPt/1jHRvU2JmCZiQfc9yDHaRlTG7rjyE41F7XNWYjePuoGQNe70e3z8yyEKc07N062DLbDhuhvO2hRPf2lrS2DcdhBv4bvG48+bSLlxYMgZH6kd66H4kyufLbHtJUG7Lcj6CaMK+H5cQyajU5ceVjbIuOx9bhlZrmGd8F6dcufYdOjnMtDag4r3jdQGx5Crgea/+1G3p/wB9QZWFxkTyMONjlDE4mC0ci30NdI3Ig0+qIzMpcj8JG4duP+o5mLlzpqThndC+m3YdzPvrafxba4PH5w3y4mxhMOjbGyi2ZshuaHODcMuHPiQggrVhgfzjdVpcmVFZw2XIa2sKsj3P0lLvsWMbZsurZANuNV/eRRfxfvFurAriyOxZfSF9h7R/kHBho5iiOLZ1FhT/AAn5uZGDY2RzZyCqF8ibx18C7+W4ZPJx7/2eRm4pl9uv5wFy52UPjONCLANbSfiLxPi8knOhY/i3Diz7H+sBsn4MgYsR0Ddj/Iw7Q1xsE853G2622Cfk1LUL5bZMS7wPxjqQPcjtBbc2E5XDO7Gi54A+B7yKceFN2PK7ZWBUhARt+p7xSZ3yra2yI4B2gUCOxmk492jVyWKCluq/7/OI2elvKcMNtBgTZB7bfeWDlXTo37jMRSmmP1ELfpSfasqjA/l5MdNV9RzJIMeA2czjeT/DuuSPtF60pO9/lKL1Fiz0aq95TNRN8kTrpy2vI4LCASLEK8JwGrGQHv0MAKC1ySE9ukosQaua8HhmbLhOfIwTHde5M24/DU0xZsirlKiwzfhv6Tnl5cZxtuYZVyhjdit/vcAHvLyLiVnQlvMQElVmg6nAdWuo1JwKuJSPKXqT/qYjN4niYMMeiTGjnlu/0HtD2yt4h9ZO2zTeJaTSadExo7ZnBscDb/WYyjHz8wzBCLLqfb5PeYXys+T9mEBNVQ7wM4fHn2jKXbqxHvKePV2rlw0YdTj0+RcmNfOYGm3Cgb9u8Wc2RWZ1c4yxNhTE4SVNqRYN895eY7nsn1d509Ztn2ulbiyhdzbV5A7CNRWKeYE9N1u+YsAegIdzEciunxNj6cYMRYuQQBY+ZXgQjdQq6PX85aO4cGwCekNsWFdOSC7vXWqUGBj2gWAfzl2T8+TfiTGqAV1Yd4JV8bEEU202BzxIMhLLze3pNIbTthZ8gPmgVXQH5mej2Rpdhdd7AL1IAsn4m3VZVzJtGVq/gEzLjbDtdsAJIJHJo+0AF2zqMrHceP8ApCzd2pwauNsaqVQBd17mXlT8jvCzAspZdQcjM3JKEVL2YmdvPy5cpVKRFPJP+ggKcaKFO7d+IUb/AFJ7w+SUx3FE2s2S6FEnd7cS/KGHMVy5CXUWBXf5mnUa79hiwYQoVbIyV6+e19pnyWMirmOQbODRDUD7RltV4IytuYkWATYUm6jMO9SuQr+D4gFN2UriLueoG3kxlMNihbdl3Xu6j2mr1oTtb6jIBuQmiPUSOBLXOqofSS5N2DIHYVi2qu4dx0gnKjsd7KpHdVu5mf4aUMmRxRY0OQDzNRC6bMFGUZgRycZNczIzIGJS6I9jNGHIroSyb/LBLbnAse3vc1REdtmQhTW47jt5FSO25zuezQon+UvNiIxpmGLYrDg7r3RVqV4BuufmukIlrYzAYSQxHvZuWuIhSchIojapI5J977QMO9XTKpprNEdRUJkFmzyetzQM3ttbaxSz60A9IjDnbJiQJiCPj5LYxXA6X8j3+ZndBjwVSFnP4keyB7V0lYs7KNoZqI2kAdRM6+Tsf4mL/is1zzcPc3m+Y1UB0I6ge8gdkayu2r529jDYp5K+hgaqzdE32/KSXkwg4GzHLhJBA2h/Ufyijj3v+zW1rdSGyB8/MoY94YIpYAD1r0B+Zs0+ubQ4lHmY8mPKrBgg9adgCe9dambbOuTJPlmUUoKNtOMklg21uTX/AHU2ZNH5YxZMuaxlFnIpuvqOtfIicOPHjz5F1WJsvFgLz+dxGPG2XMox7Wvk23FX+97QvN4pjeBpEx5MWbVY2qtjDkHjp/KYtM2VXKYwvC8B13KojvJxJqPJ1DtjZfSF2bju6Ae35xmXG2PTHGdBkZwSEyMdu3kdu/MPb4vOzr6JV8+fC4feSBxt9IHPSvyiTmXGA+Io56MOb/Wbcuqz4cQCouIuoXIqgm+4P1+YqtPhyquuV3XIAfMPBUc88dRLHL+KxWmOM6Z8rFiVAsduTNAwY87U2ZNqjdwedp9q7/E59vksj8NjdtFD4v8ASahgfFgD5UPklgWUcRyl+xKYBuzt5inhdrFPSL+n/wBd5WpwqiY2OYbgoKBB0HvctgMupO3IfKcW2726811lhFy4x5WTeEqge31metNds4XGMePkhurkEgH2uOz43xjE2JtzOu7IoAKg+99+IzOSmEgpSiyHQXz7GCuCnXe1I1Bfb6Gpe2+RrQFOMovmbd1dB2kmjJ9yVtvqG3jgAiSG/wDWtOOWkAZ/wgmbcOhXHjGbWt5aEWF7mXmKOAcQ2YR0VR1noucjhMbStPo9+VVykgH+EXN6YNMilFG6je+6uJx4Tkb7yzttBpQCLPxMOfIjallyHyq5I6czjblndSuskxjpt4hp8GVVeioPRff3g67U6zN5raMo+AIGbgblB6mcHOUOW8ZLCuTfWHifLgxOuLUlUyJWTjrfaM8GM5V8l6PwajTqP2qozjhi1n8/rM+VvPII2qlgbqpQYBGFFry33fPErAyKpTNvOI80nW511rpz2bkxpiwFt4yc7UK8AnuZnbkCr3e8q+AosAmWFZeTGTQtOxLh8lvMfYR/w2T+URW9qRSR/nUYUYC3Wh157whmyBBjVht60oAI/OSKTeGFEix26zq6YplxtSbSBy13OehVXUi6+TZqNw5xgyOcSEhhQ3doZTZl0dmUopxLe0NuUmTFgZiCuInHW4c3X1lIwbIA62fjrX0jMzABlQMoobRVXMkCDH5gOZX29q44mojTnUbNoXjoOee0ym0wXv4c0VIkGMsgZAVA4IuyPmGk1as5HwgnUWnRtp/0ggoisNOl9yxBJIiEZAPK37RdAmP02UYsYcsx3WCOwqFnBlJTUsNQrqvqW/pUj5sOTMWVCEF1uPX5JhNlZf2qYAUIok9D8GZ8jNmYu5A9wFoD4AjIGpMmJcRxYcZyZH4Z+9ewilxafyXytqAvZcai2/P4jVw+WMbAXkLX1IYDsK+YGZtO671wHHkJHCm1P+sJ/Df6o5EVFZUKUOSB0v57ysbZc2TGMKbeiglbr6ysiKuRgzBQrBuDus/lGZXz5UXdWPG1MW3mq+n+kiHzM2VgjYy3l3wB0MXixOXAQKSAH6fEsYswYnYwo+kgmx7GNLI+oO7UNkaqLlKNgdP+seuh/pRxvk35dxYAAMelX0HzK3higZVKjpt4/wA41Dk9K41Kkgk0eoEX68rKhDbcQJYgdB7x2BpjQ6dn1GZlUenEBzXPt7QG8tQuFSuVV9ZyonqBrpZ7S8rh8wZQ20jaL6kRePIx348O7GGXaQv7/wAH4hJe0fg0rZ8LZNyIMSlmtvVX0l5MjDT+U+FN6kXuU7q+sp8L4NHWV0HmXSkWRR94rEmXUZPTeQ/vC+TKXfNvBv0iYxlZ9oAQD8TkDb8x3nrgYZdIqjKF5cGwDVen2lfdWzqDuTduoqGF8DrC1OLS43RdNlVweDQIr5N+/MrZbpasheN9j4sjlM1+pls/oY3JqNRlTyQaxs9jCppQT7CHizabDl3Jp/PAs8ngLXSohVzYUx6oqSmSwrMOIcW9Lox1zaZG0zbVZuWAb44uBl02dchOTEBkLKL7WeRXaUMZXIi42R9wBq+Oe31l6dMeTI5zFuOOFsA/WPXK7HlZ21rerzMpNNsXgn4EWyKMZ4/aMCpEPO37QLhyMwxfhcjaa+nvDxo+pytsDZXAvddEAdYdRdg1GDJgdM2dly8KRbnn49+Jo175G06IuXM3l+trawpPMHy8b5UV22ptL8+omu0ja58pxhwKUiwqBQB8ATPNs/jRWMvp3Qt+0FennoD7XL805MSYkUs5PpUAUfy7GasiY8qs+PCRsveWFxRx0RjxvibIMe7cXIo/H0HaUynfyrKyq5xbsbs208ZEqv8AP4j6yvjKvmagNqrVlgDBxaTCMbvqNQm4Cyq83+cvC2PzD5bbBVqT0B/6xtl6ElnZmXKgITBauhUI68XXc/MLA7DUO2l3NlYXQAse5rpBVQ2JixfHsPLAX17R2pHlOuXDm24srBkQDlR7zPE4a/puNMrYkV3HFWtcN7/mIX3fDgyHJlDNkDGmJpGI/wA5m1yszLlOUZVbm0BAMaubKf8AzXJOIgKpHB45H1mLLrbW4NMb4V2/eUFktQ2nr9RJEajGxzMdiAE2Bd8fWSPrbztbf//Z</t>
+  </si>
+  <si>
+    <t>Productiva</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2025-11-11 08:47:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D101 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mili </t>
+  </si>
+  <si>
+    <t>/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDABALDA4MChAODQ4SERATGCgaGBYWGDEjJR0oOjM9PDkzODdASFxOQERXRTc4UG1RV19iZ2hnPk1xeXBkeFxlZ2P/2wBDARESEhgVGC8aGi9jQjhCY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2P/wAARCAHgAWgDASIAAhEBAxEB/8QAGwAAAgMBAQEAAAAAAAAAAAAAAwQAAgUBBgf/xABBEAACAQMDAgQEBAYBBAEDAwUBAgMABBESITFBUQUTImEycYGRFKGxwQYjQtHh8FIVM2LxQwcWJCVTcjRjc5LC/8QAGQEBAQEBAQEAAAAAAAAAAAAAAQACAwQF/8QAJhEBAQACAgICAgIDAQEAAAAAAAECESExAxJBUSJhEzJCcYEEof/aAAwDAQACEQMRAD8A9NyKqRUBrua6uauK5irGuVJXFdrtSooKstVFEUVJdBRdG1UQYOaYVgRvUg1BrhFMqoxmgycmhBGoDVsVwjBqQiGiAZNB6VdGINSFKVQij5ytDYgVkhEVWrk1SlOGq101zNSdFdzVM1M0pYmq5rhNczUltVd1UImpqqQuqu6qFqqaqELqruqg6qmqpDB6ur0sGqwaomdddD0vqqa6kY8yrCWlNddD1I6JBirhgaRD0RJMUaRuuE4oYl2qrSZo0li1dU0EtV4zvSh6lQGpWSxtNQqa7BKs5ygyO9MeXjmurBQg1zFMMg6UMpUA67iukV2pK0RTVcVBUTMeDRtA05pRGINMRsTQlo5MbGqSfFmuyLg5rnNSTOkZobNk0Qnagud6Ums1ZXodQVI5HLtvXGbNLg+9QypqxqGe2aEKa5muas1DUkNVrua4ak5UzXDXM1FY1U1CaqTUlSa5muNVagvqqaqpmuaqiJqqaqFmpmpDBq7qoOamqhD6qmqg6q6GqQmqpqqhNV1VIcPVg9L6q6GqRtXruql1era6kOGqwODS4eiB6kOJCKlB1VKkxvB/ELOGBfXuelbiSxzj0g15u4/h+a0mSS39QHStjwudlzHOhVvlWZTo00eDVSu1OMgIyKA6EVuUFGXeq6aZKE1wR5pAIG1cIpnyCBmhlKkGvNMIh6UEgRjUxAA6ms65/irw+0JVXMrD/gMj70VNzSSMGh6MGvNr/HFsThreQD2Irb8N8YsvE1HkSAv1Q7GjZ0M4IoLU5IpIpdkpAJYKN6yPFvH4bJTHEPMn7dF+dW/iDxFbO0ZEbMzjSig7/OvFyZI3bU3VieTVsyNFvGb64YmScqvZdqV/GSFyTnbrmhQWtzONUcbMucZ96c/6Tcx4OA2eQOlZtjUjY8E8cKyrBcSFlJADH+mvVV4B/B7uIl9IdefQckfSvXeBXT3Xh48w5eM6Ce9UuxYfzXK6aqaQhrlSpmpIao1dLVRjSlSaoTXWNUJqCaqmqqk1zNSWzU1VTNTNSE1VM1QV0UFfNdBqgqwqK2alSrBSak5VlU0WOEk05Fbbb1AiFNTBFaLQKBQHi7VbRYVbNW8s1NNSRTUroWpQVLK4lkIwQU961PLQ7lRmvK+AXyQExyuAM7Zr0q3sDEBZAc1kjnjaqMmqrggjIqVLQegBcVxUFFqYp2NKkZGKXZN6aIqmnFUq08Z/Gt3LGYbZCVRlLNjrXiZGI719I/i/w03fhnmxLmWE6hjqOor5xItaQWrPWmLW6kt5VkjcqynII6Upg6sAZz2ruog4ORSn1D+H/G08TtQJGHnqPWO/vU8d8Zh8OgKoVe4b4Uzx7mvmkV1JA2qN2Ru6nBq6zy3EwLuWZuSTk1DR6WWS5leaRi7seaJ4ZDDNfpHONSt01Y3pcthtHAGwriyNBMkkezKciil7PykjjVIwFVdgO1SJcZViMnjeqQzx3tskkbA5G47GiLHoRSe2K4V0XdgiFsjCjOSaxPC/F5bWUjC+VJJl/b3FM+OXgt7Lyw2Hl2x1xXn7VxrAPHWumE42zk+kIQ8YZSCCMgjrXDXnv4e8S0Sfg5m9Jz5ZJ69q9BIQK2wqTXM1keJfxBa2TFMmSQf0r0rOj/i6Mt67dgPZqU9MaoTSll4ra36/yZAW6qdiKZNQVJqpq1cxUlSK5ir4qwQmpBYqYo3kntRI7dmPFSLhTVgtPizIHFV/DnPFBKBKusZp0WxxnFWWDfiolBFR4Yd+KaFvtREiC0bTkcQFFAqV2slUjNU8sUSpUg/KXFUeAdKPUq2NFVh3qUyalO0+URyHIOTmvWfw9OsmFeMkjrXjFbSwyNq3fC/GDZzAKuVNc52n0FCCoxXaSsLx7lQWjwDTtbKVK7UqTlSpUqSjIGUg8Gvn/wDFX8PPZytdWyFoGOWAHwH+1fQ6rJGsiMjAEEYINO0+SeFWE0t2kmhljwfWRtxilvGYZYb3Eu5KjB9q9xJ4ZJ4ZCtu51x5JVgNsE8fPesrxGxjvECSDDAkKw5B/tXm/ls8m706esuPDxhOaZtSFJbrwK9Jb/wAHyMxhmYCQkYYbjFZ/j3gk3gk8cbSK6SjUuBivXtyI6tR96u3ANKq+X+lHLekVI3Y3D2s6yoTsdxnkdq3bjx+HyC0aMXzgKf1NebjYac5qE52BoslW9LXFzJcyNLM2pzyTVY20ttzVG2qRuAc5pQ93M8RilUke/vTM/wDE99NaiIuE2wWUbmkLubVakY4INZ+ramQUZpS2STkmh6zmqasVBk0o1bzvFIrxsVYHIIr3/gl7/wBSshI3/cX0v86+dptivoH8KRRweFjUQJZDqYdR2oTTK4rmmjMM1ULUFFTJpmKLPSpHFk09FFpFFpCSDuKYSNV6UTG1Ss2nSYrmgdq7UoKYqYFSpUkqVKlSSpUqVJKlSpUkqVDQ3fFSRmFSgFiTUrWg+YyiLzWER9HTNVEhRgAKEzjVkip5iathmuAe1/hjxGV18pyCBxXqwSRvXy7w+9e2uVdMjfivoNh4nDcxoC2HI4NblMaFSoCDwalaKVKlSpJUqVKk4yhhhgCPekbjwaznyfL0N3TatCpRZL2thLCikHG4GM14n/6hsGu7SP8A4oWP3/xXuq8R/wDUS2INrdDggxn9R+9MTwbel80xGc0tgscHrTEOwFdGR9A0jauaSOKIoyKhAJoQBbJINDZwrDf6VaY6W60OEKZl8zvuOwqQjkuoCuCrfEmNxSjrpJwCBWmsIUtgde9XEKgZIzmrZ0xwKKi6jpCknpitL8NAx3TB9qIEjiH8pQCRz1p2A7W0EREk2Cw4Xt860Yrp0bUrEH2NJgnGTV1brQXorHxwghZ9x3regmimUMjAg9q8FqOdqf8ADrp42ADEZpGnv4EGM0xXmLTxqWI4f1qPvWza+KW9yQqvhux2rFMPVKgOeK7QXKlSpUkqVKlSSpUrtScqVKlSSpVWbFQODUNo52oDAk0fINd0ilACPapTGKlW1p8UV31kHeiq66htVtJJ2IrpRUGTvXPcA0cuhga3fDPFY4ctMhJ6EV56NgZV7Z4p2aREYMg+lE4L11v45LLOsccLANwSK9BC8gQGXAr5ufHXWSJolwUrZh/iGe+eKEDSc7mt7T2oOa7StvMPLUFhnFMg0lKlSpUkNTIqUGQYOQaohq83/HiBvAQeqyr+9egRjjesH+Ocf/b7f/5FpD5j/VijRjjFUQanNHjU1oLpjirtxmuKNxirsBgVIqy+vUeAKH5IJVhsSd6PINSE9c1WPdwp6kVIxGMKATxRQMpVDzmrIelDSg6iodwKjbE/Kqqe9IEO8VSM5XFcXdCKmBGy6WyGFSXBpq1Pq9+lKNxkUSF9DA1JpF99QPNGjl433pNm0kH+lvyqwORUnp/C/GdBEVwfT0Y9K9AkiyKGUgg9RXztZMDKnI7GnrPxWW23jcgf8TuKLE9xUrCtf4ijkAEqFT3G9a0F5DcDMcgP1rOiPUqZzUqSVK4WxXNVSWqrtirZzVHXIqALNVdRFRtq4K2BEk33owcUtXN87UaJvUKlK6mHNSjSfIiSpxwaNuwAoWM4Oc0SNt65BYJv6tqctLdLkMA+CBSkp1qoxjHJpr8MsarNDJjbemT5Qlt4PLKsjBwCvSmU8PaztxcyHBHQUtZ3MpnUK+nUdzWtd2UtzBgXGT2pllK3gniDPPqeY87BjXtUmUopLDcV85gt9NwAYySnOK1ra9labUxYRpwtMT2gOa7Snh1x+IgDYI+dNE4FJQnFDJGc1xmqhatSAXV2rzn8cv8A/oO//wC6v71u5rD/AIyQSfw/ITn0OrbfPH71aD51AOT7UdTkb9aBGSJCMc0xjGBnpvSlmIDZAoxUtHnFAOcjrTS5EION87iok3OEx9arCu5fjFXlK6wp4PJqmCowTvUjOciqMxGKrHJkb9Kj8YqTrvkH5VxGoB4q8ZwPrUB0PNVbZhVQ2CflVWbJHsaUazV14qiHIBq44oJkHXFp6jipDJvg0uWKAGoZPUCOtSMyEo2ocHmoX04YbqeaqHDLg9aqp0kqeKkYR8bg7d+1GW5kQghir9weaQDtE+n+k0bXtuMqak2bP+Jbi2YLcfzI+/UV6ey8Utb1AYZVJ7da+fNpJweTx70lJJLZyiSJmUZ5B4q0n1g4Nc014rwj+LWVlju/UvGrqK9jDdwzRh43VgeoNGgKGwcGr5BpcyAnmornNGiKyBqoYsUQPXSdqkWxvVgKjGq6q0Ec1KGzb1KU+ViJUOc1cIrb8VxXDLvzQ/PI9OmvJzUNgAYzXGyFxnahkNgZ2NDcsTgNWtVDidUHvTNtftnZm+9ZwGoYPSnY9DKAq6T3p1E2bidlt45IsCVtjRbBpXl9aZJ69Kx9baACxyvFbnhF5BNGsTHTJWi9jZYECjYUc4xWdaWzREP5hK9qaaQk1uRLlNs0Bjg0UMSuKE6ntWoFdVI+ORG48Fu4xuTGSPpvTmDS/iTmPwy5YbYjO56VJ83kQIcDbB5qozkb/eiyRSzxmWKImPOkMN/vS7QThSRlfapCMG6bimLd8jBHsRWci3G+rpTEJI9TsQAakclt1EDuV9SDJFIzYyMAAY2rTyAwGcpKpwRWVcbqD74FRCVipNXVjjuBVUGTXdJUmoOSEEAiuodjVTuKg2pS6sSSPapnDiuId+K6Rkg1A5Ccgdqu+zfOgQZGxq7vk47daCMRqjpdiR9KZhbKkUtMNLGoixvld6IWyAeopNGoqMDkd6QZb1x56ipE+RoP0oMT6HwTtUY6H9ulSMgal0n4hxVXCyRnUMg7N/eqmTZXBrpcLKCfhcb1Flyo0EpX7Gm4L+WNdKyMvyNXvoQ0eocr+lZ2CtCb1j4/dW0oJlLrndWOa954beQ31os0Z2PI7Gvkysc17X+DJybaWPPBzUHrwwqwdaT1GoHNGlsw5HSgsamokUNjStrL71KoDUpD5WhCjGaE0jBh7VCCxq4UAZNcOihmaRt6IqZGetDXY8VG1DcVVH7W1SU6XOD3q1zDHAcwtqUc70C3Z33OQR1qrMytpJ9JNUTTsYYLuNi0hDAbYpeNGtLoO2rQp5oEErRS4QgCvV2SWs/hoeTBI5rUiN+E+Li9lEerSq9+tejVVAzXkba2gtZBcwqCp6V6KG9SWIEHFbkq3DZKqao7g8UAuMZztXPMQDdhWtDYuxNYX8Y3Bt/BWRdvOcIflyf0rbV1bgivOfx3v4TCRvib9jUng/xM1vICjkJnOAa0R4ir7sm5G+9Jp5DwkSAhvbrSxOG22rLTUF7GGDFfpVZPGwqSQxW0ZZhgOV3X5VnJgyrqO2d60ZPDFhjEyzo6EE5XnH96kv4fIXHltg43HtSlxny1J5BNEsXC3W3wkHml5G1K+OhP60hLdiwOw2qxOc96Wgk0Nv1opPWkLVwkDeubmhMSPlUhFk9VMBlxWeW3xUEhHWkbbMLKRiqMMEgnrSEUxB5pt5Ne9DRmFsGl7psOatFJ3oV0cjJqQaPREkw4pVWq5JGDUDrkYDVd8SRBgdxzSxfMVWglGQvQ7GoiRsdLKeMUaFvNhZD8S7ilUbTKQaurGKYHpQjfxwEHcgYNZ8gxT0L4mZTwwoE8RBO1RJ43rY8EvHs5CUbAbY1maKNDlQaqntrTxYs2mXBzwRTwvEJrxUE+dO+44r0dlquIQ3Xg1m5aFn01Pxi9KGbwE8UuIgvxHNTUgOwrHv8AS9au905OFFSh6/apR70+r578q7kaTVQ4HSqucjarQRZehogcj3FCSPJpy0tJJyQq5xReEPbq0iEKtBkibVgjOK0IPD7iLGM4PIpkWGCxbtWJnINsUxkjKjem7a8eFNGDg0QRFCexqoUDZsGt+xPpdMQBq27Vo2IaT/5CPasvw9I8ksR8q1EZUbKjFV8upwzY0PKkK4EhoLQTA6dZrguffFFNwSmx3rM81PAMckkcmhpcGmJ7f8VbvBcASRONwawrmKcyl9856VpWM8zw4c4IrpfJxvammY/8H2pfEd3MoI/qAO9Y0/8ADXiUUrKtv5gB2ZHGD98V7dSSclhmg3Ms0YLqMir3lLwVz4Ve2mDNazKO4UH9DTnh/gniN+PQPKTGxm9Ofl1rfkvPOk9e1WiuWguVZW2961yNvJeKW0/g141tJpMmkEOvBB7UlDJgEHrW7/FatcOlyTkqdJ+Rrzm4OK3OZytjlByKKPhxQVJ0mosu2KUMtcZdRIFcB2yKsh9W9SKtkHeuUedRzQMUhdGIO1MI+RvSo5oitUjaPjrV5/VBq7GkhJg0yrCSFl7igwvqAqxkoIO9dPNSMI+QRXYzhqGnGRU681IzIcEGrMdSA0L4k96vE3Q1EzCxOlutOyIHTOKTgGnbGRTkL5Gg0Ek8ek7iooG1MzJkYPIpOQ6TiioQtp9Qr1XgpZrPI4Jryq4Yae9en8IfyvD0FYz6ax1vlouAu5O9UX1Nk0LWXNXAPSucjXtFjjO1SuAY3NStQXl88kBzha7DkEAjNemuPB7aVQY2AajWngcKqCxBNY/kjMm2daeGiRRLx7U34UvkX7AgYNaxstCYXismdWtvEUBOM8Vne29ab5RWG4xQ2t1biopPlgk1wMR1rno3GVm33hbhC0VKNYGGESSbtXoNZI3NAu7dZ49OrFalvTNw+mNawrL6l2IrQB0jFFtLaG36Zz1phoIpN1ODRaxcaQJPeurIR1o8lo443oJhdeVNO4zRElPWjK/alArDoasjlW3o1vpaNiXvUlYvGVBwDQ8gjiuijWlyUNgM5DU5BAmjEigkVRlPSuZYVr2yvyy7eWFtdWssTx/EpHyNfOAulyj8qcV9H8xh1rwni8Bt/GJVOwZ9Y+Rrt4crzK1vbmkBdhSTelzTpB04NJSDLE16IjELZFFUDOKTRitWEzA5pRl0yuM0ruDimEuAxyRg9aDMBqJQ5HahOKN6uqnVVEfJplCNqQXkQqdxV7dznFMuUZcMKWVQkgIO1BcK+o1x+a6x9RqpqCyNtirnegcHaiocioixtjrRVOD86AuxowYVE1C474pqNgw9xWcrCjxS4I3oJ5vWuetZ92NG9Oo+aDe2xk8NkuQfgkC4+dZt0SkEmqQAV7S1iIto17CvE2KE3C6gRv1r38I0xLntWPJfpR1EwKjOqHvVJJei0EnesSEd3yNqlAB3qVvS2y549LBkfGTR4nnjHx5rklsX4NcMMqnOdq8e2Yciu3K4c70neSLJcI7EZWuiKUkaMYNZF94deGYvrJ9hW8cpvs3J6uFhLEpBGPnXGXJ+ID5mvJQC/iA0SPsdhnam7XxIxTufEFc9sZxXSYy9VqZvQ6G0kqQwHaq6tQovg13BcQMwiKAnbNXMQDNoxjNWeMnRmWy6hl25FdAYNkcVeE+YW9jRGTfNYrSiynODQZr8IxUrmiyR7ZFI3KkAnrRJGLFvxuWzoGKPEyOclKyo1YsRq3rRsMBtLNvTljNcMaMlExttQCHU87U8YRyd6q0QrnPaL0pZck7moC+rBXIo5iA6V0IMZzii2/TPrQ2jwfhryv8AF0Oi5tpsYDKVzivWs5jGSaT8TtIvFfDWjkOls5U4+E966+K2ZbWngpXyilTQB1zV2DR+ZE3KHBoecivdA7tULDtVQOprhpKwY52G9RlYbmqg4q6sd6kopwcijo+cUA7NXQTUqcLAr2NC04PNUUliPanJrQiwScZOon6Cs26U5KHk1U1AcipzSHDzXQ+K5ipilCayeKIj5FBA2qyNg4FZphgHbNEjONjS+s4AFFXpU0fiYYwTvWx4IgltZQyhlMgO9YaY0Fuwr1Pg1uYrSHIxqGsj51x8t1G8OyXj0ccU1toVQx5wK01lLxge1Yvj2V8VQMcjAxWjETgEdqzP6wZXkfODvXc5qqAsPUaqzeWcVrY2vipXNYqU7Qsax4IK/LFTAwQRVFONx+tcmDliw696+bN3lh30sRp6UMq5LHY70JmKyNjPpx9aIGOjJ232rGrsLGPDHK4FVkgikdQyg99qL5wwSfkKL6WTVsB3rUysvClccIiARLge1A8yVNgCRTY09xXGdVGSBg1v3rXtSqTvG2ApGaZF0wXdcmhGVS5XpRBpbcCr+Re1CkvznAjIockiSDcb035IfYbg0pNGY2yIyRRLlaLbQ/w6Phs4NGjjWPB1ZxWf/wBVt4bho7hwnbAJokfjFg8ujzMdiRzXTXlnwOWwl0AAG3on4iJqQQpLhopFZfY1dwUUk/auXvlvTXvkbM0ZOkEZpa5jdiPLfGKyVjmmucszKehrRitXWMZlLN3rrlbjNym262N5YOPNfJHSunSFJLKqDqelIXfiFtZsVnm/mAbJg5NYdz4jNdN62KJ/Si71rx4eTyfqM7tCvvDYJvEppBcHynbI0Lv+dWh8MsAukpK7d9XX5Ubw5Iri6SOcuEbb07kn969BJ/CrqM285UHcLJgkn717/wCs0ZHkbnw6BAWAA29IDYz04P19q5F4fbXWAskkb/8AEqDWn/0a6aSaNjJJIpG+Dpznfei3Pgk/4MOY3WeLGVB+IHqMe+dqtnRL/wC3oFhLrcNNt/T6cH5GkW8PjWPS0brIP687H6V6DwnxAWt5GZIlfTsy4+nXrXqJ/EfDp7XE8KNDLtpIXf2xXPLc7q3HyaeB4HAfrwe9DFb38SeE/gmMtvIzWhb0K4wyZ6VhV0wy9ptlZDvWuW8yyWIkgaRxWOvxAd629GFAA6Vjy3WmsWW1q6Ash1DsOaoF9BJyCO9aejTk0aIw7a4wzHriszy/Z9ZWCSetc1EVueMW0TRB4UII6AVgnIODXXHL2mxZpfWassmDuKHU+VaByM5wdsCjpwTQbaJ5NKopZj0Ar1fgf8NFnWW+4G4j/vWMspDJsh4XarPJGJwREfzr1uVWDK7BNhSviEKx3mhQACAQKMsTGIqeu9eTPK2u2M0w/GLdp7i2lA5ODWhaRkv8qYZVhibzFzvtXIXjByu1Yy8mppy8nFH8v2FVa3RtyKsGB/qq4/8A5VymdcirWeG1KalN422apW55co1usaOVnibSp1rsdqIbhk0qd2/aitHpJEWlcjfbcnpQkiYwhFO+Mam7mjck4O3GvlaQKEUEnbOxNEyJdycAdDQYoT5smoA6ThW77ftVghDKFZQFGGJ61mzY0O0QIGjel2MxGwOM/ejAyogYKQp6jrV2n8x1GBtjpRqLQSO6LlhVsll9eQcZ46VZcFmz1JwDxVy5LHUBnGBisaRVQC5DHkc0xFhfST8qow1EMBgAVxZdvgOc7E0yfQPKwXYUC6ll8qVo1LNoOkDvihC40Ak81BNqBGeRimdp8+mM4nbzAwfO496vG8ztqCnbrvTfjCLBfSKo+VJIxfY6sV9XG7m2mhZ+IPG+lyT862U8SYL6JGBA75H515koV657UWKcYAb8jTqVPTR+KlWVpUDe67GtD/qtpHEXBc9dOnevIpc+kgZzxzVZrkspVWyK5Zf+fDLsDXd1+PvHnOoDJChmyB8u1BDHJSNRtyScD71e1gkncaEZ0UbgcZo8lu74RUQDrj967Samok8Pk8m8jle5EYU5LIMla93ZeLeHvCJhd6yerHB+g6fSvn4tUUhdZORz71xrTSoYHLCq47Mr217/ABLbW7+XBup5PY+4/cVk+J+PvPCPwpTcgMZFyR7jpXn1UnYknHGelHXCrhVzv/aiYw7XhulaXXcwFSf/AJIxj7iuXlstwySlm0odyBg6f7+9GjZCDrGz7ZHSnLS0QfESVOQUXn5imwFv4i0TeERSRS61Rl+o3FeWAJNelvbLy4HsSfLMjiQMw5A4/Wsk2CxsfMmUY7DesePH0mhovawmS8hjUZZmGBW1MkqOdaFfptWdFLHazrLBqMqHKuTwflR5vELy4A824cgcapNh9KM8LlTLoYqWHwkj5VEOhlAUZpFri5ztKG7erNETxGcDEuG9mGazfF+2pkbmlkdtQbHtSreHLPmQ+k/+PWot7CzeuPGeqHj6U2hPl64XBT36Vi45YdHcrLl8NYEaGGPejWvhWWBlcY7LRpvMkIyeOK7HM0TDUpxTM8rFqPR+F20FuqCNADjc9a9BbkZBzXiYfEGbABK4re8LuSVLMxAA61zrcovisobxJVHIXenrZsgA9q89PcNN4m0uCEOyk9cVsWDliN6zS54lkuFHApMB16ZFPXPxs7D0k80uJo86Qw+tea5ZfThlzQxIflRBKTxViyavUBXGiDYKbUe0+YynnOOtSp5OetSqZ4geW0ImDIV05yPfbahayrMhUAHfJohuHVAAFyBgrnOd9v8AfeuS6EkVXxrQgMAOKvJ94tOHDDKEgMMLnfBxvmhpGMaycZGdhtRVEckjjYIDgY9+PzNddSAuXUKy4WMb/U1qpWQuBgA7jBUb4NUiyCplwDncGjGWONCGQPwDjn64rOncsxlhHoAzv88EVqNa2bfQh1Djpjc/WlHldpAgGQx3I6VIS2nMhyx6Hr0wKZjERVivK4+ntVrka1XY0kdiqL6V23H3NE2iRc7sw2q8UxZimjRnc4bj2NVA9QZt9GRuPyqs+jwFcxgKMb9eKokZ3bAB7UZpPUoO4xuc89a7pRjlDkEZGaxayzfG/D/xdmxSEFk4ON/lXjdRiYruG4xjivoqqQARuD7157+IfCyQtxCozpJc5r0+Dy/40vNjzc5z6exqjHqKIN1J7UB99hXugqCUhqYtlUg6s7tQVt3MZfSdI64pm1Clk1ZxnvVtNcTCKIIDgDBUDpQ2nLfXmk7i4WR8DII2we1cjf0nO56UoQyAHPb9KMr5JX2zWc0mD7+9XimULhvkd6kfdQrBweaqHGo9l3oSS+YgUHPO9U8wE44J23qRsPiPGedyPfmtCGUiIaXwcnH2rGMgBIyTjbP0poShYEbONsb1JpXskV94eWf/ALtudYPcf1D968fNMWlYjO5rciutE6f/ANw4xzkVi3AVbiQKAEDELt0qIYd+5rhz1J+9WxkbAfnUAYdAaiik52YiiCOR9tX2qgIfoAftV1RuQdvehOeWRzTvhrss4TOzDcZpbfjbbtXoP4e8PDy/iJVGjTsOc1jyZTHHdHTQ8E8DivfDXuHkPnamCjoMVlvGY2dWUll6V6m0hS0j8u3GlTvgVleKQhb4Ooxq3rxTyY53huZSstY3QpmLTrGoe3zrasUS4s2UNgE4Dd6vbWEj3JlJHl6RsaMSsPowFUcAUeXP1nBzupwU8SBj8hBjSgxmnvCRqYEikL63288MTk4wTxWr4VHpQE9qsb7TZxu3mvGL24gv5baOUlQ2QOaXsbx47oPcxsVHtWzL4esXiU0zrqLHYmhz2/mEHAIz2rt/NjJpzt5ZPiHizSXh8oFEGwFej8OkmTw4F8O5pH/p1pLLreP1D2qp8SNncGN1zGBtRfJPJNYxSxtLtbtK68dKlCtJ4r0iOCYZxkipXnnhmucR/wAVh0oH8xvUGO42G3WjNC6+Tndzg57HnB+lCQFSA6Y65G4PvXbi48i1Df1ytpQHkdz/AL71z7hvEXEgiT+XkpnGV2JPWuxgy+Y5LeYMYIOMZ2z7mqWul2wfSzfcjn+21HiZXDRjS5f4mIwCemccD361TnmiKS+WJQAyqRgYxzj36mgmNGJDknbZenOR+lEKIsZYOobIBYjj5f2pdGkySXDIuQCT8XzrVoGK5GGOdtyNuudvyqifCEVQAd9QHvz9KurJJlCq7AfC55+Vcj0BiqyLsNsH86eVsZUBUBSdm3GOd+TXZItcbiMhW1ZY4ztxQY/OjX17lm2YHNHUFZP5TZzvgbnNax57a7RU3wUCjY46nvkUuQ4QhgFHXpTMsjqf5uEJBGkHcdtqWkuImXUCWJyDjqfrWcpqh3SojHOFG4z0NVkVpFGuPIYYUN8JxVlREYtMRp2bB2zkbD8q6btderOsvkaccY7VYz5pknywPEfBo5nVowqDkhOo9hUtfAYBKDNttlUH71uMiFN8R8sWUjb3IrG8Q8VW2VhDiR1GTLvv9DXqxueU1EU8eubaBFs7dQWxkkdPasNNpFXVsKD5jyTl3JLHfNWjB17nevThhMZpl2ZhqUrzwar+IdTvyKhlwxDKDg1TBkb51pDBxJpPGewoqgqSTqIO2kgHNAtwVYgrx17U0mSwIztmlKQq0bt0HQUQnU24Ykcb8CriPB64O9EKEqN9XvUi+k9m+p2oc8zMEjG54Ip0RaTkdeKFLbsmqRdmJxnHFRctoJ2fbHpxz3xQvEbaSO5OV0uRlh79a0/BgJb6NwuZBnUPkOTWvfWa3k6PjJKhSR1FcMvJ65aMnOniVDqRscHce9FXJBFe28W8BVmiuGCxx6dCRIOMDbJrCl8DmEzLAupRT/LjvVV4YwjGc43oscbuQqg79K2rLwJ5mPnegjb5VtWfgsEIB06sDcEVnPz4zobYnh/gkkwLTKyge2+a9PbWyW0Cwj+nk1R45InUxnIAxjPFXyxY5PNeLyeTLO8s9i6VXcPSXiSa4w4wSpo4QZ9RyD0rrRRFG2JyKzjxZTO1/DrgPCQw3FS4t45WzmuWKL+FZlP2rkesDDVvyy8VvMrdjCBANhWhYN/+OcDfFDuESSEg8kVayUi1YZx71ePjFYXUTzEc5O5rpjQ/00KK1VJCQ5JJ4pvGk4I2rhrlzvIBSMYGkUKSzhlOHjBNEkj1SZzxV9apuc5rUukUh8Nit5jJCNDEY2qUwJg+w5qU/wAuU+VsJm/ELh29PLnPA5NIzzi5kZvSAvpUfUAY/wB60xcny4WQH1McMR0/3+9KxJ5SxLgEOMn55ok132bdnC3lB2xjA22xnJNWjd2J1nSRgqMc0tMGkk0K+dB1HI3OBgUVZdMbDPAzpwNscb06+kKkgCGTIJHG+AP81RZPLC6R6jknfnvS9u+jKlAPSQcDnPGfqBVyMICBqJPqPYfKsyfkBxNHIRpQhh6iMEY7Y/Kq+YVYYiQ6gSxOeN6jK0ZbWuNIDaB/ejrbKkYur9gsRACxqPi9gK6Y420rW8EkoDsFt44uX6fId6K83lxNHaqyZ77M565pa8nnnmWGMacDZQPSg/01XXpSUuSWAwcNxt3rfSRQszNJsp22zgc7UAJKceWCxL4bbfPBNWcqzFIQCEABU75zz867cXjwwPJoKqu5YkFj7VmbymmuVZ5Ft4H8+dSy4XGeAOBnvg1jXHi8YBMHmtINlOwA9/nWZ4jfy3EhGM54A6UqqaIi8hyxPToK9mHgk5rJt7ydz/Nmdi2xNI3MzPsRgFtvlXfNDA4GPTtQZDldRO5r0aKsQBkA+5oi/wDdNVtUyxYjgbV0N6yuk5PUUhScYlPvXYyMZ7VaZC0aSAE/0mqCNwM6aCbjkRhkjf8AWmECsBtis4K3fY9BWhBkoNQO/XFIHSMMRg7cGjLCo5+dWgCgn96ORuev7VIMxqPUOP0oMynTpzzuKaUelsY439xSszaWj22ztWWnPAW03M0hBAVcHHvW2lwwljk2Cnt86yfBI0dZY3LAyFhnFOyehUH9I3FeTL++zj29VffzfCxKu5Rg37VjeZvk53B+tafhUi3Fi8DHIZSuD0rDWVQmhviXYjGcb1y8mO7sZmlmUaQCNt8CiR3CkHUp3G2KRV9w6nJG3H60eNmL+teucds1zk1WDUcgDgg53we1caRWPTOaWVwD6um1c0E4ycZFWvhHEkVzjgjtRE06SBvmk4SPKHOTsveqwSsrYY5Gcn3o1SdsFMcbqOGrjo3H50JbgRpqUZ/QVZrhVy++MZwfet+T8pLGsuUVWwdRGBTMQC2JPc4pK1czaum24zTl0GHhZMe5BBFWMvpTOqCGK6mzkjgUSNw4wzHPako7hzpIBye9OIhZRJ1bfGNzXHGWzVYTKk+ncnrQ5i6yBVXPvVA+lyGYAg5xVhIJFJG2fes7nyHUVSc9euKlUEXlqzKfUx6nkVKP+IC4hZLdnJz5xIAwdl6ft96XRZY7JWZgJEOMHffAOKfu7iNgfOXEWdALMRk7Yx/f2oCrBPII3jkwX+JWB3xk8jevRqGK4c6y2GJlPJAx74rs0WVaQg4YKMY46mrmOCRVaMvCMeptIOD0zvtXXZRCkMkyEqAGLowzRrhaAtW1uy5bSWDAnvTLEjSQPgDEDPJx2rkUZBdtcLkEEKNiOwOaatLJVBkuVQhT/Rwx69d6Zj9LoWBYUtY5pgSmkaVPLHnPypS9knuZVlTSNK5yTsBnpn/TVL03Mtz5r6gmyoBwM1WSZlvdGA6BQNOcasZ5/Wt+3OoZ+15JdMGiMY1Dcg8HOcfTNAUmKzkYkkqRxvv/AL0qrwuNBByWY4J3OB1q8NysJZGj1qqq2ndTnvnoO/zrHzyFIl8t5JCzomQVJIBO2ax/GJDNc6QCIyNW53+ZrYu8KguZHYhujKA3y2rBuJGkn1Yzq59q9Xgx52ds6RlUkKMnihOWKAdT3px442UjGNzScmVOnIxxXrCkcZJyTnep5ethvgcUYbaVHGNzUAG7Y27mhIFVRgUswCz5JAFHU870CYZkqMMRNiLHO/FEx/L527GlI2O4zxTKEk4G1ScjwDxgCm4pFkGAuw6gUCOIFn1AHsetFiZpi8cCFioycdqEKsmk+kH7/vRfNb/ic/OmIPC5vw6SSlF1cL1q4tGBq5KsL6sFloVxGDgoQSCTjttWjB4eZlYROvmAZCNtq+VAuoHjZbedPKmK6h3HbNFiG8CKLahmwJFkJ+hptsH1kKNsb77ZrFtXaGHU4JQOc4234rb8h5LdJRIHjMe2k8Hr+nFePy42bqM2d2IAVUDdeedxS7qhuGl8tQWYk9KXZJIQC76kLaQQOMDfNEZNEWNerjn74rldq9OogVNYGQSVJ+n61G1RIMgHcE5GCB3osKmVERyWyNbEcnfHFFkUggMUZSNmz19quRJdEmbVLKrbkHbHOM7gUYOGKnO3Ge1UmXVIp3Da9tqKqL5auGVSx1Hg46GsS8jTmo4Ug+ljsaVlimNwERDgkHbn50U3OqYRspI1ZwpAz8ulWnYFXQBkbO2rkVv/AG1IookilAkyFwcr+9FRNmUkFTgA9813OWSPV8IALY5Hf9a76VzGpYlBntn6Vz38i9rW4WFN9yeT7U4boNbMpUBSuwxSCuASBtuf/VTX5MOGIYqdwPv+VaxyvUEoqgkoQMkdTxRtOqQvqxkd6Bq9alRqB23OwoltP6HBGQoOPYVThqKaI2IJbjvS5SWHoCmwHtTLv/L0qB6Rvtk0VULHWxODwO9Y1tkqCyam+JegqU0iI0jAqQNwv/jUrcx2tEvOeQcaEXIVdQ49/c1LcyGXzPKC4Rzo2O+nA+prslvaxx6G1zKcKdGw46mg/iEezvdhFDqCDOFG5yT+WKMMct2qBF5YVYzx6UycjJA9+KMrNIFEaqrnaJ/L1ae3P+9azHVpI1jQNNIpyVVtpATgge4rWtYDG7RRguzEaz04+Ff3NdPU5cHYFmbTHMynA1zSgAADoPnS17fLM0JRCLctoQadj9KevHWG2aM4K4/mNjk9gKx3KMvmKsk6A52xkEcda3qdKT5oMv4j8Qo1lo1ByyKBg9j7ZptpAzIjOWY7Y3PPvTUMQmaNmZSi5BZnwzAjjAFJqf5srhVXRgIS+dPTOe2TXPKb0culr25XXoHqRSFwWwPlxzQDIfxZkWP0AgmMnOfbHWl7hvJUxSxqzk5DMpLA/IHFCmkkaBnWIu5wdW+UPfamzrY+DF3dG8W6jZmJHryfbmsvUoU4J3/SjQuJJWEpVG0MMhskjGN/71musqjDuV07YxXu8etagWmnjiOG59qzpZvMIAG46iryqXySTSxBB2roYdhPp1sOm2a60hY9cV21y0HktjWTmMHv2+v60Iyk9MY5HarYdZ8bb/KhsCwJAyRuaq5yR0qyy+WQV5G9SD1aZMtweabgfY55xVJYlZC0fwSDKj/iw5H60K3fLaD160bJ4MQox967NLJE63Vq+hgNLhdvmflVHcaDihW9y9rJ5iaTjOMjI+oqTQtfG5ShEpLv0YnNG/6vKSDtWM0geQuSFzvhVwBUEm1Z2Wy/i8wB0KM/8j0q3hsrXF61zeTaUICjX/UOpyeKz7O4aInGgqdysiBlPzBpi5nNwwJKIzAZVVwPp22pie68N8PtPEv4cFvthmc6xyrZ5/Sr+AeEC18MltrhSXMjBvpsMUr/AAhIRBPHqOAVYL8xz+VejwFcuOX6Vi/VMebvYvwUrIASCpyrb5A6+9LyNHL5iFlUg5APv/v5V6O8ggvo/LlJVhw6HBHyP7V4zxW2uYL020KF9Ocsp4zwT2rz5Yau4dGWkUiPy29O677tjP5miwvmPyyVZVBbfnH7UisgiBGNUmnCA8H3yPrQRcu0jNpAQHY6eR8/zrCl40cWTzA2NhsSe9cV4zhCcZJG/Y96VafILFmIGNQGxFEWJJo5JEf0iPJI2wQR/mueuWFbq4VDCpX1MS3cAZ9uOtP+kgyA4ZucnIPc0gyeZuG1MoBOo4AB6CmIpv5HludB6bHJz9PlWssdxuw1cRGJiAxxgKuoYztn9DQT5gYMWyw533xxRp7gNr0AERtpwxBGwxn261RBjDEgdd1BOfaueoxYgzhpM4YHc/2qaAvrJDZFSCRZThgDyWJ4x9a6UDS6kYfyukbb4qkXrUd1ld1hBVVXkk79KI7GJdUWpsgDAGa4piMWoysxY4w50/TipOFiGfWkW2WUawd+Mjin1q1V0OlGkYHf4i3A7cf7tVvMZw7sGWOPKtq4x/vSgiTERbWXUMGPp3XbqDxXT608pmOSSdWQTk9cGr11xRrQ5kxKQrALIMDPA+tSgeWzQ+WN8acNjcf3xtUqn7LKlu1fxBY2yIhvlf6dtjiizxGCBLEkNJL5kpIOc9FP2on/AE54bl31LcwEiNSgwUydwecY+3yrUjjVg7qozCAkb6cYzyAe22a6TWuGaQsLGSC3Eat/NfbfYxg9c961YolsYFGcylee3c0ESeW6gbk8k9BQbuSQMS2+VJMjkaQegxVtb2Bd+Zc2bKPWQ7M2DwCMD7EAfWsqwleK8tvLbSvqLA9QFz+lPrepBcJPreRgp9X9GDtgjt7URongYXFuoW1xkCNfWW/4E87n8q1GrN8xn23/AFV2W4KiOFnyWlITrnrvWj5CBWDT8eolV1A52HYddvffpQUspZ7exe7dmaMvNIH5LNwP8USUu9pGgwHdzI/seFH0GTTdWs7WZoEhaJdUiBtMZLDLd8bdKVnazMREmkBmOhCC7Pgc7kAc0tcNM8riFGCxHRGChO3f55/WpeRzMyJ5TYaLOVB9JO+PzFGvylLGd1hnLxlvLkXAB7A7j8q48omjy25Xt1HaiDwu8aBI2hbIlOWAzhTjeqzxLbpCgbLFCGZTscMRivXjZpASD040gUowIyccU5KrqgJRgG4yMZpOUkHfmuiV8wnnatCMp4kuPhvQNu04H/8A1+vzrOeMoiMf6s7dq4GK4KnBG+RyKz21oQ5OQRuO9Cya1UZfF120r4gBv0E/9m/WkZIRkqMo4OCj7EHtTsLWcnq8pjhXPpJ6MODVZ0NtORjG+QDVXDLBpYEFG4PuP8U1P/8AlW8R/wDmjbQ/96z87RMsQ3J33FXj1kYVc9tqtLMjsRCmhF+HuR7/AK0WFxGSHUkDqDxTtBLBN/8Attt7VZYpc/8Aaf7U0l2ApwX52OocfaiR3Sl/UWbGSdXFXCKAFWw6Ov0okcuWGxJ6ACr6w0vlxxeonHfHtTtgJ7e8jJi5IzleKi9T/B1rdRGa4uozEsqhY0POM816G6kYyxouTpGSP2oFq+uPOOBual9NHG0UiSDVq0sM/n+Yrhlk3Jo4UV1HA+leZ/iSML4mZHbVHJEvobgENv8ApXoI7+Aquc4YbHmsfx+xubrLWjB5THtF1IB30nuc8Vn2mU1KMpXmEkZsTN63d9h1P+N/yoczi3YsDpYjUN9quhzcpE+BIEClDsRnc7fX8qs1tJPNGxUo+rYAb4Ht/vWs3HXbCjI/lM8hC+rByfi7YH3qW0/lxvDGNihOjjO4NDv5CXMEbq+k746secUCGKYXsbFCAo1McbD5/OiY8LRzUyMs+RNbtsxz8B7HHv8AemmnaF1D5Dag0ugcb8UlGZbS4SSHcOdjjII7EdfrTBiE0LSwy4EkgH8w7ox7+x6Gmz6b2r+MkjuWcjfJ4GckmixXbkq5cqA4zvkb85pW4iktZI2YEashhxp+dFfRK6AHSMBgcYA6msWRjbSuLmIuoQFQrHSij0sO/uf70FJ2xpOAynUB29tuaBb3DzQTDSzYUGMBSDqzjI+YNVEc0aI0w8vV/wDHwx/xXO8HdavmGVHZRkod4yud+47VLSR47gkqFGPXjIwO9L2cqAlXwnmK2WQ7YzscfOuiR4p1icEN5owDsW3z/u9OrOVPtoSRqbgSQMYnU62CjZhjY/3qrFkhMkSYYLl0O+nffGenWo8scRjGnVyFJJA2JH5g4xQZlmhl1IWC6ypI59gRTlWrRFdXYhXDk5O2BvUpdXXBcMQxOoB9/bc/lUrGPHQD8Dh/DrJ5cmuTXplI3GrHwjvzvWs82hEQjSygMQO/QUnaRR2EKpEMKM792PJrkL+ZGJSMGRtQ/wD48CtblvDkPJGcq5kHpXj/AMqzQtyls8d8QVJIOo7n5e/9q0SCitcNliikxqB8Ixud+vvSUmlm14IQrjQDls5B1H2xmmy6/ZkKi3BbywCyZAAHbFXSdkmeBUM0bApJERkMDk/72okEspiVhtjHp+vJ70xBEYZ5GYgn+nbvx+VUy/HdamWulrwyNAn4eDCjShA305GBn5UBmYICU2QHSpH0yfbimAqQsf5mXlJyurk+/sO1UaOKaWRznWw8tgSd+Cf24ol3wz+2LLas1zBEZSWc+rfGO/65+Va98FuLfUiD0BdRLYCrjOT7VWG0CzS3MpCrIihVU5PGD8v1pa8ZruQRYVE0kKg64HWtW9QkriWCJI5JLiUDIP8ALJwf8V2S5MMsUdvbxaiW/mSHZepP596joJrKN5VDaWKqrchhgD9qB4pbxxW0b3TE4YsY153HBPSt4at0oU8QvZLwqpkZokyFJ69zSlvavcTnSAFQamZtlUdzRLSCW/maQssUEQy7nZY1/wB6VoTxqLSJ4fTADnQdmdsbFu5PboK9W5jPWFnwwRz3qW5b/t4zq/qGct8uT9qzpWDSuygKCTgDoK1vC7G6lvmZ42QvG+lmGBkjH96Tn8KvLeNpJoSka8uxGP8A3RMp7a2U8JgW4v40ZygGXyBncb1oeI2aSz3UobDYV9+N+f0qfwxATdzO+pVMRA9Jw2460/e41hY9JkKNqXPYHH3zWLlffQrJjs2eEqSrxNjADbr3I9vypj8FpSVo84mDA55Uj+9DtI5LZplOAE9SnOdu32rXt8i8ljRv5RDKyHjPQj33oyysDzNpCZcgD+tQflvmrsq6iz5C+YQd+BxmtaG0WNnxgAyY2680GSwE94YyzIpVvUFyu5yc77HimeSWmXdZaW8j3HkgesHBxwPenPwckeou6jWNsn3rXSAxws0So8gAQ42zgce+1Zl1YXtxeF4UefWxwqgnSM4Gasc/a/pH/DLKO3YSuS79T0Ga1AF2IbI6ZrMi1wRpA3qdD/MAOfUeg+Q/WivOioZNPXHPXb+9dfaThPSWUokVURyki/D6tv8ANWnQ3Ew0sFnbJKtsM8fQj8686kx/DSOucgBhv74rU8G8QiuIlN6xSQyYR17jfevP5MJ3GpR4ZkTzDNkGNcBANz3wKfhl0IGlYiQKHUHYrvkj7Vn3KwSF5opuAWcaevO29L2kzzl3IJUE6z1xjuPyrzyet47PLQvrRdZNukb3TEMSOoxyT0rO/Dy+YGMjMrBU0s2ANjqI9+B+dNKDCEukkLI7YIznJHU9ua7K0QkKuG1RtpDdj27U55ZXpmsSfw6GALPC+UX1Mj9ADyeuM0IOzRMragmo62A+I/P25rWuI4ZJVHrR8D1LtRT5HqADYJwyng99uM7V0nklx5DKSA29pHNltT6vRpyAoOASfvVLSEysCkIUzNpKqdSv8s/+q3Xk8yNlYaCqglgBkKOgzz9qSmE4vLedGKw6wx6jng9qJluGgSIlzaCBo5FGkAHTkjGcAk/4oQtmWAxooOdKh9O64GTkdOKHdxvDPM4B0gnYAlTkn/FM+EMTdeXMzxxgesdCccfnVYuAbu7kjYKiiKN9/Li21dd+p2Iq3lG6W3doycx4kOOVDHAz0OOlNS2wvirImWj04fjGc7EdehqslhN5ieWdYQAtk7gk+23/AKNHHdOppeaH8OZpI0xEVAQZ+I9BvxsM1RbrzolgMkescavS2P8AjzgjP796elWOS1UMxbSxRQN3zzn7H50lceBISQZQiYUelcknnJJ5BomUvIi8kE0sMTqBjUxJdgNs5ANdnkmmjCqgJZ9ZblTjG+f9FVniX8M8Ls8cQYRrtvqGCP70KRmimUeaRFkmRAepOf060QUwFCDTImbY7+sYK+/zzipVZ1K5Ro2OtQACdgOR9djUrOp807nybnAOyZwvoH7miREDU+jCAYBx+lLl8MgPIH68/lRppF9MQ4G5/tWcbtzJXUzSiVUcJgAFzwoqlnatHfzvIHEbR4iEg+I4xn7mmUgiZwFQhQdQGePmep/SrJOzXOQpKJyRyT/auly50th3fkxXJQN62wAoPYAfSuyuUtArAGUAYA6YOf8AH3pWOJZbtZiMtGz4Ujkk7N8qPEiSw3AlzIurJAI3I7flXOzeWoS8cMv/AFJZG/7BUlNtjsNx96Zb44/hyFI3O4/39qHr8u3JKhWU6cYyR23+tHWMtaqxwCUGO5rV64ReW42VN29s/CvekJLVpr6C6t5w/ltl0bZsHn2O1Hk1x+a6HUWbQoxyeT9qEAY9QZ/5jDOkcAD271qbx6RjU0FtqUIyhycnknHP2pGaNJ7eSWR8QOodmYEkb549xTKkqmWIMY30kagfvVl0KuqSIgRjGFOcZ9tu35043SJwxpc2Rja3NvZ/0IT6m3+I+571Wa0XxC3R5FeNFdm0qu+nSP7c1qLYwz5aK4kl9K+YWTSwHTA4+1DnsJLWwuvDrbzLi8nwZHY40r/xJ/Xp0rpMue2py54ZNbiyc2+PKhyBk596oDd3HhE8nlia4aaNVUDOBuTiu2PhyWPhDw3TB3fJkSJh16auOMd6K87m1j0MIIndm0RZ9a8DJ5JrnhfzyynLIXh9gtvfPJNK5fBHlF9Zx8+ny3NZ/iMpHicEYhyrqdxk6Qcg09ZEf9RRdQ1OS2kdBjAH0q99CZdQWNSI2zzke3HPyrXtrPdLJsowLee2OzqNPIJA32/PP0o+hRfvMr+p1+HpnTj+1GmKh0YYU88b8YodqokuC2xULls9NsU3K0bMQBDDK3Ot8/LB/wA1a2heSI3DZTX6FBOy8+rHXv8AKq2qZjnfR6VUkdKqxk/DBHmK5yQTySe32rE7M0usAldUcHZgw0ndiBz9e1MSTjy1jkIjZiSQRgHsCPzpZEmmlEOSWkwGIGMZ4q1/MumWWRcrH8Jxk4BwDRLsEzZXEEiXEYaVDIGLRnUBySfvRbiON/xUTs0eXMiuq6seoDjtuKXt51FwkUEog1MVIX0qfp1rYnuDH4jLHJEjorFS3BxjNdM8ruWlmXFvLZ2M8vmCRW0hXRsgAHjuD3zU0IbK3kkbQFYu23O3GKegkhZpUtpZI3iwjhlBVhufqD79qDc2nnFHeRYkxkAKT9gPlV7bslukBb+KQHzIhlBswZzuxFac0Xm2hkTzVkAJZk2yOxArCVrOzm81IpJW6OxAC+4FaVnczXDRx2+hMnLhs4xjn3qzxs/q3jlqH/DJZFtmUnfPpzuMjBP5HFNuJJWOSpK5LEgDHzpa0VwfMJaQpEdOeGJ2zn/eKuyeYMSARKWySp5Hf865720krBQjpErkbM2MEH6UGcO6ROmGJcYI/wCXTNXifXNPswVfSRpBxx0pqG3lZWTKOCwICnHXjFG2C0NwXlJClTkBQDtvnj70SKdGkEBBBZsDfAJGxP5fKuJ+HSV3RMlnyEfYahwB9RXBbW6XQnEQVwuvSCQqb987kmjX7Nq91LfxvrtY1kizh4goBO5yc9dulU8m2eF3iAHmAjC7aSRjg/WrzvGiy85diwIOMk9u22KDJcqodmIWQnVnGd+5H6045ZWaENQw+UjIigelQF77Y3riRqrGNIXXIyyspIz7/eg/iJXRjKWfVhQyruR1xTrytJFraTAI0hc/njvvWZvnZ0Wna2ijjie68kklxlNII4xsPzoEV2daiSZphHjJAJx96auJkKI8kaGMHSDjYnv3zXBGGGXCaFPq3/z2rfwvb6DkkS9IHl4CAuin9OaTmlUvCGjLGXbD8KM7jFNPEY30ITqDZDDsP9FS+SNbaRtYyp1JsRjI9Q2pnPAuslJiJW1wRFwo0ZCk6Oo32xnipSV+LmS1jkjfEb+hwCcZ6fPapRcJezwfT+ZKzYyFGfnXBFJJPpU65GGogbf+gO9WSQq4gKYJYlvYCmoEWGGSU4LSnOrG+ntXCZzHpykKxLLCjiUfzSSNI6dq7bAq4k3xjAH6mrKxkYldmbbPYVSeXI0oxCLy1b3qbvyo7ISgZ0zqYk55OaBAy28sMSaYwwI0DJ3/AN7125vNECiFct0AGWJ+ddt7Ji0TzZ1KdWn32/tTj9EV7UTXEjuh0MysFPU45+VBvLgmIKvwknJ+RxRvEHaOJQGKyBxkA8D/AHFKQKZIlKli4LgLjOok9adqFbl188lcjQowT/Tnc/Xf8qHZWz3My3OdMQGnc89/ypqbwi+vZ5BDAUjyfU+wONq0bfw63sPDxbT3RJAJdYhqLdSK6SaTMuCtypkgYBIz6tQ2x3HemLa0ubiItGh0OhHmP6FUY9+auPEIIH8qwsRG6j0yTDUftTKQ3F3cJc3Bdo1AcJIcAN236Z3+1WtHYsEaeG2YPplmTSDpzpLE4H2rGS+vby+ngk8tY9RKoMcA8kddu9a1zEHQK9wARMjkpliSM+n6mg2trbwvLb2MLM5/7s2eueO3es5ZSY2q9FZyAViwPUMdsZ4o0ts7lY4omMYXSSu2PbPSno3ggjZX8t5DyIl2+rHn6UC6up7sQ28eI0eMMFXgfOuGF9ZozUCisbKKaJYpA84y7SZJXc/CMdsflWZ4hI7WkgRXWNXY+k4Mg7k9jWnbhPxRZJlcYCnBG2PbpQfLmht2WY6mZy/l44/YccV2lva3KQdXjClJFTbAXkkUYqyQrGwDGQZbIwQOg2o8tur3oQEmN8sdsADHpGfY5oLMIEWc6mjxp04ySwOzfbFax3WXLdtI0qdmyu1BNx6BkKrnI3G4x71JozCreknHqGWOTkciqrFHcSKoLrIRqDAZBFGto34GjSXU80jjRbrnnJyQarcRvZ2hnlCy6FLMR8LZP7e9a9rHBY+Dt8BLECUg4yxPGT2FZwnTVMragjqRjGRjj9KxllJYifhjwp5l0AFDphG07c9R32HHatV7JZJZ7uSRUibHIyTlcbDrWTENUzea4WLJwAegOwFFmnF0+l8qgxpCtxj2reWUvZGlWNZVKEMNK68DBJAq11INSQELp0q0jEfCoG+Pfmk1DeYRCwbc41c46VreWi3AAjZnKBTg5zp3BI+ZNc5bMvZPPGwTy45pWjGuQjynHA6DPOa04IUtYyIVKkkJkMN9/cZq/iMEbSxs6qCTpA50L160Hc3lvAhfca9+BjY/pXfPO5dIdGZlJKMw3JdpNjg/LAozTLmBggXzVYag3GP75qRkMBJglmIDadwcc4qaysZ0wLL5a7Rk+kE964yy0mYYxKkjoGDmPtgNyAf97VIdMcnk+aPWmcD+jA4z8qkjskUZkLatI/U/+6pclBFO8efMkPluePn9xWLlvcSq+e5Bk0MgUNkjLhsZzn7CrNGozqX4xksPbH+auoKqGOdTZ9YGcbfvmha1MLo27OeVPHy+mKz7XXKdlnAAaMEknGO3v+31pV4boqXbXuAwJUt14JpoP5Kjzo2jJ9KKRlmPypRz8JLMWwzEgYC44275rphk1BLcMI41wWLAk75we32qyzTCcwGA+WACsnJBx1PWuXaPHdu0KukZIORjHANEjAkbXIzbDGoA5AO335+1XO9ToLeVI1qyqSNOZD8iR3/SoCTEArJrAwxYbk/P8qa0FLW4YTF1IjQMeDvnI+YpNZWYvrZdLH05+I/THSi+04g0uUC2usrnowByQcDirayrMjlGU5wG7e/WrxFI4Y0dtKED1nYk9/vvVJkLyMvwJGSNhv7kCmXja0ClrDdKVXzIkY5IU7bDnHTtUoturFdS7xgj0qcE78b1KcfJNcrVH3knCsc77n2qt5JqJUHSiDc9qOYmjDyFev2rPkbDFnBCLvv1NcrPbNjqOvJoQRoMM+3yFCkVvL1Kp8tTjPc0RVQeuWRMkZxk7n7cUS3hkkZWkI0qcqBwff5Vqy5ZcJe2tlhjV2GJedX/ABFEiczBzCuRjClup71Hkt3QhpVZc4K53J96v+KVYyiBY22wSdxXSWThCS20CyvLO+7jYdR8hzmhx3UKRMbS30nbBk2J33PelJXlN067spB0sN89t6VmkwRb5/maCoc9W6/n+lMpE13Ekzve+I+Yi5IihGwHTOKJJc28SgeQXHHqO32FZpYWkUVsuGKjzJW74/zTNtHPPFHGiBmCl3ZtgpO+5+1WdsiEnvpkDOgESg4AjXH502kMzw+WxYOPU7scjPzPGxrttFCi+s+aI/UcA6AR+tDuLlpbnST6FIArGEuue0YQQRhtbiQuBkk4XY/c0rfPNPFJHCTpAJ9OFCjvQrOJJWkkkyGL6U25H/ur2j+cs4lyhYYZs4wOMVi7ta+A7aNpAyxuAcYDHge9WBkFlGqsDIBgk/1b/l3oF5dQJEIY86GJCqo+L5mixsLe21yJiQ8Kc8nvXSY8SM0O3ijsnSAELqGWfOGc78dqlkySWplUGEFicqT8I/01W0u2M2ZQnmup0lRjH/kD17U7JHIzvzgMcnsM5FOXk+Ir0XMmmMXD/A4yob5Z2/3pS1vM06yPIiiNiGUAfFtuaD4m8guIJGUlfKJVcbb5zk9BjFSxaSSyBVv+5qC9s9P0xW8pxqHQobznKs48tyZIzjOAdiv6/Ue9PiOFCzFVAjUBtOxPYUKG2NrBFK6kEguMj4fb96UKvLrkKhlXch+3f3Ncct3LQacQN34XF5iErJNkKfTsM7UnH+GS8aFLeLHDalzzwcntWgHaPw63jAyCmSaBJiOA5hjDPpLAtjIGAPl0reP9tmTaiKs9teII4w4Qx6FGn1c9emKxYAyF7pyUjDHGOSeAB33rehdTbvNnJwUdj19z9PzqoSBTK5iDp6SpznTv0+5rXtJdUkvDf5xWcxmOPOAOjHOB9afhvY/NkiUAEPkDBBwT36UdYjb20mtASqkodI5PUUgzlr828dv6Tg6tIBIxn61i4+13WpNDzlSmXRHH/PT+efpUQx/h3uDGFYEjH7fXP5UEMGXII0klic7BQMDb7ig3kqusMWrys+vfr2H71i4/TJsTgoEKRvq9XGM53xkdapFdISfLGjuQc/WlIo9bgNgADJOc7e1Mv5ILRmZiQM6gMA79eufcCtY7Gh3I8tWTf0Fvnvir24H4l2JD6gRpI2LAZB/L9aUjjcYO4jVNI66s568fX2o3neXoESI76stnbUMcfKsY7tM/a0kzvJ5WGZdPqXsSeg70G0iaWZfWwAJc56fWmdEkMgZ4mZAdmxxt1zwasGCy6VwNUgTbsP8ANV3OF0HNITIzphCjBQoHbnehII5XaTy/URhs7ggHO1ULI7EOpJwXCk9v9zTNq6M7FoljVslcbhTt/bpWpLvlBSyweYPMVmEhC4znVzjb6e1OqkRiSSFhuNDZ6qOftQJUjlYI0aLcAbDVyP74qs7tBBGisyOXAwo4HsK1lN601DV3K/4CGKKFCurUBzsOtAOUQNAqRSnhyurPO2enBol/K9vHAsanWSF3G2/A/WgiJpFkXD6UXLcYYY/XbGKN3YvFDAlKu88gaNiNLH1aj8v3oiX2t0dHZFAO4xpJ66ux+dLm6OmMSHK5K5AACn+3AoFuWsBJHKkWg/Cpxpznkd+OtWEt7pjQmVYrlVU5AJOMbNkZB+VSryETqjtFqJOVXI2Hy7CpVl45bytfQt5caVCE56Vn5EjKzOjIM7BsnP7UN5nuZ9vic4A7CnLWx3OoEIpwBjmi/U7c+14IhLJ5rrnAwo71e6f0SRoSW0kkryduKtdTeRGVjI81tgO1LhAmsqxL6SSc9a3/AEmp2GfDEysqMcZbWyj+nA4pqyl8+9YndSQMnrg/3pWz1PYhhhXcbnt70xZszz6YlPkRJ+Z61XiWpZStrHLK/wD8jFmB9+lKW1zJJ6UMrn+kZ1Zpi9tGuHVpZfJgXc9Sx7AUI30NpGY7KPQnVgd2+v8AasYzjkm5rSBUzOQZGUApgbfM9q4Lh7kGKPAij6p6V+f1oNvbysFmmkWNCuo5G6j5fY+9ce4WbQkSlIAwI9/dver02jnniJEijDRqvIbcN3ORSemQ6mcZzISNO4x0qSOZI2kjViGA9ONwAf8AGaJHEZGBjJA3JYVv8sZdcm9OK/8AJyTk7AGi3EhW3k0Aa5T6hj4SOarLG0Yj8wB1YEjB7c57Vzw+OFEMQckkZUu39X+a4y86pnWkgtoreFJZyDpAVB/yNJX8ryXepSdhnINPTkXBMlygjjiOY331Dbfaqeb5boqRaYdW/Qtn3rvbLrTNcSABIriWOJXKZMjNhs52267U9Y3H/wCJLkBj8OVG5ydsUl5ivJdx4GtSMnchRjfGfp96pYu26YIQqSpxyV3yPua5Zy0ymrq2/E2o1HSUB06T8QA2+/FCe1L3KSudKQxhQi7Atj9qtbtqjEb4CLlNuRt/nNDuZT5DRMfLOn1Md8gU43Le78Dpy6lP/wCMSCR5hXQvLZO3610QRpPI2MsNjITtjsPtVoGljjJJISNA4dl1dQBj71zyuiYkiOWXBxqPbPTJplkQ97OkAt0KeYxQbYyNz1orBZ43dmyX2Qhsb4/YfrQ7hib6KJyGRlVFQDJ1dT8qBMyI5QepUwgwdzk5P3/at3LhrEBJQpEcwxDKxT5YorRvPcohXyxnEhU9Bz99vvVlPq0hPOBwQpAzgjcUyJFjUsqYdttt6z/tbKSXjG9SPKkqPQOpJ6faurEsFypE7JJ8QDnIPbcdsfnRoreK2eS6Meq4YYXGScccUpdyM7s6ksC+h1xuu36c0yoe8jOkW8MTiB8sXXdR101my2xnumdXyujSpXfGeuOa0Ybjyzry0YK509R/iqy31pOwW4tmYnYOnpcH6VvGreg7dUtrGSQr5jnfbgb7bDrmrErLbytGUE8O8mntjjIpqWyMv8qGZZDq+F20P/ml7OJba6n9Dec6ZaNxg4z7bUSEvLcNFAkSBfWup8j7D8qkb+c2Y0jSfTkIxyCf/Enih38JF7KiAlRjSPbGxNCjVVdZHk1kA5SM51fX/eKxjjQ0LGS4kuGiJ1ZGqWNzzjqB34pjVHjXqZSHDDGGwd9s/wCKQtL13EmtQEQ4JBxj69/enUkRn8qXaSUlUlUbN19Q7/L86LOT2aVlkdSBG2ACCAM+43rMZpZBEZ4nV5W4P9JByM/TNNxRSxnz2jjkQ4KvFuCOD/fFUuGeASGNW81sqmGJyc7VrG/B7N+UfMa4EYcHA8w8fLvRfw0EkqvcvtG2tTk5BrJfxIQrlUjVNA1Mo0lu+Me+3/uiW3iAmEiwOVkXIw3fr9B+1b9flqSdnLidJXkWEOoAyZGIIXA5P+80O3uEJCgMwZSVX64x+tD8OlWVCi5w74CMucHBJzn5b0WZhExj0hdXBxxt0+tc7NMXnson4n8ayBFmiKhlZ8HUDx9f7GmAsckrRusRiXJYsgPzGfrR4kLITMRrjY6GQjOknqPakBHJFqWdVyzZHUadqrxzFxow1x5UuiZQiAgCMjnbbHf9KlS7VporK6DDMa7g8Ej/AEVKrfo7kL+HwFUeZvkK0PxX4ez1MS8jk6VodywSJEUYzvjtWTc3GrIVwf6c+1U/ByizXTea2k6pNXrft7Cn7f8A/ptR39ODj51iiTJGngjOe9aSysLXSBvnGxztWee0EUcwi3i4yFJ7CmwBZwKoIDHA2pe1LvLMz7Rw+kf+TUeVdcqu/wAKsWNWVt4iL3UN1eS+VFh22VsnGB1oFnYQ28ogY+fON3C/Cn+acv7ia2tEjgJ/E3J0jHKr1qtkGt7YQDGoAl2HJJrW9Ypo3CLLCB5pTcBT0I7UI2VvCHkdmZxjJLYXb2odxKts8UnxMq+hex6mh3Ba7hMbcuOcbiuf8kwkl+S5bXkUrlYfJKkZ2XJNEluLjzFRAiRgZJP6YFUtfD2hURwJ62GSeuPeo/hzj1zXMYZG3RDqxnbetW3Lro6+UaeKU+XLln4JXIH+aI+Et/LSGMjJ+FOc+54rv8tpUTSkZOPVjc+9ceGS3vhGHOlsgEj4h3rMx10hEjkiheVBG4i9Mkcg1aSOQD+dK27LJLKwWLQ6ekAbggg9TTRaaO489FB80fzE41D/AJD32pO4iKTmeJSYXTGex9+2K3rU3i18cKRN65jj4vUT+n71fU2zRJhU3zjYdK7LGVAEpALHOx6+9NRwpDYOmrUoZcFjudXP0yKJn7zhmTZaWR1tS3wEDC92PGa5MuqznNsuZVVoyOTqI/ei3MaNbBQdc+dYX2Ht360FYyiXEoOSfiAOnJ4B961OwXsImsbDFxIOdTgDUcYOBjjk03+GMbpNGWiR1GYTg4NLy2pRYgXCRbaiTnU/b3NMuWaeNQPQDk+1GVvX2trTKwSSSIgzMNAJOMDO5qgiM0i6EZcnSzjYsD1xQY5mnnQ6gsZYhhtx0H50Tw+WX8Sylm0xoz4PXb/IrPNnLUiQSRxwlttWcbnNWE5c5KhuuR3x0pWKGVvMjy6RnYnHP0605Z2rxZaVgx1bEKRn6VSXLHUFWiuBNdqnxPG3PYkb/wBqEWtluTGJTqZiSFTUNjvkijC5MV15UUa6VbLdNR5PypVGtWUr+I0KTqfAO++eeg9q6Sy3RlWdrZisMo1SspwyIQOuQc1a1s4oLkE3SPG3oaMqcjtvjc5xV1a1I1iVpFJCgohH0+VcfykBAnXIyNCoM/8A+1b67XS6Mo1TSJqKyMMMcc/+uKv+Llu5lViQoB07bY34q5Z0s5GgSJdQR8lQTzhjvyc0r4dPN/2roI5BLDSnqQHbc+/ajFqTkC/tfxsKSrciF9GQspwrnger6daXgsvw0UaXxMYJJVlYYB7huOtN+JQss4MmlLZEEJySVPy5IPz+9JrJH4eyxC5ucad41jUrITvg5O/bit/DNnI00YSB/wAOdSM2SVG/vt3q9iomcwnKoVUqSec9PmDx9RRY4mliEi2mnIxpRgMDnccHttXYrFolOQWLLojEmzqCd8Z5I4rGM7px4oTTXFtd20aKybYcAHBH701fyTmNmjgLTqv8uTB04IH3NcRXMgaTKyRoMqwI1kddPepfRhkl8xGYHAYkbH7Z/wBFamOrHSR54WzO8clzII9LjMZOcb9QM08kqyXKNpK+tsb7AH4qLPBbCOPSqouQwAOS3sOw/Ws8xmMOCxIZWAbI/I9q3VZWzHcaZGMSaRINOSMb8deDtj32oZDAojk4UkEgbjjFJ287tAYfOcMCGQ9z2z9BTPnNN19bHOnv0/WuGc54YupeDVs0gnWUDOoBWBG43wRXSgCrGoaUK2MuTkDORigW8y6JAG0nIyvAzj9xTNqPxLGMnDRqxUg87EjP51z5t0wKYvN8LEbuR6yMg7jO4/MCpVQdXhRbJADncc7b1Kzcs8f60wvcvJOf5QLORgYrLurS4tHBkA9QIGDuDW0pSCNmVT53Hq4UfvWc7wANKFNxKxxljsD8q74zfIkkn7LxgzOSThVAGcdK0IWDW0gAHxACkriWREUDTqz8IG1FtH0pgnbOomueWWme2lgeS422UsfnQ4isseuXISMFmI6+1USTELqSS0mw9hmrXMiRQ+QDjTu3zqx/GIC8umYFsDU+wHb2rnh2qOBnl/7jNlgegHAoWvVkxgMcas+1M2dvNcnQgI1DLPRPapbzDclmVNTkhVx0rQjtYrZVku39Y3Ea81GeGwiMcOCyjLOaWgD3UuSSWIya5+SSa1N0rXd9cTh4oF8mMMMsNsjHHvSyYgiGUJ1HZu5o7KNJ1kgKCNhvmlRgziVyTHFwp611mXtjyqM7h5C+WBT0qcbE5o0i+VflnYlUUYLHpjP60pdTFhbxAEZYPjvXbxla3mmkGrAZgM7E4om9EX8RO9vBHENKbrrfljzt2okDSR5aRV8pj6s8Ajt/al4PNa1VAuYiQ0bA5IGPy7U5GkXmo81ySkaf9tRks3vW5ly1N74DupPL8uWNE8p8gORlgRuQc8bdqAki29mrzy5aWT0x/Lg/PmmjMtvcT206a7VxlNO+DyDSfiUCrNbxaRhE1yHqGbcD/e9a9ZdRWFYlnivNRkkeIZk1E7bb49ulHllhiiS4uIyPMGRGBvnrn2oYmW3JZmJAI9PT61RbeW4M0fmeZHN643JzpbsfnRjf8cmB5US6lgkYDKHWOmPp9qMSUJOr+hm+vAoCxksBvqA05HSrpNJCHfT5qNgBSucDP5CuO/amQON1SREA1b+rIyo/vTsejynDnTJuAAMj8u/5UCO2sL7S5imt2zyu4P0NONYzWqIYBrjJJZgNwB7dK6zxtetnTNnjEIWQK8ko/qUb/Wr+dKYjJOxJPAAxgUeeWLSwYbIBL6ep9Qx78ilLaSfyXkmBDNHrCex6ftVlN3TOhpbY20rNI5GYc4zsC2f80jMnpSSKRFB0hihBwf8ANO3iFrWKNySqfF/4nSCB+uPlQ7MQvC4W2kIXJBZwRqHH61Sab1quTyCCLQraWkbJUe9LmXSGQMqy6Qdjkj5U7BFc3M2mG1RUBwZnJ9Xy/tVbixtkaSDLW8hPxOow5x36DJFa9PmjVo3hEpu7G4tz6ZFRgGxuQRzjvkD71zwizEEba5JJHRcnWee2wqlgJLLxBA6nUM+bk7lcc0V54IgTr/mZwo1ZHG2R+1b+WsfugXkrwyTG0ldZXhDMMbHf7cZpSEtcK8JXRNGf5ZP9QO+KPcyAXsbBsnQFYat+N9vnSUwlVlKx+sEbnk/KqdaFnI/h1xIJYlkYmCZSpVjnSc4/350bJtQ0TRRhizhcDSDjTj9cVyaFLuxEsRC5ky2ATofg/t+tGWFvEDYzTnQFLCUKQc7YyD2O1GWsZv4Z+Sd1PJ5ctyzakAXywwzpyd8j5Zo8HiBkh1wzNFICAQrsq/4qkSIbadW9flOVk3zsM7j6Z+3vSU6eQ2pUVkOzgcSIeo7fttVOeDs1c+I36egzMpPDMQwbtuetdeZL6JNa67gkqOjMOoHTPt16UtPFi0JOJIC2AwPAxz7MCKXbWhgjVSSVGpQOpOcj34rfw3u2HpIbZERlZ1Y7am3x7fMfvVZlGYpcZLEhh2bgj67GmI4IvEfJE7FZ8MGfozDv2PG9LpbyJaukw8sodRUjJJ4OP79q5XkZcjMx8lRJpL6yDkYyANgfvT3hwii8QWRHO5GtOuCOncVmSkG1gAOx1c89KNOwXTJGcHzNB+hFZvcscz4Lx+D4IBKyEbdd6lFuHEdgxlyFMm5A4yTgmpWfJhu9InHeRrCn4iTI1Y1gbqfeiSWygF0x6hkFeG/zWPajz4ZIpAdJw2fcH/3T9rfCNvLfe3J0gdj3FdO+gVhjM8qITpJJJz0orgIRGOBtmn5bdUZ5uqjDfLvStpCJpvMfZBu1ccpbloGogILf8Q4/mN8Cnp71nzNrSTzP6ick9K0fEXUy5AwNAVR+ZpS1sJPELhIhkRL6nNdZrqIXwKza882Rsqh9IPYU9c+IRxz/AIG02VBl3Ht0q19cpa2n4azGFUhSR1rNjTyommmOJG+FR8+tNvwkupCF1McF+Bnge/vT9jlIjKMg42rHmYzzKN+cVr3Mv4WzwBuFyRXOzn2QczHy39zvQtGpxERuMEnO1GhjF1GUJwW2B7EilEk8hWy2mQg4PasYW+qL3My+fGwbDg+UtOSoskKwkghgdW/v/igpZwCATzKc51xAncMetViCFw0rEoN3PtW85bZojRxMMFSNIPA/enrSFZ/NzIS6Lq0g7kfKl7iVNJMbZQJudOBnoBSdpcSReLRzwrjQApGc56HP34px701O2xeL5wghQoXEQfWdtWeFpDxCaSSz/EpGPOjASRc7gjv79Kt4zcCLxx7</t>
+  </si>
+  <si>
+    <t>En Reposo</t>
   </si>
 </sst>
 </file>
@@ -413,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N5" sqref="A5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,9 +480,11 @@
     <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,9 +521,91 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ahora se puede editar los datos de registro
</commit_message>
<xml_diff>
--- a/registros_vacas.xlsx
+++ b/registros_vacas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Downloads\Veterinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFBBA52-FF70-4CAF-B15C-F52FD8A58760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3E4AB-C4D3-45E5-B838-794BAE81E4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="A5:N5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ahora se puede activar el dictado de voz
</commit_message>
<xml_diff>
--- a/registros_vacas.xlsx
+++ b/registros_vacas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Downloads\Veterinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3E4AB-C4D3-45E5-B838-794BAE81E4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA195D34-35EB-494E-A94B-B68DC8584D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ahora tambien se pide el estado corporal de vaca en el formulario
</commit_message>
<xml_diff>
--- a/registros_vacas.xlsx
+++ b/registros_vacas.xlsx
@@ -431,10 +431,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -452,6 +452,7 @@
     <col width="15.44140625" bestFit="1" customWidth="1" min="12" max="12"/>
     <col width="13.77734375" bestFit="1" customWidth="1" min="13" max="13"/>
     <col width="26.6640625" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="8.21875" bestFit="1" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -523,6 +524,11 @@
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Enfermedades</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Corporal</t>
         </is>
       </c>
     </row>
@@ -532,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-10 10:39:54</t>
+          <t>2025-11-12 18:41:39</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -581,6 +587,17 @@
       </c>
       <c r="L3" t="n">
         <v>3</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Ninguna</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -635,6 +652,70 @@
       </c>
       <c r="L4" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-12 18:08:50</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>b101</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">estrella </t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDABALDA4MChAODQ4SERATGCgaGBYWGDEjJR0oOjM9PDkzODdASFxOQERXRTc4UG1RV19iZ2hnPk1xeXBkeFxlZ2P/2wBDARESEhgVGC8aGi9jQjhCY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2NjY2P/wAARCAHgAaYDASIAAhEBAxEB/8QAGwAAAgMBAQEAAAAAAAAAAAAAAAECAwQFBgf/xABMEAABBAAEBAMFBAcFBgQFBQABAAIDEQQSITEFE0FRImFxFDKBkaEVscHRI0JSkpPh8AYzVHKCJENEYmPxNFWDoiVTc7LiFiajwtL/xAAVAQEBAAAAAAAAAAAAAAAAAAAAAf/EABQRAQAAAAAAAAAAAAAAAAAAAAD/2gAMAwEAAhEDEQA/APfAUE00IEmhCBITSQNJNCBIQhAIQhAIQmgSaSaAQhJA0JJoBCEIBCEIEmhJA0JJoBJNCASTSQNCSaASTQgSaEIBCEIBCEIBCEIBCEIBCEkDQkmgEIQgEIQgEIQgEISQCEKqecQt7uOwQWoXOfNIWF2d19A05VDDyzvbnlEjPLMdkHUQsLZCfec8f6ipZhV5n/vlBtQsWt+8+/8AMUtDdPeD2zn80G5C5zg4gOa54Hm8/mm1tmy+T0zn80HQQsILRZBd++fzRYJ0Lv3z+aDamsFA/rPA/wA5/NSoChb/AN8oNiFjqxqXfvFGUAjf94/mg2IWYMjcNbB/zFAjjB1s/wCo/mg0oWflx2dSf9RSEcddb/zFBpQs5jjLdz62UwyOq1PxKC9CzhrBemvqU8seho/MoL0LMWMo1Z+JUTHEHAhrttrKDWhZWhgGrT5alQprveB+ZQbULHkb2+pTDG9AfmUGtCy8tuvh+pTDB+z96DShZy1p/V+9RELNaZ9Sg1IWblRn9X6lLlx600/MoNSFikgJrLQAOu+qmIW1sg1IWUwsGw+ZKXKFaNHpZQa0LJkYPeajIwgeE16lBrTWRrfGcoc0dCHHVXRSFxLXbjqNigsTQhAIQhAIQhAk0JIGkmhAjsufI4unNi6XQOy59/pXnpaBgtIuh6IL9RY+SnG0HMTW3VTDRmIy6UgpzAgjRAo6gK3K0h1tG/UJOa0ttmuqCsCvVIvAJde3RX5BZ02UHMbTi1vVBUZyQ3L8dE7cTd6eikXRxxtzDTqowyOmDX8tzGnWnCigAQLI29EB4ArunIwB2a9DurC1gGoFVugrElqWezfQ91J2UN0rZV20ka/zQTujQSDj2UC8N3NfGkw9leIivVBMOUgSotyu1a60F7GuDXPANbEhBPMaQHHakF0bXAPeA47NJFlFxl2USDN2sWgRcfNGfT+aUj4oyA+QNJ2BcASlzGhxYHDN+zevyQSs66IzVv8AeqRioA43MwdPeCnz4MuczNDdrzCkEw4qNnqEOkjtoEjbf7ovf0T0J1OvZAZv6tHwR00OiRutD8UDJN32Ts1aQdbuvzUgPXVAxmI8k/EehUm0Bv8AJOtKvqghr2Uad2VuwCNLB6hBUWu2pLVvTdXZhSg5uYNF+qCJvaqTs3VKdDbXUboaA0eaCsOLnUKUqO1KVDMCNt0ad90ECCdwovj2U5DSQf21QQLnA67KTHEubQ60pCuu6bWDOEFyaSaAQhCAQhCAQhCBITQgR2XPGbO6trXQOywfrvo7FBa33C4jXsk0lxAFtA6qIeQaH1Q6QjYAeaCejnFlfVc3irTGYSHPPiLSGuIsb0ui0ucLFX3WefCcwscSTlNiidCg5LTJJw5sxe91zU0ZzYF7EofGPZA4F4fzGksDjpelfGlfI2PmOHLkJMhGVt1mAvZVvdA4NaY5X5nklou8wHXVA3YUh0Ae0tBn0aXEkN3opYmFltLGZgcTlrMRYI2V7poJZI4Z2PY+TVubSq+O6g50JihAgkdGT4D5n476IKXRNcOU5ptmIDcgcTlB6eivxzI5cRhMnidzCx2p7XSg98eUsOHeSJAMo0OYi+6M8EeVskDo+W0yNs7UfI7oJYfDxSYM4iV2WZsmYydiDt/JUukeOJsnAcI8/Kvp/V2r4TE7EF7sO6OQjPbhofPTS1U1+DfhHu5FMa68hBskjT5oLOJtbIcOXAH9KB/JYMQ3w4mOMfo2SMyjo0ncBbZpopGj2nCuLmUQCb3NbqqV0OlYcHDRvOY0KJ29aCDVw5oidK0jLIdXsaPCNTVfBVwRwy+1uxJpwkJLju0DakRYyDD89scGUscAQNM2tX9VrmETcRGfZWySOByk0KrzKDM4RyN4g+YXIDu7cCtK7IwjxHjRNPlDvZg5ziOv50rZcVBM6N5wzXOLSbe4CqNVfXVKWWJ0hL8JG92UPLi4dfPrsgrc6OU45843AIDtw2tKWZ0j43Q4mv0scTC7uQSRr9FslxUU0gHsrJCGNdTyA6j0AO6lNKzmSvZhGSCPR7jQJ0ugOtIOYWiLDzNNFwmZqdTen81diHN5OJa4tLuaw233b8gtL8VhmumHsrCWNztOUeLS+3mrnzQMljiOHYWGi4gCmE6Dogy4t94gzsILcOWi83xNCvP6LrtIewPaQQ7Yg7rPhxDLJNHyI25HhpoDXS+y1sDWtDQ0ADYBBBpIFb6J9NU6bZIG/kgtArQIHVnQ/VAvSr+JS90lSCCwkhgyhDTuTv0tR+NJAAkboJgmvFt5pu1ApLKANUqvqgk668KL0F7qBZpuVHLQ0KC3MDqE9c19FUwgmlOh3QMkgbde6V06yRolQPW0FoJ8+6CTqcLVZaDtoUFhFUbASvVAvED/ADU2k5h5nVANqTa023QWppJoBCEkDQhCAQhCAQhJALCRUkmvXstwIIsLETb3+Hr3QLTTTVOqFIFZR4dfVSY4B4GX6oLMugpRykaDqrNOyV10QcyTCTNkMjAx1Sl4BNaEUq34CV2UkRvJeXuaby6il1radCExXQaIOMeHPc4ZgxgDC1uS/Cc1gi1oiwrmw4aLM0vicHuq9tdlZIYXPldMXNLH0CH6jaqHmqGlhikdyxoH+Lna6X0QOTh7pJnOcWlplD6N7BtUo4jhuc1HTGcssIA63dpyvjZXLHgytc4NfoPEN/r8lZJMwYsnTLnaC7PpdOQUSQ4uWJzJJGNzNy02/ifkqZMA8l7WynK5oGu4IPhWjEYhom5jGOcyMC3NcMovf6KOIdAcQOe0Vyzq51dUFb8NiJmO5srReWg1vhFG79VH2KSpIhK0QPdZGXUdSAoRvicfHEwuyt/vJaI09FqldAcQBOy25DWd2l3r03pBVJw3mtd+kAcZC8Gumlg/Jb5sK2d8JkylrLtpG9rA2SFsrXZJA0OYbc7UDK6r0V7JIHTB0jWmNzn05xsH3fJBbicCC5rojExrW5Q10djdVtwAe55mLHkxhoGT3avUdt1F5L42lsTzyW5xbqrXTp2H1TzQOzZG/pTLYo67jXbakDlwJlYIzM0tyhpzsBIrqD0tOXCFglDJy1knvNDbd209VUSMskr4XBszHa5t+o0rTRTkLWT8t0b/AAZAHXuM+nRA5OGxyMkbzKzZaIGraFfch3Do3tlLpHFz+o0Da206qyAgS8x0Tm86zea76jStNFq7nKfmgxxYORkznsxVB7g5wyA2apdAFrtQQR5KA0IFHXzUw2hQb9UCe3wnsq6I2+Csc7KBp9UtLsg36oIgg3R16qWUH1RQqq6907A6HRBGgK20TYDY8k7FbFKSaOGNz3nK0DW0Fl+ayz8Qw8Bp8gJ7DVcjHcVZOaHNbH/yuAv6LAZMP+zL+8PyQdeTj8LXgBjiOt9FY3jWHe3Nmy+RGq4Bkwp3jmv/ADD8lWJMKDoybX/nH5KI78XGIDJTnFvS60XUjkZKwOjdYPULx/MwwPuT/vj8lrwmNiwzg5gnGviGYUfoqr1NEaJHNp0VGExcWJiD2d6IPQrVoUER6pFtoIo6WlYA1u0CynRNhOYA6apgjzU2EaBBYSBVndCCA4UdihA0k0IEhNCASTQgSEJoEVgOkjj5reVzyCJHu8+qCWbTXdWR0QCQqbsEHRXNIoX6IJagEqEcl6G/JN5puihmHdBeCPn1RoSFUw2VZmpAnRsLw4saXDYkCwlyYw68jL66BSOoNKl8zI3Na57Wl3ugmrQSDWDQNDW9gE+UwNyhrco6UFVz48+QyNz75bF/JWOnYxmZ5DQOrjQQVSxgDRorsszm2QSAtMk4MPMa8ZauwRVLI7GNaGkyMp2otw8QQGUHUi/UWmNRrt8wkzExyCwGkXu0qOZjnlrHgvAstvxAINLY7rW/66K9rdKWCDH4Zzgxk0Zcf1Q4aq+HHYaZ4ZHPG9x6B1koNYF7+mqiARpfogOvXfTTzU2Cxd3+SADel6p5B1PopivVB12CCsZaPiBKiSQSPgriL6Uk6i3cIK2G0w8dUHICDf1TtpvUEeqAAa4aABRdG1pB+WmykSK1I3SL7G23mggHDZ26kRokMp1G/qoltXlqydUDcNT5rz3GMcZp3RMvlt006ldPiuKOHwjyHeI+FnqvLOe8myT2QD3aaKDXkCjqO/ZSyyOFgkqTYdrtBAusaWU2t8O1FaBACCbICDGWjUlBRdUHClEvABoG+hWmRhLNDdLG9rgdCUG3hmMfh8QHbtPvC17CJ4cxrhq0i9F4JheXCjsvU8AxHMwpjcdWGh6IOxmFpOrZRcDuHFLNRA6oJZXA6aqTCQ4X3UM3bqVaw67dUFqaEIEE0r1qkIGhJCBpJoQCEIQJYSwuLiO5W4rKzd3+ZBWWu6ghEgkOGeG3mymq7rU0D1ScwboOWDicxD2ve0DKABdmtDXr9VnkZjCS39Jo7Nv5VX4rs6NB1FdVAhhfXVBzY4cSWeHODkO5cNaFdd1phjnMrS4PuzmJOhHSvotdM3JArTfZPPHeUuFnYXqUAbavK42d7uKRSyxTAsnDWNLDWUdu5J1XqnOjzAFwzHYE7qrEQQPLDMGEtdbC7ofJB5nFCHnxzQZX1iRzXEnm5r2F9F0OMOZKcPlfDJy5iHROeAHurb1Hmtpw+EbiDMWw80buNWEzHg3OfC5sJc45ns0JJ7kIOHFDzuG4wuADGPe5jWOOUafUKcjGxcHhlkgZI4RtDA8A6ld1rYGsMDeWABqwVt6Kh7sK+oA6E8v/AHehy15dEGLDRQ4GCOBzmB7z8Xu6rHBFHBxScReENia7cnqunIxkj2uLRbT4SRsl7O0W85c1VtqUHDwRbFNAI5I5s7HlxEdFtAm+/wA1q4U5kWKw7IXxTtew2QwAsrre/wA1vjhDHF7WNaSdSABa1sYw/pGMa0u96hWqDRf9fipAm/P8VUDp/Wybbqv6sINId0s0mT2tVN19PzVjfdQIWBqSgjzKLJGgScTVbHyQPUUBZHdKikC8Cuv9eSA6m+Kz6j+SAc6he+vQKNg2RZ0qgU7zNrKB30VYFXlB+KCYJBAsV5pB4dqTXa+qWbXXf0UXmhbug26IOFx+Uy4lkQeMjBZrzXFcbOnTYK/F4kzzveepUYGF7watBbDHTNd1cGE7BSYDXVaIY9LBI80FIj0rX4JmLuVrDSNrPxQY3EagIOe9ooi91mczddN7HA6t8tFnlaKsaojmgZXa9F1uAzcvG5dg8V8VhfHsAKV3DnFmNid2cLRXsGeIDVN7Qd0mUANknv11QGU9D9VKPMHC+6iHajbyU2G3NBQaEIQgaSE0CQhCBoSTQCRNIScLryQM7LKHtbmvUglauiy5A6+mpQQ9oAe1rgSXGhQ/qloo1uVWIw3bVWAoPO46RsbOKQP0lmkBjb1cNNlRiwIsfI4Bkj+a39G5pbKNvdI3C9K+ME3okGgDWr7oPPPeTFNhSLxDsZnDK1IzXfpSrxT8gxHMjY/FCZxpzXZiwe7lIXpS0aIABKDz2JlxL8a7GCJz2YdzW5h0H62m/VauORvmZhhGL8bnDS9mkj7l2MtFSAtB5QCSQYmZ8ZBm5UlEd5NB8grWMDMe1rWZz7QSWyRFr22Tbs43HqvSOCeUVqg8zEMQ3GMxxieI5nlpJP6p0bpuKpVYOMsxcDWxufleczZIcro7vXMNCvUOACqMdnXZBRTazFhA6oEJldY0b3VjxYIGylECG6CggolZldQ6eaIS7VvcK6SMPcBdWeyTIaeyn7nsgbSHDX4qTXAa+V/JQ5ADy2yNCbTEQIJDjdE18EFwcACL7qQcDem52VcUYc1jr97t6KxrBQ3Fi90DzN76bp8xhFmlBoBZY380nRhrsos6b2gsLo7zWL7qBLSLBsHbRN8VNFE1sVFrRkBdfvVvSCBbq0nf4IDidxQ6FWUGg333OircywddD0CBEGyQ0a9Vkx8rocJKd6adfNaTbbLjTeoXO41MBgqv3nAIPNZcrhmG+2i2wNpmjRv2VYaHxMIFkFaYTYqkE42bWSbVwYR7pIPks7g4mgco81VC6YvIJoV1QdFr5DQcSk9xGwIVTHFp8Qqx0RM/TTYoBxe41moFVOhGmptKQuaxxaKPXyVUZkEYdvrXZEJ4cAW0jDgiYGtA4Wpk2M1EaVqoMdk1OmoCK9cxwoUNU99d1TG4ubt8UAuB111QXhtnQkKcbXZ9ToqWuB/Mq6M+IWOqDQjMCdClRGyA2vTsgaAQdjaCNKSa0N90UgaEEIQNCEIBCEIEVmDqLh5rSVj1zu9UEs2uiTpHMYXAZiAaHdVukNlrKsbuOwUT5vffe0GaKWeaXkEuDmA2/NprXz6q5jZw4FwkPjs6Haz512QJGAuzlmZh1Jr4FW+1Maxzi9oDdzaCuQTOaQ1r82ckXpprSXLeXWWyGOtg7UH5q0YiJzsnNaXHpYv5J86FrSTIzKDROYUD2QVwRyiepLIrUk6bdNdfktrGNbdDc2VmkxEMVcyVjL2DnAI9uw7A0meMB/u24a+iDUWhRLaG+6zSY7DxuLXzxtI3BcAQo+3YfPkM8ee6y5hdoLZNB5pDxDcqInifGXh4LW3bgdBW6GytLQ5ptrtQRqEA9gDUR/gqvaY52AxPDxdWDYV0f3BAPzlzctX59FW15DwA4E3Y8KcspjcK1vcKtjoy7M0OBGu+iCx5LZDZDSQdmoiie2Wg4C71rfRVPmbIfG03tYKk3EEyZqugaHqguiLy/KCKbXTZSjdn0aTmA0saKtsoY4lrKsm9UB7WHM1oae+9IL2h7mXYB7UlTzFmzHNVhV89ttdp4RaDiQCXZQb+5BZkOXKHP1FlRBLYnUXHKa23SGIZocosbJc3Owga5utILWAuZuQegVBdlbdOPTVDpnteHDYDUdFHOXnxDKdyBsgZIPUWuD/aAVywTuSV2XBwHgAu9157jsmadjTsGoKMG4CNzDl30VrLaRo1YoXU4G1pbJbtDd7oN7S1wsgDy/ophrAB7qztfY0Np7lBYXixqKGypfI1p1pR1c/yUZBQQaY5GObRO3ZFR3s2vNZmutlqZOn5oib8uXTKs8pa57QMugSc7z0VEZuYHzRXsIHHKLoadFeKNdlniosHpop6mgRYQWhgKsjaC5p7FUteKrboro3eJo7aINKaSaAQhJA0JIQCEIQNCSEAsbxZeASLOq2LLrneNNCgz2AAKoVQAUSbWhliQ7fJAJJBFba6IOHjcK13EImi+XidZWVo4s1H9eSxY0gNxuGcx3NkxAcxoB8Q01XqHvLCMx1PStVHOHNcC1zdKtzUHmZGxEYmGOEnEnEHlEMNjUa3XTVbXYQfaseayxw5zm1oXt0B+t/Bd5oIIB7Jkb1WyDz3Ff8AxsLnWG8twzcnmdR0pUz5QWPAe0OhyAuw9tfROlVbSvTAEN17oc1xO+iDhyRF8nDnOwwaTeduX3fDoD/NZmN5eNkLxKKnJAEGYEf5q0XpnURdhKqaNR5oPPYaYtwsuFME+ZzpKOQ5dbI1Q3HSjhvJjgnbI2INBLCBeg0XeFFtCqVDzlNFor0QcnhccuHnfC+Ooy0OBaSRY0Ovnuu20+HzVLXtI1q/RDpg0UKce9IIYh+Z/oo6NjA6n7lNgzauoNHkEElzr8PyCCk+iM1G/itIbTbIbfp1RTDs0D/T0QRZ4m7eW/xKnW1XqVOJo6VdbUpOjcQS3L5IKqyka0AlTQ73gpUdAdz5KRjJGoFoKwAS7W76KBAaMzjRVrm6EDcdwkHFoALbPogix+uUm9tUiNRre5VpFgmh8lDNTQAN+4QRz6DMMvxtea405rsXQGzQF6R+w0FjXZea4hNWMktsRP8AltBkjaXMsBTw7XWdNQdbVrMRTKEcXpkU4MQGynwR+L/kQXRxuoUFYWOFChrspRykNH6Nmhv3FZzCSC5jBXXKgoELwar6quZrgLcNNlsE7daDP3VXJKwtotZfTwoM7IzdAb6hReKIG9+av5wBb4IzpXupGQN1yR3/AJUGGTcg2ClEwiVpI2IV80wsVFGe9tTixDRJfKjF1+r/ADRHpGNLGgHf1Vod3+SVh0Y016aJEkDZqKsFUrGAZm1vapDr6NVsbtRoNSEGxCVJoC0IpCAQhCBpJoQCEIQJZT70i1LIf7yT1QNgt7ida2UcxccrQLB8Th08lAuJeWxmv2ndvJTzENyjQIMRxD2zxx5WtsW55F73qhmJe1zxTXCm1p56/RaXudmNkBrWkknoogHLmY+712QZsNPM7wiiQaGgutfNWQ4qWTNnytoXsN6+a0VJzHa9AVYC52hOqAwrjJF4jZB30/BXkClXZsaqWU9CgllbewVbmDlnTW03B/dRt46oG1jQzLpfdZcQKJB3VrnG7oX3VL362QCfNBRlJdoFIRge+fgEOea8OmvQJa/1ogbjm6UOgUmx7D+gogHT8loiYbBIoD6IB4rSunyUK1ugr3ts6dECIEXen3IIxirNdE2PI/JWtjyNIu7UcpHS/RA5BTc1AqHM8AJaM1d1cLyC1Xpn1cNdgghmDW2W6oc0OZ4d97Ui0a2bJ1USMrgbonogqNtcTuAm5oI2oeimfFpeo3KrcchBzXlGoQVP8AABsVZteTxVvxD3dC6xWi9NxGXJg5HHQkVRXlJDZ6ILBfLoGj6ojtrgSdemqzO9Ugdd0Hbw73VmJ0rurtXtIB+q52Ei/Rm996WljQew7oLzD+jADhmVZjplHf1Ui1uXcaqqQeiCbaAonUeahK+qP4qku8VaWqpw0N6boGdc1nfuVNjblYLHzWOh0KmxozjVB7WN7XsAFbJXrVquBlxMHkplhFUSQgtbVhTAGZvqqQTodbVsRtwrug1oTQgSE0kDQhCAQkhA0IQgSyEU5/mVrWJv95KP+YIGGgaNRSCEgDmGvVASxtkbJG73SAD96iAG0B6Wsf2nC3FSwzXG4OJaXbPHkVlZxKSNmLnfIS1svLZG0degvzQdt1BziTWgVU2IZhoHykFwYMxA6rBLxKKDFOhndI000h521HVZMRxeKXCTsa2UtLS0PLK32Qd9j+bGyTKQHAGirQbC5eH4hHHh8Ix7tZWANJGhIAU28QviHsxADeXnBvzQdCr3ScNFEPDhvooSSNjaXE6DfVBF+ZUus3Z+qwuxsh4W+eOTM4BzmucwDr+SoxuPlGFhc0tZzquTLozRB0g0XuPhqmaB866m1yMJLy8PNN7V7QaJ1doCAeilNjpg3CyMDOXNQdodCe31QdYHt/NaYdGiyuNPjXxycmGEzSAW4A0GhbcBjRPzGFjmSRkZmu3oi0HQqgUm6LkzcSnkxT8Pg4A8x++9zqaEYXiE/t/s2JjZG7llwym8xv8AJB055aIaqxIRqCqC8veXErNjnv8AZZTGSHZDRB20QdjmDKA47hU5mvvI6xdaHatwvNsx+Ljijw5k5zp2AxPO7Se/kFv4G9w4U0A2Q533oOkcxFiwb62rQ+yAWn1WbmuAoiwfX8ldvWU1W4QSmAyXZ+CqL9coOtfJNz8g1sg9lnmJAJLsoO5FoOdx6QtiABvMdr7Lz48TjfRdXHNbjMW7xksYABruVndBGxwawaDc9Sgxsgc4gnRaYoGgjSyrmxbKxkJB1+5BKIFpogfIKZYS67Taw1qQpHVm/wAkFbmyCsw+KrOZ3RaCXZQKsKmQ2dPuQUiMg2VCdhLaKvp9baqtzCd9URiLCzcKTAXOHdaTEDodVUYCHeBFepwJvDRkndoWkbrn8LObBx5jqLH1Wyju0oLhVk+anHReB5rOM16j5KcZJe31Qb0nPa0W5wCB6pBrW7ABBWcTGL0ea7NOqbJnPBuNzSO9a/JW9NEi290ERIKt3h9ShSygdEIGhCaBJoQgSwj+9eepff0W5YwKlfvuTqgDdqOe2kM6bur7lB4MwoWGdT+1/JTLS2B48qFIMmM4VDi8OA4BslWHga3+S42CwBn4TPEw+Myk+Vheme45aEb/AJLmcNikw0crXwvbcziBQ2vRBz/s6fGSGXFnJlYGBoNmwN/xQ+DGPwzMM9kcbTTM93fTQLrsdnc9vLe45idKo/FSxEMkzAynxszAnIBZo97QY5sCDgI4p3AEAWW/quH6wWTh/NPE3PxHifDHktpq/NdwMBBuJ1ncmiuLhWvZjsaSCXB4b50B+SDqumdm0DAB3JKb/wBIwg5HAiiKIVDGyGzyzXckKxhIFZHP8m0g4cr34TCyYGWFxebEZGocCfqtscU0HD4mtiEj2tAc1xordNzSwHlZcp0JcCVAunHQX2oIOfhcLLJi5pZMPyWPjyZbFnzSg4XOyeF0swdFB7jQNfium102pyNcO10VNsrnCwyx6oONxCKeLFczCmQOlaA8htjTb4q/gzOU6a8TzZHG3AA2PM2LtahxKBs74nuYx7DRDnZfvWSKZ2L4qZoG5o2NILgdCfXqgcpxHDsXLPFEZIZaLmt3Du+yynFzT46HGvgLIYnZC71XoImvOpYP3lZlc6wY20d7KBtY3Lq35KE0DOU+gAXNI19FeOZ0Y2u+b+SollkJoZdPNBzcFwoQQxPkYDM1uXMCTQ7K+Dh7cNhyxz3uZzM7QDWXy8wtMTps9NyEHzVzy9wPhbY7OQUCJoFCjR0BRlDHANJBPkmWHK11UQdRabHG6IOg3QU4t7hh3PYaLfJcDEyySOPMeSOy7uPAEDyTuPmuG42dNkDggtlnqVXkOc3qVph8LANzuT5KoEGzeiIGsNEgq0NNNs7qIIrQ6KTZANN/JFSLDRvY7FRDS0eRT5gLCPwSdICNBSAI6dFEx99lY2rJtSNa6oKSw16qJZ8FfYrdUlwJ3QQbEb3HxUnQirU20RWak8wo25ERw8skDwGuoE6hdnD4lkjR4hY3Fri01zmjuUTaSjWtOiK9Gw7dlZERmbr1WaIExts9FohDi8Gzog2oQhAIQhAITQgSaEIBCEIEue4nmygjQHTzXQWF4Gd5vQmkA1pIsKWUhlHq4JRuYBQOZ3ZqlI1z2WaAGuUdUEi8A0BmIWeRpe7xkEdhoFdlsAN26UlyySC4gDz0QEDA3OAAAHaK3Jai1wa8geKxeiC5x9OwQJ72s0c4X26lZsjjPI5jGtzVZI12V1AXTKvqOqtY1pc+j2FH0QUNgBILyXkd9vkrS2hop5a1SKDHjY3PhaxhoueNtNOqxvw09upztAa1O9Dz9d10nU6U6gBorfqVFzmbZ236oOY1uJBBAcac4jXe7ofD8VrwTHtbIx9nK6r3tXtrU2KHYpwt/R2Rq7X5oEYYz4nRtcfMWrGMZVBoHoKTd7qbDlFlBMNAFBGVVG7tWR5iLd8ECmdlbQ1JWUjXeltyh24UDA0m0FcbcjS7qdlKLVxUpGu2A0HZETdSSEFT3Oa8CgQfLZPLmcHA/DopPp2gINn6KAAY8i3dygpxDS+J0Y1JGhK5n2fIHalvci12HW6nXoNwogZhRGvmg50WFdkqwfQ7qv7Plr9Xp12C6T4y022ydmjoEg9wGgs3WqDC3h7ywjS96tSOAeAdvLVdAT6NOU2dtE2yFwd4evZBzhgJK6UexKi7h8l0Mumy6Jc4tBGnkrGss71SDmM4fINyPmpHASV0+q6wb2HxKl/qCDijh77OoVbuGS17zV3S09KKgarbVBxmcPfmrONFM8Nkv3xS6pYCgCtKQcyPh7g8OcRopS8PzEHMF09Oqg5oOyCLG5Wgbq2M+IeqgGUd1Nopzdeo6oNaaSaASTQgEIQgEJIQCiZWA1dnyFoJJfQ27qVaIIh7SaF/IrJf6d4INE9tFtWHFZ4pS5prNsTtaC0VRrSvJStoO+qTXWNCrAdN0FWWMm6Fk9EssYIIa2+5V19keSClzgRo9uYai1UXt/WflPmtJBSIKDOHtaT+lv0CbZibLWXZ70rxvWizyDKdhaCRkkN6tb6C0qJaXOLzXmq/vV7WeEAjzKCtsLWtBLQXbk0olmujPorngdlWIxewQVSRZy1hZqdXEDYK6IOFsdZrY10S5bcxcRqfopcoF4PlSCeUkbH5KtwcToDQ8lPltbrX1UuQw6gkH1KAiBIpwVtjso8oAAAu+aXKAO7v3igkSqppSNGgpublDjb9Oziqnt1IDnmj+0gTZXNddE+S034dBWizxxHmm3yZRt4lPKbsvfr2OyAeKokeL8VHMX2MpHYop90XvvcaqIY4uc7mv0GgsIDKM1A6dRSCCLLWgmlINJNcx222iiBJmNu0GxQJrrcWkHTqgRtI2Gm2myUjJHbSaDWu6rInaNZDoL0/7oLhFVDLo3ZTDKFjS9SqHGXMBnrS7r+akwymKs+v9eaC0gAg/gmRRutVW1sljXUeuv1UwHE6EaeZQMEoI8kxn6kfMoGby+ZQIAjdSq+iPHfT5pBzx2/eQAFaKVWNAo5zdV8bUg8+fzQIijsoEbK3MD1UTv7yCOtaJsPibpuVFxH7R+alAC+QOF5R1vqg1oSTQCEIQCFW4tc7LZsC9DSEE0JpIIx9T5qahH7vxKmgFB7GyNLXiwVNZeI4o4TCuka0uefC0AE6lBhxzWYQaYtzCQajcM386XLPEsVGByXN2AGdnyGhVL5JJ5XueC97uhsknfb+vyqdQDmk6O3yjTvlsee380GwcYx4cA50Qcegj1+WZA4zjy1xzQChYuPc9ve0WW3OABOVpNDTKPp5366JRUGDNTmOBb4RXc2dd9aQbDxfHZiOdDbTRuIgAfNIcY4hny5oAazas6fP+vgVkdI0NIb/AHZAy5tSAfy1Gu43OqrLc1E5XN10yb9ScpOm/X80HewE+JxoN4uOOQEjIYQSa3O62OweMdV4uP8Agf8A5LgcMxT4MewlrWte8MJ2HkPL49V64bIOcMBihti2fwf/AMlP2TGf4xmv/R/mt6EHOOBxZ/41v8H+aXsGL64xv8H+a6SEHMHDsUP+NGv/AEf5qXsOLu/bW/wR+a6KSDnnA4o74xv8Efmpey4sbYxu1f3A/NbikgxDCYz/ABrf4I/NBwmM39tbf/0R+a3JoOe7B4x2+Nb/AAR+apkweJ29u+UQ/NdN5ofiqCfX8UGH2XF7e2/ARD81ZHgMY0WMdV/9Efmt0Uf6x+StQc08PxZNnH2fOEfmonBYth0xxF71CPzXUVOJkZE3PI4NaNy51AIML8Fi2i/bzr2iaEfZuKcLdjjZ1/umrbHiIXwczmM5Y1zZtPmrwQRY2Qc77Pxf+PP8Fqj9nYnb24125LV0BNGTQkaSSRQI3G4TEjCaD2kk1v1Qc08OxNn/AG9x/wDSamOHYmwfbzY/6LV0QAeqkg53sGM/8wP8FqBgcYP+P/8A4GrooQc/2HGdcef4LUvYMX/5gf4LV0UIOf7Di/8AzA/wWpewYu79vP8ABauihBz/AGDFf48/wWpfZ2JO+Pd/Bauimg5v2fiAT/tztf8ApNQOHT9ca/8AhtXRQgxx8OYP72V8ut+Kh9y1taGgACgFJCAQhCAQhCCLmB29/AoUkIBJCEEY/d+Kmos91SQC4PHsSee2FjzQb4gNjfRdx+bKctZq0teZ4vzBj3ZveNVlHvGun9boMbZKcLOa7Js0Nbsaev3pZXPOjSMotzgco+Hw+7yUGudbsj7NVbQK66H5fcpZhQ8GYA04EXXp5IIkuDaZVn3gNr/KigAscwPFn9YZiBWwsVqOmik4BzwdHHZgbr08vu12ThZmL6cQQbBI1PS/6/NANke5rX5Gh0gAvSr2IA6UADqoBoMUj4wWjSgLzdhZHrsrHO6NjskkBwYWg9b63r+KcT2tc1xbW41Ou9Dy6g/JBUHmJzJMrg+N24zGzfy26dvVe2YbaCO3VeJmYS/XM4ltHMAbvQE+ui9dw2UzYCGQm7YNaryQakJIQNI7ISJoEoOTPPjI2zSZy1nNyNJqgM1fs6euqQx0t+KcAhoLG5c3M3s2K28tq1XNwXEce6bBukmxGSaTKeZG3lka7Ea3oreG43G4gtkknnLac4g4cZDV/roNTuJ4sNrkfpSxjg0DNehLjp6AeVq/E8RcxzHRPjDXQ8xrXDV+ooBUe2zt/s6MY51zckPzFul+ivxuKkhiwzYmsM8z2xtc4aAkWToglhMdLNzy/LTA4gUOhI/avp2Co+2pBASYm80NZ4NdyCTt0oWPVWcOml9tmwuKET5GsEjZGMy5mnSiPVdMMaDeVtjS6Qc1/FH5JJ2ckxNsNaXeJ1NsH+Sqk4wGlwMDczXPDvF0aCQfjX3rp+zQZi7kx2W5Sco27LNiIoSSBEyupyjz/M/MoM/2y4Me/kghr8uVpdfvVe1HvoVZ9quNPbEx0Ra9+YSa5WnU1XXoqxhYc9siYCTeg1ve1uiwcMbA0RtFAiq0o7oFhcU+WR0csXLka1r6Dswo31+Cxf2hkYzBgvgdNTwWsF0T0uui6MGFhw98pmW99zfzTfC17rcg8jLDiHcGfyo+ZAS+SUAFnjO1NIstG9d10/tLGYRjHTQtbh/C22vJLbrU6bBdwxAsya0qjhR0KDzOGnEWJwmKldy4TiZ3cxwoDNsfiotilnbhTA4sfJiZ5YnbbCwfQ0vUx4fK7xC/qr8rdNBpt5IPP8IxmJcyR8eDe9s+IeXnOBy9uh36/JVSGdkXFWtxL3Fs0bcz5A0kULF7Am6XpQ0DYAddAoOhicHgxsIf7wyjxevdB5A4rEujbh43ytAmlyNdPXha0aZ+tFaYsViJzhDDjJpMS9kbst5WMb+sX97Xo34LCvibE/DxOjb7rCwUPgoP4bgpJOY/CwufpqWC9NkGkbJoQgE0kIBNCEAhCSBoQhAIQhAIQhAISQgaSaR2QJuykos90KSBLzHEntfj5nNzA+6DdGxQ/r4L05XkcWHHEzeMufmINkeLXr/XbsLCg07MMtgEm3H01r4HZNzM1uDxvYHwH039NFL/AC20VlBNH43636JEM6Bw1u71+aCM125wcXOq687/AJfcpgvz273r1FDQ1Xx/r4VuuyQa6Enqb8vihhLgA2hZ000+XnSC4WwhmbRrqJ6jTbRKnRlrLBLgbqwXbbb9tfXVV20gUXBl9ANSbIP9dFJzDnDbDidNqBP567Wgrddx5XeIA5XAgkV5Cx9ei9PwJzncMiLr1ugTdC9rXmM2Z1E01o18NDUb7/1XZel4C4HAULprzVivPb4oOkmkmgi92VpNE+QFlRle1kTnvNNaCSfJTUZY2yxPjeLa8FpHkUHnMMzAw4rAt5MwdIM7Q6UlsZN5dD1OqrwcmFDWjDMxTnVIOQZ9AB66UQbC6sfBMPkY6cl87cn6UaEZdq7baqyPg+GikjezMHMjdHd7g90HDjGFbheW5uNbHNCMkZmDraSAKGwP81bUb4+TI7GyYjP4WF7S+MtF2DtVFdN/BoCyNoklHLjbGxwIttGwfWwoP4NmaXDFTDEFxJmoWbABFbbAeiCjh+JwmGE+KdJPNIYmve94F5bLQ2htRB0W88WwrWxlznASSmJtjqDR+HmsjeAgRNjbinhpaGSjICXtDs3wOu6cv9n2S5s2JlGj8mXTKXOzX59Pkg6LcS2YSNjBzRvLHCtj/RVDrvy9FPA4aSKXEyzHxTPBA8gAAfjutZA7BBnw0Wuc/BaUAAChohAIQhAIRYuuqaBITQghZ1FphOgi0AhCEAhCEAhNCAQhCAQhJA0IQgEIQgEIQgEIQgEjsmkdkCZ7gUlFnuhSQRdYaaFnoF5bFjJPPnaWgu1FHve3UWvVLzXFmsGPfm8JJ1IoAggdxqdEGO3OaXAuyHxG+99v+3VItrwlrjTqcBr51/X4oaQbLHmu5cOvoh4u/ECBqb7+iCoi3R5SS0WfjdFTaXBzmtHi3IYSB59P5+aTIxlJMZDRQLqIaB8dFJwY45meIA6Zb0vyH5oKg4vLSaHanXXoa/mm0uGpb3bsNLHwUJHML9HjQ6a7D77tSblc9zm3RBvYWNe3r8UDdmNlwOaiKHhJ+fXTv+S9NwJmXAA2bc4kg9OgHyXmmtIy05wbm0vqfmR8bGhXquEta3h0OV2YEXffVBsTUS0FwPUKSASTSddGhZQcps2KbDFmZiC5ucP8BJJN5VBsuNhe0yNnkkFgtA8JGXTpWp87+Cs4djcTiOI4qDExti5TWkMBzVfn1VPGuKyYLFxQxyQRgsL3GUE9aGyCL5OJcvIeYJI2vJIIGbYjoQdyK02V+KmxDcQ1sb3A5WZWBlh5J1s1pp56KiXieLEjYYW4d8rYOdI6zlI7NXSwWJbjMHFiGggSNzUgw4TGYg4TEPe9xlbGSGkbHXpQ+Wqi7iOMZnaYiZIy0uAZYygW4jyOleq65Fd1IAUg5Pt8uZzhMwnMRysmrRYAN+YN699FXHxadwaCGXRzEjrmGX6Fduh2CWVv7I+SDlM4lOWB5DHh0gGUDXLrdamzQ7BA4nPk5mWIx8nm6XtdDX6rbipMPgcPJiZGNaGCyQ0WVgh4oObDHiuHuwzJ/BG51EHsD2QdDCTySOljlDM8ZAJZdGxa0quNkUQ5cbWMG+VoA+isQJNCSBoSSkeI43Pcaa0En0QNBC5+H43w/EzMhinuR5poLSL+i6CAATQhAkJoQCEIQCEIQCEIQCEIQCEIQCEIQCEIQCTtimou90oBnuhSUW+6E0DXI4hgXPxRmbHNIXAaMc1rW13JP4LrrBxHEyRAMjazxA2X6j5df63QcZ2Blt5fC8va0urObJHne3moTxwQSGN8xGVviax2Zx8hZNEEpS4svGWVzngtr3qBA7C/jdEIbjWsaDFg4mgajOS/c2a0AHVBBuHwz3gwjFB91QiZIPQEV8/wWh3DXsbmMcrddHSPjYG/LX6qo8QxTyGMfyqGUMaa+X/dUOc5zC57i45zYdqLO+/Wj1Gg7INRwsb2g85tbl7pwWgDsAdfiqBDgWtdmxTnOG7WNzV5XtaoAaSXUA52hcTqfn/2TBppsEHQb/T+tr+CCeTAgg5cU/XUW3T4gaffqvQcEnhkwxZET4TZBq9fiV5eUZXeMECtL1r+Xr2K6PB8SY8ey3PcHnISNnE/0PkUHqU0k0AkhJ5ytJ7BBz4cJLDj8diGg3M0ZLIqwFnxMGPe0OLOYZIeW9tM8J73/QSZxSd2FZLzIczqJ20GW9s2v0PkpycRxLC8ARyHKwsa1jrJcCfXQA9EGV3DZ8GWezRyS5sPyHeIAt89V1sDhhhMFDAATkYBZKyR8QmfJm/RGIujAIsGn/HooN4q90paImlmYNsZury272G3VB1j6fVSbssOCxrcZzCABldp5tOxWtpr/ugsSKAbTQc/jUDsTw2RjWucQQ8NbuaN0ufPimcYlwsEMOIBZK2SQmPLkruSurjMa3Cmiwvpud2oAa3br9yJsayGeKItcTLqDY/E6/BByxDj/tw/7QDKIrzZBWQu29V31lxeNiwmXmAkuBIqthvuQiPiGHllbGx9vc4tDeugvZBqQhCBrPj6GAxF3XKddb7K9U4maBjck5GV4Nggmx1vy1QcrgeGxTYsNLzw7CmO2sLG2O2q7ayw4nCsa2KItY1pyNGUgdqHRTZjMO97WNmYXOFgA7oL0IQgaEIQCEJIGhCEAhCEAhCEAhCSBoQhAIQhAKLvdKkov9woBvuhNDdgmgS8/wAelkOLjYLytbY10vuR8Oq9AubxLhjsXKJGSUcuXKQKHmNEHng5wGVjngkEucLAPrr9FHMWktBaTpW5/wC/qus/gU73E84AgaOs3aJuAy5HCOXNdeV72fuQcgucWAlwojp1+G6k6yLBb4hfvC9PX+r89R1XcExDhXMbpqC0kG6001UTwTEu3eyvMknW7+p/7IOSCYywNbTwTodO/f7/AOakKZoS6r971+Gmhv4/Pru4E8NBErnHXSh5VZ+H3aUk7gU2U5Zx5Aj8fXX+ZtByG+8LLa3ADdR/P+fwuwWZ+MiDnEUWm2gAjxaemn8+67X2FAGHxvLq0F0Lr/t8ldguFsw5a97s72jzoHrpaDoDZNJNAJFNRexr2FrwHNcKIPUIKc2FIaLhIedBp4iO3dSe+FpOZzAQMxsgEDuuC/g2KMWDYwNaWNyPcHA5RnzaWPuT4jwnHTSSyCRsshiEYcQG5wScwrpoRr5IOy44Z2aI8na3MNbdyEcqFzcoYwtLR4aFEDZchvDZjO2N+GFDEOldiMw8TDene6NVtopcPwGLw0DnOLGyaR07UmNooUQdCdSg6+VrXZg2nUBtrXZGb+iF5Y4HFezmsJO0OzDkg+67JTXXeuupPfotEWFxvNxJLZ2uMclyNf75sZMvwBQeiYdRsrbXn8dFMeGYKMtkdTmcwBhJAy63RBOvmskEeI5mFE7Z8rYxu2U/rn9k6Gq3tB6TEYWLEEGQGwC2w4iwdwa6KL8FC9zS7PpWmc0aNix5Fcg4qVvDTGfaBMyfM7wPvLzOhrXT6JY/FulmmfHNiWfox7KI2uaHvs2CK1Owo9EHalwkUwaJAX5WloLjeh3+OijDgIYXMe0HM1xcCTqSRRWhl5Rm3rX1TQNCEIBZMbgzispEuTKCPdsjzB6FawANkFBx8LgXTx4mOSUcozOaQG+IgG6u/wAFpZgJWuAM7XML2vd4KJLQAK102Cs4cbjn/wDryf8A3Fa0AqcNiW4nm5QRy5HRm+4Vq5vC/DjMewbczP8AEkj8Ag6Qe0vLA4FwAJF6i0Pe1gBcQASBr3KwYMl3GMeTsGxj6H81PipdyYcgBdz46BNA+JBtTVJnAxLIcptzC6+mhA/FXIBCEkAmkhAJPLgwlrczugurTQgjG8SMDhdHuKU0k0AhCEAhCEAov9wqSi/3SgY2TSCaBIWXiHtPJAwhIeTRNA0KOuvnSwiTimc2JA69srS2rP12pB2ULkc/HcyIETAF1SXGKB7CgdPP6qOJxWPZJIGNflEhGsegFiqNa2L7oOykuJLjeIRE20hhdo4s0Auv6tXOx+KafCwSEE5mZC0tABo2dNatB1kLn4HGzYiYNkDaLSS0NILDegPruuggEIQgSaEIBV4iXk4eSWryNLq70LVii9rXsLXAFrhRB6hBzW8Ue58bBC0mQX7zu4H7PmpniWRscksJbFI4Bj8wO/cdFqkwkEpaXs1aKBBIIHbRQbw/CteHthAcDYNnQ+XZBRDxKKaWFjWkGUOIJO1EgfOirW4tr8ScOGPztvNpoB0Px6fHsn9n4YOLmwtDi4Ozdb33VohYJnTAeNwAJvoP+6DN7bGY2SZX09jpAMo2G6rZjonyBoY4NP65bQurI/nspfZcAY1odKA28tSHQHceijJwnDuv+8DRqGh2gsUaQRPEYOWx+WQtc0uNN1aAaJIWj2yKKTlvzjbXKaFmhZ6Ws54RhfH4BRBFEaNsDUdjopyYBkkmYudlLQ1zQ7RwBseaDQzGRPjfIOYGMFlzmECvLul7bh6tzyyxfjaW3t3HmFVBw9kUM0QdpK2j4Gg9e2+/VR+ymljG80gRuzsDWAAO7+f80Fw4jhACecKBrY960012U243DuNCZoNXRNaVf3LI7hMfLaGPqRrs2cgmxZNbihr0QeGPc1zXztyOokNYbsNoaknTr+KDb7Vh85Zz48wFkZhoEDFQmV8Ye22Vm8Q0vosI4ZI2F0DJmCI2Rcdusjv2+qTuEukYInvj5TCctNNuBcCb+H5oOqCDdEGtELNgcM7CxPY5+cl5ObqR0vzpaUHNwkwgj4g4tc4RTvcQNyKB/FXyY6MRTuiHMfA0Ocy66Xv6KvDwg4niAdtI8D4ZAuU/AYyHCTspznPgpzozZJz7D/Sg9AyVkjba4G/ytY+GsbEcXIT4n4h5cfRcvhsWIZxGNs0bgQDI+tmlzAB/9pCtxGcTT8vMCTMKbufCw/PdBt4ZIybF42ZjrZI9hae4yBXcReGuwgv3sQ0fQrgsweLc6R/DrdCxxEL81XYy/QE6q6IcTczDe3RhrIpWlri7xOJIFfAEoOxI7LxOMk6CF31c1bFku+LV+zB97v5LWgaSaECQmhAkJOaHNLXCwU2imgEk+ZQNCEIBCEIBCEIBRk9w0pKMnuFA00k0AkhYGcb4dI/K3EtLqvY/kg3oWY8RwgDSZ2DMC5tncA196tOJhBkBkaDFWfX3b7oLEUq/aYcwbzG5iS0C+o6fVN0sbbzPaKIBsjQoJpqsTROFtkYRV6OCZkYP12/NBNCVjuEIGhJCAQShCBpIRaASOyeiSBH+tFHSxspH+tUigBtpaRHf7kaeSfzQQ22q/RWB19Comz3UXfC/NBbvshVNfR1PzVoQNCEIMXEMRiIXxjDxlwoud4b6gfiVibxXEZGOc1viOoDD3AyjXfW/hstOP+0HSgYUNDACLzDUnY69lQz7WOJbnDBEXnNRB8PT5figzwcRxJnxOWNgeSxxBDuuVv4/RXO4vLG5wkgunaZQdW5iCfgASoZeKMfzGRAvkaBISW7javIa/MKwT8SMbR7P+kzHNbRVaV19dfRAvthxHuQk0XXzKFC9Nve02WRmPMeLa/kucf0sgGxdZDa28vNaxPjWxQl+DslxLw2PzFGr00s2qHTY57opTgSJoyQWFhpwIN67aEBBsHGoczWtjNuaS3UftUB5Xv5JS49krwyXDuuBwkdlkBDa0vz32Wf2vFlpDuHNo6lpidvX1Jsjy6qeJldFNlHDWuEcjcrmx3pvY9Bp6oJwcTgONkleHNz8uIA7g6nX5j5rrRSCWJkjQQHtDgDvquBFOIzM6TAiTmajKw0BloM1HdoXbwTYxhmGJmRrhmy66Wgtc7LWhNmtAmhNAJIQgEIQgaEIQCEIQCEIQCi/3UAkuIqh37pSe6gkhCECfo0+i+c4NxOIeb2adPiF9Fm/un3+yV854eQJn6fq/iEHRxzHSDAkPDWxwl7iTWmcn8FaMOZMDisSMS/Owkva1/vsy0D5+SjiXtbPg25C/NhdG1YOrjr8aWcMxMULntljfHPE6Ihr7DS3b0A0r1Qa4cQ6TiGeZ3LLhIYBs26FOJO22/dbZcz8ZypwHQOma17rt3MMYDdPXW1y5CzGYaaZkY5bA1ge4+KO9XNAv3dfqpDH8ieOSOR0o5oke5wylwbGK+8oHhoX/osPlD2B7Y8xdRIbKdK+ajLC7ivEpeUwMDRTRe7Wimn4aH4qLnOODixQPKMj8zG+94s3id8w0UpexRgxPnmbA58IlfYJsNI1026fLzQacPPTJI8X+jbG4Tumcb/XIDaH/MSqnS4isPNndM8vdM8tFZyAM7R6UqI8QGHGRvIMc7XW0DWR5JDQD02JWiHhmI9r9mkkaZWiR2YWGi2iifIlx+SDbi8TLFjY8SczBPHmLXGwxrmgUfO2/Vc7DjFRYXFtldiQxkIljIcQ46kddxqrYJ5I8MWvMGI8AYaGYx+Lw3e25+ixh8zYYWtkcWShzS97jWVu4v4aBBrweLxT3A4nEPhZDC5r25yJD71EA7n+S0S8QnfEzFQSS5BCQbJAFPoE/wDNVX6rJi3x47iTJ4aiEjG6SENsku3+X3K3DuceCYvByZWSPcHBoPhouAOvqCSgtZxzGy4p0TWNzyvBiaHGjXTyvr6qnE8S4hh8VOx+IeGsAs2DRygkfX6J4TC4iDiWGcQCGSBj5A8bkbV5ilVjY34nF43FwjPF71bWKA/NBvn4nix/Z7CTxSOMzpA0u0t4F386UuDcVxGI4kYJpc4Md5coGUitfqsWOEg4PgsK4ZZ45gwtOuU0S0eehCjwvENwPFn+0/oRkyEu6mxQ+/5IG7j2PaybNI1tOOVzmDvouhxLjE+HGDdAG1MwucCL7fLdebkD+S8OjLwbeAOjc1X811ONl0zuHhuXNyyC2q1BAIA+B+SDfw/jM2IZjOYW3C3M2m7aHQ/ELNB/aTEOERkjhFuAeKIJHWtVj4TIxuF4k+g0FlB11mNO0HfZZI25H4fnRhzhI0VRLem59DaD0vEOMyYTiAwzY43MyB1uJ63f3KLeNPPCZcXkj5kTqLWk1uK19Cubxl3/AMXffiYI25iTR69FCIgf2YlMTf8AegA7Wczdf67IOjhOOnEYqKPlANkvxB1m6sfNSl/tIMPiZIXQ3lcQ3x+9Xw7rg8Pc13FsOXt8dHRx20Ov3qGMp2MxmYAM5jqd/Xmg9ZNx6KHBxzllkvEcjA7+7dluieqnguMx4ufkmJ0ZI8JcRTiNwPQarz2MLW8C4eWREguBIu70NlWcB5Y4rKdyI7Fu0bsDp56fVB1f/wBRxcnmnCzZMxaHCtSDS04ri8GGdECHvEjS4OYARQ0/FeLdKXYUtc9zGtcSBdA+fy+q6vGpWRTYNkVtYYS0V2sH8EHoMPxXDz4STEgPbHGSLcKzaXp3UIONYOd8TIy/NKQGjJ1q9ey4WBp3Bsex7y9sQLo2k6N0JFfG1k4fM+PEYQwyOiYZAHAdjQ/CkHr5Mfho8we/VrmtNC9XbI+1MG3NcvuOLT4TuDR+pC8txKVuC4uXRVGWtY2MjxVpt9fqrGBj/wCzhMhzytkEbgNKzODq+42g9THjsNKIiyQESuLGaHUi7H0KrdxXANxDoHYlgkaS0tN2CvNQTTsdGYWF+HjlZznAbOux6UCB5rHiXf8A7gxHfmuH1Qe3ixUckr487MwdlADrPy+a0Bed4a7NxqXynk+4r0QQCaSaAQhCAQhCBJoQgEIQgEIQgQFbJP2UlF+3xQNNJNBXiDUEh/5T9y+f4CZrpX1h4dWjoe48177GGsHMe0bvuXz3hliR5Fe6EHceXHluZh4nyDCEtrQjfbXoq8MyKfBTNiZCzJG2KRmQ1ncRZ3+HwTM78NxHBTZLiEUbXntZP4EpNjmlwGJfyiHubys42c/m3t5EkfBBRJzIMU6DEQxwMfFcxeDR11J165UmxwODo8RBH4XRHPqA4FoGUa76/QqWKw04xMkQyvceZmmItrnuAaQB2BNV3IVb5AMfJLPE8sLwXRMHiYQwWa+P3oNHMjmgbGWwTMjkZCeULNuJzEa+QpWRYvOIMPHFC0ZBBculhxsga9AB8SiKaHCtwsb4eXyXtdJlZTy5odv66V8VRG6NsuEcGRSlzi1zJyByn6Gx26C/JBGaSCPEYMSxsbE1znl4ZZ3zd1fiuZh3Yc4hrY3vc5wMduzNtu5vsss+fFYdjImRuAiLTmfWt6n10oDspycSfK+GRmZsVvjdGP2DVN9NEEIMcGxZfZos0xzvBBADQKb111v0pTxuIw8eE5DcmQPbpkIDA6O8wF9dVdi4Q+FrpZS4QvkYxxbq94GorpZs2suGwkjs2IxdjIHNddeNzNcum2jd0DxTm4iaGN2HiMxDM7CCTd07qr8Xi8NiYXS5YWx2/JE6yXiwC8Htf3LJE1rXwmRwkeImujY3wl+t1+6puxBkglyNjyz1NFHlBcCZQKvtpsgtw2KkxGJiw+HbBG8AtZnBq8nj69fwUsVimFhwsQw5ihNnfxX4RWvY2q5WxyQQvdI2N9XnYcvLJedHHvRP7qzztjlxk7mEMGr2NNAk6UPSkGyfDMbg8I0siyulDHEXbavMd9B28kopTM/Dw8jCuGIcGl2pLa8XfsSozxztwMLMU94jmc5zTBbnEluortt9U8IyOGJsvgL2PYAB+o3NRPqToR2QS55xeCyRYXD52s5Z1o+Jwy1r8T5psdIGQSPw8LnxwvmZ4rs229b06owcmGcG4hsYjljaLcGkl7gRV9tG7+afIZw6aKCYiXNG97CBXLdrp59UFEGKw7cMMMIYnkwucdCMrmh99deysY6ZhxMksLWRFjZA2yR4gWjr0Fj0CoOFcySeaEctgw7ubfis1WXy1F2q24HPFCOcz9NGYxodC0/iSEHRZPEYJ8RjImunbh46abzHcA77Gws7sXicJhuUMPGI2vcY7aazB4031INrO1hZP/tlseIqLCdXk7ADyu1ZI+fEQuY6N0jiWZXRt0DnEOcPWz8kBg8ZE3GQvdFE1jALeQfACTvr3crZHOmdKI4sK5nOdZdeYlzqoUd6Fqh8cOIxQADYopJXcxhoODQ3TTsKJ8iptflmDQGth5srszdw4ksaT6aV8UF8eM9phihZBAeVLy2NF0QW1e/mTahgHOw+Oia6CISOIaC0khzQTmJN/wDdVOw78NhW5SW4gPe2xv4RQ+eq2QwyAYVjnZosjopBYqwCQ3ToCLHqg5hmgjjjfJh45GFgBa7NQJza79KW8zNfi8LmYyaM2zO4HVoPa+wJWfGzc/BxuboQ1pY49Mo2+JB9MvmojDDFRDFxZY2hjpHMu82Z5FAoNWGxeE9mlbG2FmbDFz46d+kO5O/b70zNhpeICJ2HjZiOTkfK4mg7KCBV9gQss8ckDnRubmkfC6F5AqjQIZ67/NTwbHtw8X6B7p5c7aqzYpl+gBPxQWGbC49wDMLQMnNBcTTRlt167kA0qX8QidC/Nhg0tkc/KbvVwIvXtSoa58MLWB0YBqOh74NDU+VAj4lacY6GQYmZsAyvMLry66g2B5aBBdFPgof9oyPayV9FtG8uhur3uvgsz5Y38cmAgidcrtbOuvqtcghLeVNhxGXtbyHtb7rAaeT2J7ddFz8Pldx15bQaZTQ7DOKQei4cWnislRNaebJqLv713gvPcI14k8/88pv91ehCATQhAIQhAIQhAIQhAIQhAIQhAlF+w9VNQk2HqEEk0k0GfiBrh+JP/Sd9xXz/AIZVyWOg2+K97xU5eF4s/wDSd9y8BgGuPM+HT1QdbERCXieEa1pe5sMXhB3BB/L6q7GmNmCmdPOHzxzFvNb4WuJIzaeQAWbHRc2Us5ZMjcPGWV1OVunwNfNWzxRYbD498NB4liBjf4spuyTfe/ogqxLMRBiZ3Yt2aRuHLWOaMrXO3aa89R6gqD2skxj2zuIndiW5shq21bz6KQkdFEGRTRCEuDmunGbK7M5pBPWgbVjR7LMJ3Re08pzmyhjcxaBmb8LJv0CCjFmR8bYpZGBpkbUoPjFh1CQnqAVICKTFNhxkLYuY5sgkY23ZnAHW+m+qWKjixjHvLyJSc0zWVlLgz9UeprXzUcG6TEY8PmktjSI3lx1c2yAB3B6+SAbhn8prA3DkOacRmEniuwdR3DbA9StOHYxvF8HlAZUji6jo4Ekg36ZVkfhQH4VrrjeYWvfLG3M4aHT5kJwnBzRQ57DuX4WBhrNrnZfQHe/NBpdzyZI8Qc7mwyyPcT7rqLHDTfXKVe+d+FBv/bY/ZbfVMzNBIJ8qtJzR7HioS/nGUGdr6rKKDc1eZJ08lhjfPLnwMTCwybNIDsjQLa2+t7/FBrgZh4ZDLG4PkjIfGwblrm6b9i8LNMyeThckb2ZJcO7kl2Wr1zCq6ivqFvxbZYW4iSIAkSRty5bPgjDvwWAiUyyOjnikw8kwka4AkeNxBvvQbSC+XCR8oOmDmva1r3xgeFjiaaHjtR1+Krn5ceKeySKMZ8Q4sdWrWtdqPQgO9aVcMWJnw0bM5MD5eS97bL8xoguPYGh81PERMxUkEcjnjx5JHx14SXPuz6d0F2Kle0xtwweXNlMsJPu5XZSACOlEg9rWcxuwc7RKxkkUji6QsN5s5tpFb1lVZOKkje+OWWEW9sDAa0GUZa9D07LU3DyB+EkDgA5jiY2nRrGNto8t9u6CHCwcFi8MZyBJLTnEOvQgga+f0oLPPj3GWN0Mhe1xc5znCrqQuBr0V8UAiwgjxQDzG9rw69oy3KKrzFUoMixUGEtjw1jGBk0dA00ucN/I9u6DNiXQuc8QtzchkkZcHEWBeU181YyaP2YYaZrh4Q5rc2vhcSAD3IsKPKxQjniew5hAY3WAbfmst9fECtOUu4jc2HdkaBEa08TWkhvqfxQE7cPmIMUtEscx2bSiASPUX9yhzpBwesOaYJGPY7qHEuJBPcANtdGd75HTtbG0xyTxtgOXQEgE/cNFhw0cmO4S3CNa2NzphkBFX4SSfSwR8EGb9HFjXvyudFMRGXOF+F2ho/tDW/ijmF8T4nNJZHM8uyi3PIutOw1UyJMRPOYgG4drzNG2Xe275R5krThycLM2cNBdyzJ62X3foSPggTjJNiTWKf7S4uY4kio3FujWk7jUhEb5HPMGGYIwzESOc9p1oNI2PcAqrCwuIwzpcJE+R7ZJGiz43UCC7sosxLnxtdyQ6UgNMxu2jeq87PzQQr2iWHDwwHnNc6RpD+lWPLcKx0bpHZvaA6Z8efmZaGUktcK+WqrxjGnBlghEToGtuIWd7s35OI0VgdG7CYySOEiN0OQf5sxN/GrryQaOZhjRZJpIzMXON34mih2LQNSo4SL2ZkBkmaGTPeGvs2GmmkA9xqVmbKwYSaJ8JbLh2BwsjwgOqj5+In5dlVh4H5mMkc643F4hJOY9AAPqfRBonhwseMMbZHkCRkbiSCQwgU9vmO/mrHDnQva64mvcHMyaNAaHCvI6bdiqHxvMnLaYCYS39IdpjbWjXq3ZXYmfJgIMxEji5pIabaNCPF/za6+QCDUMWJn4aGcjI64Hl58Ubg6wa7aN1PZc7Auz/wBoHHvP/wD3C2YbAQy4iGbGTOe7FiujqdmbV/CvmsPCRm420/8AVB/94Qd/gLs2Nvp+lP1YvRrzv9n2kYkH/kefmWfkvRIGhCEAhCEAhCEAhCEAhCEAhCEAoSfq+qmq5Onqgmi0IQQmiZPC+KQWx4LXC6sLnxf2f4dFmyQuGbfxkrprHxF87eQ3D5sz3kHLQNZSdyCNwEFcvBcHK8vcx1lmTR3TLl+5TZwrCsi5YYS3m805jdnz7hUTY3FQvw8b2NDzQcSNJHWAQ3XTQk/BVu4piIyzO1hOdwprSTIA/LTdd61QWngOCL4nFrqiqmkjKas6itbvVW/ZUAIILh43OcBXjs3Tu4WAccnDWudC2yXeAA3oT8qA7d1dFxd5maxwicA4NJZZz2Tq0eVaoL4uD4SGRr2RtsOc46DUk9fToqB/Z7CZI2ubm5ZJaSBoCDp6Wb9UScYeJXMayKiXBuZxGXLvm7XWiTeMyyNeY4G5hlIY5xs2aA23KBjgmRrORinxStzXIGi3WAB8gAoS/wBnojiY5cPJyWsIdkDb8WaybvqCQr5+LGDmZ4P7uTITm0rKDe3noFB3G8g8UBBvVtmw3vt1+Xmgq+wOXDio4Jgxs8WSi26o6H4Cgs+I/s3NOKfimeBpDKbVG9L+Z+a6n2k04sxsMRiaATIXGtb8q6dSoP4xG1zgInu94sojxBt5j8KKDI/g2KkYHPxMbpmu5jXZSBnoCyOooHTzVeO4DNJiRLhJIowMpyPBy2Dew6fzXRk4tA0SOa18jI6zOYBQu/Py+eibOKYeS6Dx42sGnckA+WoO6Dlt4BihC/DtnYyIEGMsJBNWbd52Rr5LOP7PY9hc4Sx+KRziM5pwIO+m+tehK77OIxF+R7JGO5gj8Tf1j0sWlHxTDSlgYXEyOLW6b11QcLFcEx7pWmMtcxkr3sc59FuYD7iNFNvCuItlc1rtMriZswzSEisp8juu5Lj8NDKY5HkOHTKTZ00Hc6jTzS+0MJlvnDYHY3roEHnsfwLFOeBhohy2gNYMw8Ia0Vuf2i5WO4Li35qdys0TTLYDuY+y4jy16+a7v2jgiHO9ojpozEnavX4j5qXteGzSAzMBjFv190IPLu4JjmMfCzxNkLsxAGmbLrv0IPyUIeEYxscznwShzMroxe5FgD1FgnyFL2VBwBFG0wAg8kOGzxRTRCOXm52NEpvJQHvAdPVSiwM5ikj5ckTGzPDHMaQ/Rjuva9vVes+azPxmGa97XzxtdGLeC8DKPNB5ZnDcXhYYHOAke1okokkCnW5p8iCDXcKrBNlzublklcWOjjZMCG6kAt8mr1ntWGcaE8R8Oas4270pMmheQGyscXjMAHg2O6DyBmfDC1zXvc6WN8b2OFBp8IIvroFN8rYmMbzTJnc5vNcKJaxtNbX+or2Iy35qWRvVo+VoPHyTQzRYWUzAySVzIv8A5rWuOXX9XZUvMs0jMPGW1KIy6EVZOZx38l7QxR6eAaeQQIIw4OyNzd8otB4mdxOLMUJjllcTndlsPeXt6dtNvVTjzYlxkZlimD3vGYeJ7soBa2v9RrzC9j7JAHh4hjDhscgvukMHh2kFsEYIsimDS90HkeRFiWyHO1kbZfBqLbmrK0/FoJ8iVS+CODDuwhYHStxB5pe3TYjTvWq9l9n4TJl9njylwfQb+sNih/D8LI7M+BhNk363f3n5oPMQYMTTui5zo3CUStdWjIx4aBPo3TsAsHBB/wDGGnu8GvivcPwWHkjfG6IFjyHOGupFV9w+SzwcGwOHm5sUGV93eYlBzv7O/wB8Df8Auj/9wXoVnw2CgwpuFmXTLuTpdrSgEIQgEIQgEISQNCEIBCEIBCEIBVTHK0OOwOqtUXNDmkHqgYNhNZGOkw1h4L4+hAsj1QeI4VvvTBvqCEGtJZRxLBH/AImL95H2lgv8VF+8EGpFLMOI4I/8XD++FL27Cf4qH+IEF9DskGMBBDQK0Gmyqbi8OR/4iEnyeFIYiE7Sxn/UEA6CF2bNEw5qLraNfVAw8QcXCNmYuzE5Rv39VLmM/bb80cxn7Q+aCD8NC82+JhObPqOvdV/Z+E/w8fvZtuq0BwOxtO0EWxMa97w3xPrMe9bLO/h2Fe5xdFq42acR389tTp5rVaEGR/DMI9zncrIXaOyHLY7GvVDeHYdt012r2vPiJ1BsfBa0IM4wcWQN8VCTm76l13+Kp+y4b8T5XagnM4HMBVA6eXqtyLCDA7hcZkL2yPbtlAAplEEVppqLpRfwmN0WTO6srW6gG6JNkHeyV0L80rQc5vCGMjfG2aTKWOY268NgAnz2CWI4ScQZebiHEP0bTay9h2I67arpX/Vo1QKJnLjayycoAvuppX3QgKXGxHCZ34h8rJIqEhlY0g6klpId5eFdknVKzug8+OCYlrZGCVmV8dEAkZjpWnSj1Rh+E4uPEMe50QLQ53Mbq4PN61WoF6DQdV3rN0RR9E7OU/kg42F4ZiYnsz5CA1zS7N0ObTa71Gtpx8PxbZGFz7AhDLz1Xgogdd9bXYBPqm036oOZBhsYzFwSuyljGCJzb1rLq7977lsw8cjMRiC8uLHOBZZuhWtdtVo6oCBpO90900IOGDxUBlZyc2gcNCdLJ0230+pRzuIhoyc5zg4ZQ+MDNoM16aUb7ad13KQg5mGkxbnwhznlhe4EvjokZbs7V4rChDisU6fDxveA5wOcGOgdSPnoNPmushBy8PjcS+bDtkaPG0FwDCLu7I7VQ+a6iEIGhCSAQhCBoQhAIQhAIQhAkJoQCEJIBCaECoHollaeg+SkhBWY4yaLGn/SkcPCf91H+6FYmgoOEw53giP+gJexYU/8ND/DC0JIMx4fgz/wsP8ADCR4ZgTvhIf3AtaEGP7LwPTCxD0aj7KwN2MMwei2IQYvsrBXfJA9HH80fZeE/wDlu/iO/NbUIMY4Zhmim80Dymf+aX2Zh+jpx6Tv/NbUkGQcPjA0mxI/9d35pHhzD/xGK/juWiVjnPY5prKdR3CsQY/s4bjFYv8AjFH2ef8AGYv+IPyWxNBi9gd0xuK/eb+SPYZOmPxP/t//AMrahBh9hmu/tDEfEM/JL2HEjbiEvxY38lvSQYvZcX/jb9Ympey43NftrfTkj81vSQYTh8d/i4z6w/zS5HEANMVCT5xH81vQgw8niI/3+HP/AKbvzRy+JdJMN8Wu/NbkIMOXiXfC/wDuTH2iBqzDH0e4fgtqEGPNxAf7nDn/ANU/kjm8QH/CwH0mP5LYixddUGTnY3rhI/hN/JHPxn+CHwmH5LWhBk9pxf8Agj/Fal7VixvgH/CVv5rYhBk9rxH+Am/fZ+aBjJv1sBiB6Fh/Fa0IMzcVK4/+DnHrl/NXtLnauGXyu1JCATQkgaEk0AhCEAhCECQhCBpJoQCEIQCEIQCEIQCEIQJNCEAhCEAhCEAhCECTS6oQNJNCAQhJA0IQgEIQgEIQgEk0IEmhCASTQgEISQBIG6aSaAQhCAQhCAQhCAQhCASQSQNBaEAmkmgEIQg//9k=</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Productiva</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Brucella, Aftosa</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Ninguna</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -652,10 +733,18 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="18" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="8.109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="10.88671875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.21875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="12.88671875" bestFit="1" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -702,32 +791,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-12 16:28:04</t>
+          <t>2025-11-12 18:12:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A101</t>
+          <t>b101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lola </t>
+          <t xml:space="preserve">estrella </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>c0001</t>
+          <t>c101</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>lolita</t>
+          <t>lola</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -737,7 +826,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>nada</t>
+          <t>sana</t>
         </is>
       </c>
     </row>

</xml_diff>